<commit_message>
show stock index table on web
</commit_message>
<xml_diff>
--- a/fund/Jelly_model.xlsx
+++ b/fund/Jelly_model.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="350">
   <si>
     <t>编号</t>
   </si>
@@ -972,6 +972,9 @@
   </si>
   <si>
     <t>影响程度(-10~10)</t>
+  </si>
+  <si>
+    <t>影响分析</t>
   </si>
   <si>
     <t>信息描述</t>
@@ -1072,13 +1075,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="yyyy/m/d;@"/>
-    <numFmt numFmtId="177" formatCode="0.00_ "/>
-    <numFmt numFmtId="178" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
+    <numFmt numFmtId="177" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
+    <numFmt numFmtId="178" formatCode="0.00_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -1100,14 +1103,110 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -1122,63 +1221,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1190,61 +1245,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1301,7 +1304,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1313,37 +1460,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1355,73 +1472,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1433,55 +1484,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1525,15 +1528,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1553,7 +1547,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1573,17 +1567,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1595,6 +1578,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1617,8 +1609,19 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1627,148 +1630,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0">
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="4">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="3">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0">
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0">
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0">
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0">
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="5">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="6">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="8">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3">
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="3">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3">
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="6">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="4">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="37" borderId="8">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="10">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7">
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="39" borderId="0">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="34" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0">
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="38" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="33" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0">
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="37" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0">
+    <xf numFmtId="0" fontId="3" fillId="38" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="36" borderId="0">
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0">
+    <xf numFmtId="0" fontId="3" fillId="39" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1792,26 +1795,26 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -1834,7 +1837,7 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -11494,19 +11497,19 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="9.66666666666667"/>
-    <col min="5" max="5" width="17.3333333333333" customWidth="1"/>
+    <col min="5" max="6" width="17.3333333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>313</v>
       </c>
@@ -11525,45 +11528,48 @@
       <c r="F1" t="s">
         <v>318</v>
       </c>
+      <c r="G1" t="s">
+        <v>319</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>20191011</v>
       </c>
       <c r="B2" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C2" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D2" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="E2">
         <v>8</v>
       </c>
-      <c r="F2" t="s">
-        <v>322</v>
+      <c r="G2" t="s">
+        <v>323</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>20191211</v>
       </c>
       <c r="B3" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C3" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="D3" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="E3">
         <v>3</v>
       </c>
-      <c r="F3" t="s">
-        <v>326</v>
+      <c r="G3" t="s">
+        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -11585,119 +11591,119 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1"/>
       <c r="B2" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="3" spans="2:2">
       <c r="B3" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="4" spans="2:2">
       <c r="B4" s="2" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="1" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="13" spans="2:2">
       <c r="B13" s="2" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="14" spans="2:2">
       <c r="B14" s="2" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="15" spans="2:2">
       <c r="B15" s="2" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B16" s="2"/>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="20" spans="2:2">
       <c r="B20" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="24" spans="2:2">
       <c r="B24" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="25" spans="2:2">
       <c r="B25" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="26" spans="2:2">
       <c r="B26" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="27" spans="2:2">
       <c r="B27" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="28" spans="2:2">
       <c r="B28" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
not show color in col 1 in invest table. modify invest table to not include formula.
</commit_message>
<xml_diff>
--- a/fund/Jelly_model.xlsx
+++ b/fund/Jelly_model.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="360">
   <si>
     <t>编号</t>
   </si>
@@ -887,6 +887,9 @@
     <t>20191211 22:28:01</t>
   </si>
   <si>
+    <t>投资日期</t>
+  </si>
+  <si>
     <t>状态</t>
   </si>
   <si>
@@ -896,7 +899,7 @@
     <t>指数</t>
   </si>
   <si>
-    <t>投资日期</t>
+    <t>总投资</t>
   </si>
   <si>
     <t>恒生指数组合</t>
@@ -1104,11 +1107,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="0.00_ "/>
-    <numFmt numFmtId="177" formatCode="yyyy/m/d;@"/>
+    <numFmt numFmtId="176" formatCode="yyyy/m/d;@"/>
+    <numFmt numFmtId="177" formatCode="0.00_ "/>
     <numFmt numFmtId="178" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
   </numFmts>
   <fonts count="23">
@@ -1130,6 +1133,36 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -1145,31 +1178,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1182,7 +1193,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1190,30 +1201,6 @@
     <font>
       <b/>
       <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -1228,8 +1215,40 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1252,23 +1271,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1320,7 +1323,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1332,7 +1365,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1344,85 +1461,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1440,19 +1491,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1464,43 +1503,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1563,7 +1566,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1583,6 +1586,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1598,22 +1610,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1633,17 +1640,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1661,148 +1664,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0">
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="5">
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="5">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0">
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="8" fillId="0" borderId="0">
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0">
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0">
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="7">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="6">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8">
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="8">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0">
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="5">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="10">
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="9">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="5">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0">
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="11">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0">
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0">
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0">
+    <xf numFmtId="0" fontId="7" fillId="36" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="37" borderId="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0">
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0">
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0">
+    <xf numFmtId="0" fontId="8" fillId="37" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="36" borderId="0">
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0">
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1840,24 +1843,24 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -1874,7 +1877,7 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -10262,7 +10265,7 @@
   <dimension ref="A1:S26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -10281,32 +10284,35 @@
       <c r="A1">
         <v>1</v>
       </c>
+      <c r="B1" s="10" t="s">
+        <v>289</v>
+      </c>
       <c r="C1" s="10" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="F1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="H1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="J1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="L1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="N1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="P1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="R1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="2" spans="1:19">
@@ -10314,7 +10320,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D2">
         <v>501016</v>
@@ -10335,25 +10341,25 @@
         <v>284</v>
       </c>
       <c r="M2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="N2" s="10" t="s">
         <v>241</v>
       </c>
       <c r="O2" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="P2" s="10" t="s">
         <v>238</v>
       </c>
       <c r="Q2" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="R2" s="10" t="s">
         <v>214</v>
       </c>
       <c r="S2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="3" spans="1:1">
@@ -10374,7 +10380,7 @@
         <v>20190909</v>
       </c>
       <c r="C5" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="L5">
         <v>20000</v>
@@ -10438,7 +10444,7 @@
         <v>20191008</v>
       </c>
       <c r="C7" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="L7">
         <v>10000</v>
@@ -10478,7 +10484,7 @@
         <v>171</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="L9">
         <v>-31575.22</v>
@@ -10510,25 +10516,22 @@
         <v>10</v>
       </c>
       <c r="L10" s="14">
-        <f>SUM(F22,H22)</f>
-        <v>0</v>
+        <v>1448.08</v>
       </c>
       <c r="M10" s="13">
-        <f>L10/300</f>
-        <v>0</v>
+        <v>4.83</v>
       </c>
       <c r="N10" s="14">
-        <f>SUM(F24,H24)</f>
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="O10" s="13">
-        <v>-2.035</v>
+        <v>1.53</v>
       </c>
       <c r="P10" s="13">
-        <v>39.3957703927492</v>
+        <v>150</v>
       </c>
       <c r="Q10" s="13">
-        <v>0.302114803625378</v>
+        <v>1.53</v>
       </c>
       <c r="R10" s="13">
         <v>-152.116402116402</v>
@@ -10545,7 +10548,7 @@
         <v>277</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="L11">
         <v>14298</v>
@@ -10577,7 +10580,7 @@
         <v>229</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D13">
         <v>13000</v>
@@ -10603,7 +10606,7 @@
         <v>230</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="H15">
         <v>3000</v>
@@ -10621,10 +10624,10 @@
         <v>17</v>
       </c>
       <c r="B17" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>300</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>299</v>
       </c>
       <c r="J17">
         <v>3000</v>
@@ -11031,28 +11034,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C1" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D1" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="E1" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="F1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="G1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="H1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -11063,22 +11066,22 @@
         <v>20191011</v>
       </c>
       <c r="C2" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D2" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="E2" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="F2">
         <v>8</v>
       </c>
       <c r="G2" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="H2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -11089,48 +11092,48 @@
         <v>20191211</v>
       </c>
       <c r="C3" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D3" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="E3" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="F3">
         <v>3</v>
       </c>
       <c r="G3" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="H3" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B4" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C4" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D4" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="E4" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="F4" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="G4" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="H4" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -11152,99 +11155,99 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1"/>
       <c r="B2" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="3" spans="2:2">
       <c r="B3" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="4" spans="2:2">
       <c r="B4" s="2" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="13" spans="2:2">
       <c r="B13" s="2" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="14" spans="2:2">
       <c r="B14" s="2" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="15" spans="2:2">
       <c r="B15" s="2" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B16" s="2"/>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="20" spans="2:2">
       <c r="B20" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="21" spans="2:7">
       <c r="B21" s="3" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C21" s="3"/>
       <c r="F21" s="3" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="G21" s="4"/>
     </row>
     <row r="22" spans="2:7">
       <c r="B22" s="5" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C22" s="6"/>
       <c r="F22" s="3"/>
@@ -11252,77 +11255,77 @@
     </row>
     <row r="23" spans="2:8">
       <c r="B23" s="7" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>1</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="24" spans="2:8">
       <c r="B24" s="7" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="F24" s="8"/>
       <c r="G24" s="7" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="25" spans="2:3">
       <c r="B25" s="7" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="1" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="28" spans="2:2">
       <c r="B28" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="29" spans="2:2">
       <c r="B29" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="30" spans="2:2">
       <c r="B30" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="31" spans="2:2">
       <c r="B31" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="32" spans="2:2">
       <c r="B32" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add means to fund level.
</commit_message>
<xml_diff>
--- a/fund/Jelly_model.xlsx
+++ b/fund/Jelly_model.xlsx
@@ -540,6 +540,7 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
       <right/>
       <top/>
       <bottom/>
@@ -547,61 +548,61 @@
     </border>
   </borders>
   <cellStyleXfs count="49">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyAlignment="1">
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="10" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="10" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="14" borderId="2" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyAlignment="1">
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="10" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyAlignment="1">
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="10" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="10" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="10" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyAlignment="1">
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="10" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="10" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="30" borderId="8" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="10" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyAlignment="1">
@@ -610,13 +611,13 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="10" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="10" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="25" borderId="7" applyAlignment="1">
@@ -628,10 +629,10 @@
     <xf numFmtId="0" fontId="10" fillId="18" borderId="3" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="10" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="37" borderId="10" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyAlignment="1">
@@ -640,58 +641,58 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="10" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="10" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="36" borderId="10" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="10" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="10" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="35" borderId="10" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="10" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="10" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="10" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="10" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="10" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="10" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="10" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="10" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="10" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="10" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="10" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="10" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1680,8 +1681,10 @@
           <t>中</t>
         </is>
       </c>
-      <c r="H2" s="0" t="n">
-        <v>105</v>
+      <c r="H2" s="0" t="inlineStr">
+        <is>
+          <t>115</t>
+        </is>
       </c>
       <c r="I2" s="41" t="n">
         <v>2.1742</v>
@@ -1820,8 +1823,10 @@
           <t>1.142, 1.124, 1.081, 1.027, 1.04, 1.016, 0.998, 1.014, 1.035, 1.025, 1.061, 1.03, 1.025, 1.03, 1.005, 1.002, 1.036, 1.025, 1.018, 1.038, 1.074, 1.041, 1.064, 1.052, 1.06, 1.084, 1.115, 1.086, 1.097, 1.098, 1.085, 1.079, 1.124, 1.146, 1.149, 1.133, 1.15, 1.135, 1.138, 1.099, 1.063, 1.086, 1.123, 1.121, 1.116, 1.145, 1.189, 1.195, 1.208, 1.239, 1.251, 1.284, 1.277, 1.29, 1.291, 1.312, 1.314, 1.326, 1.282, 1.264</t>
         </is>
       </c>
-      <c r="H3" s="2" t="n">
-        <v>105</v>
+      <c r="H3" s="2" t="inlineStr">
+        <is>
+          <t>115</t>
+        </is>
       </c>
       <c r="I3" s="41" t="n">
         <v>1.264</v>
@@ -2253,8 +2258,10 @@
           <t>有机会</t>
         </is>
       </c>
-      <c r="H6" s="2" t="n">
-        <v>105</v>
+      <c r="H6" s="2" t="inlineStr">
+        <is>
+          <t>115</t>
+        </is>
       </c>
       <c r="I6" s="41" t="n">
         <v>2.196</v>
@@ -3451,8 +3458,10 @@
           <t>11月大幅下降，是因为分红,盘子太大</t>
         </is>
       </c>
-      <c r="H14" s="2" t="n">
-        <v>104</v>
+      <c r="H14" s="2" t="inlineStr">
+        <is>
+          <t>114</t>
+        </is>
       </c>
       <c r="I14" s="41" t="n">
         <v>4.8361</v>
@@ -3757,8 +3766,10 @@
           <t>少</t>
         </is>
       </c>
-      <c r="H16" s="2" t="n">
-        <v>105</v>
+      <c r="H16" s="2" t="inlineStr">
+        <is>
+          <t>115</t>
+        </is>
       </c>
       <c r="I16" s="41" t="n">
         <v>1.712</v>
@@ -4654,8 +4665,10 @@
           <t>2.473, 2.472, 2.439, 2.467, 2.458, 2.43, 2.451, 2.407, 2.433, 2.448, 2.478, 2.478, 2.507, 2.501, 2.509, 2.484, 2.504, 2.484, 2.492, 2.514, 2.534, 2.559, 2.535, 2.545, 2.543, 2.562, 2.575, 2.575, 2.56, 2.565, 2.574, 2.569, 2.577, 2.577, 2.579, 2.596, 2.597, 2.6, 2.588, 2.586, 2.591, 2.623, 2.625, 2.643, 2.64, 2.629, 2.6, 2.582, 2.6, 2.61, 2.631, 2.621, 2.619, 2.633, 2.647, 2.65, 2.664, 2.667, 2.668, 2.688</t>
         </is>
       </c>
-      <c r="H22" s="2" t="n">
-        <v>103</v>
+      <c r="H22" s="2" t="inlineStr">
+        <is>
+          <t>113</t>
+        </is>
       </c>
       <c r="I22" s="43" t="n">
         <v>2.688</v>
@@ -5732,8 +5745,10 @@
           <t>1.7582, 1.7673, 1.7644, 1.7642, 1.7661, 1.7506, 1.7709, 1.7667, 1.7823, 1.8018, 1.8127, 1.8165, 1.8116, 1.814, 1.7913, 1.7937, 1.7938, 1.7787, 1.7791, 1.7916, 1.8, 1.8027, 1.7847, 1.7984, 1.8323, 1.8423, 1.8501, 1.8439, 1.845, 1.8371, 1.8083, 1.8142, 1.8209, 1.823, 1.8148, 1.8259, 1.8422, 1.8237, 1.8085, 1.7809, 1.7907, 1.7907, 1.7898, 1.7839, 1.7542, 1.7555, 1.7626, 1.7641, 1.7722, 1.7847, 1.775, 1.7794, 1.7841, 1.7774, 1.8144, 1.8057, 1.8216, 1.8156, 1.8097, 1.8065</t>
         </is>
       </c>
-      <c r="H30" s="0" t="n">
-        <v>100</v>
+      <c r="H30" s="0" t="inlineStr">
+        <is>
+          <t>110</t>
+        </is>
       </c>
       <c r="I30" s="47" t="n">
         <v>1.8065</v>
@@ -5996,8 +6011,10 @@
           <t>0.861, 0.86, 0.824, 0.792, 0.819, 0.799, 0.773, 0.785, 0.817, 0.818, 0.835, 0.803, 0.799, 0.805, 0.785, 0.782, 0.798, 0.79, 0.784, 0.8, 0.823, 0.8, 0.818, 0.808, 0.82, 0.841, 0.857, 0.842, 0.838, 0.833, 0.825, 0.824, 0.853, 0.874, 0.87, 0.857, 0.874, 0.869, 0.864, 0.831, 0.808, 0.819, 0.836, 0.839, 0.837, 0.854, 0.864, 0.874, 0.892, 0.91, 0.928, 0.951, 0.946, 0.951, 0.962, 1.006, 1.017, 1.022, 1.006, 0.991</t>
         </is>
       </c>
-      <c r="H32" s="0" t="n">
-        <v>100</v>
+      <c r="H32" s="0" t="inlineStr">
+        <is>
+          <t>110</t>
+        </is>
       </c>
       <c r="I32" s="47" t="n">
         <v>0.991</v>
@@ -6656,8 +6673,10 @@
           <t>1.126, 1.13, 1.095, 1.058, 1.078, 1.053, 1.04, 1.047, 1.071, 1.066, 1.092, 1.06, 1.054, 1.063, 1.052, 1.05, 1.069, 1.062, 1.061, 1.08, 1.101, 1.088, 1.094, 1.086, 1.092, 1.111, 1.123, 1.118, 1.118, 1.12, 1.102, 1.101, 1.116, 1.128, 1.119, 1.112, 1.136, 1.135, 1.132, 1.125, 1.103, 1.109, 1.13, 1.13, 1.133, 1.142, 1.16, 1.154, 1.174, 1.194, 1.189, 1.205, 1.197, 1.203, 1.221, 1.24, 1.247, 1.244, 1.236, 1.224</t>
         </is>
       </c>
-      <c r="H37" s="0" t="n">
-        <v>100</v>
+      <c r="H37" s="0" t="inlineStr">
+        <is>
+          <t>110</t>
+        </is>
       </c>
       <c r="I37" s="47" t="n">
         <v>1.224</v>

</xml_diff>

<commit_message>
catch get current price TypeError exception. modify HSI name.
</commit_message>
<xml_diff>
--- a/fund/Jelly_model.xlsx
+++ b/fund/Jelly_model.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22368" windowHeight="9420" activeTab="1"/>
+    <workbookView windowWidth="22368" windowHeight="9420" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="基金" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1475" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1475" uniqueCount="507">
   <si>
     <t>编号</t>
   </si>
@@ -1125,9 +1125,6 @@
   </si>
   <si>
     <t>320007</t>
-  </si>
-  <si>
-    <t>100.HSI</t>
   </si>
   <si>
     <t>恒生指数组合</t>
@@ -7842,7 +7839,7 @@
   <sheetPr/>
   <dimension ref="A1:CS41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
@@ -10772,8 +10769,8 @@
   <sheetPr/>
   <dimension ref="A1:AG37"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="Z3" sqref="Z3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -10975,28 +10972,28 @@
         <v>153</v>
       </c>
       <c r="Z2" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="AA2" t="s">
         <v>369</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>370</v>
       </c>
       <c r="AB2" s="10" t="s">
         <v>265</v>
       </c>
       <c r="AC2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="AD2" s="10" t="s">
         <v>263</v>
       </c>
       <c r="AE2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="AF2" s="10" t="s">
         <v>249</v>
       </c>
       <c r="AG2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="3" spans="1:33">
@@ -11310,7 +11307,7 @@
         <v>20190909</v>
       </c>
       <c r="C6" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D6" t="s">
         <v>185</v>
@@ -11512,7 +11509,7 @@
         <v>20191008</v>
       </c>
       <c r="C8" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D8" t="s">
         <v>185</v>
@@ -11714,7 +11711,7 @@
         <v>141</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D10" t="s">
         <v>185</v>
@@ -11913,10 +11910,10 @@
         <v>12</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D12" t="s">
         <v>185</v>
@@ -12118,7 +12115,7 @@
         <v>178</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D14">
         <v>13000</v>
@@ -12320,7 +12317,7 @@
         <v>253</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D16" t="s">
         <v>185</v>
@@ -12519,10 +12516,10 @@
         <v>18</v>
       </c>
       <c r="B18" s="10" t="s">
+        <v>376</v>
+      </c>
+      <c r="C18" s="10" t="s">
         <v>377</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>378</v>
       </c>
       <c r="D18" t="s">
         <v>185</v>
@@ -12617,7 +12614,7 @@
     </row>
     <row r="19" spans="1:33">
       <c r="A19" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B19" t="s">
         <v>185</v>
@@ -12718,34 +12715,34 @@
     </row>
     <row r="20" spans="1:33">
       <c r="A20" t="s">
+        <v>379</v>
+      </c>
+      <c r="B20" t="s">
         <v>380</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
+        <v>373</v>
+      </c>
+      <c r="D20" t="s">
+        <v>185</v>
+      </c>
+      <c r="E20" t="s">
+        <v>185</v>
+      </c>
+      <c r="F20" t="s">
+        <v>185</v>
+      </c>
+      <c r="G20" t="s">
+        <v>185</v>
+      </c>
+      <c r="H20" t="s">
         <v>381</v>
-      </c>
-      <c r="C20" t="s">
-        <v>374</v>
-      </c>
-      <c r="D20" t="s">
-        <v>185</v>
-      </c>
-      <c r="E20" t="s">
-        <v>185</v>
-      </c>
-      <c r="F20" t="s">
-        <v>185</v>
-      </c>
-      <c r="G20" t="s">
-        <v>185</v>
-      </c>
-      <c r="H20" t="s">
-        <v>382</v>
       </c>
       <c r="I20">
         <v>2.2221</v>
       </c>
       <c r="J20" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="K20">
         <v>2.184</v>
@@ -12819,7 +12816,7 @@
     </row>
     <row r="21" spans="1:33">
       <c r="A21" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B21" t="s">
         <v>185</v>
@@ -12920,13 +12917,13 @@
     </row>
     <row r="22" spans="1:33">
       <c r="A22" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B22" t="s">
         <v>174</v>
       </c>
       <c r="C22" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D22" t="s">
         <v>185</v>
@@ -12959,19 +12956,19 @@
         <v>185</v>
       </c>
       <c r="N22" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="O22">
         <v>1.244</v>
       </c>
       <c r="P22" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="Q22">
         <v>1.022</v>
       </c>
       <c r="R22" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="S22">
         <v>1.8156</v>
@@ -13021,7 +13018,7 @@
     </row>
     <row r="23" spans="1:33">
       <c r="A23" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B23" t="s">
         <v>185</v>
@@ -13122,13 +13119,13 @@
     </row>
     <row r="24" spans="1:33">
       <c r="A24" t="s">
+        <v>387</v>
+      </c>
+      <c r="B24" s="10" t="s">
         <v>388</v>
       </c>
-      <c r="B24" s="10" t="s">
-        <v>389</v>
-      </c>
       <c r="C24" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D24" t="s">
         <v>185</v>
@@ -13155,7 +13152,7 @@
         <v>185</v>
       </c>
       <c r="L24" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="M24">
         <v>1.282</v>
@@ -13324,85 +13321,85 @@
     </row>
     <row r="26" spans="1:33">
       <c r="A26" t="s">
+        <v>389</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>376</v>
+      </c>
+      <c r="C26" t="s">
+        <v>373</v>
+      </c>
+      <c r="D26" t="s">
+        <v>185</v>
+      </c>
+      <c r="E26" t="s">
+        <v>185</v>
+      </c>
+      <c r="F26" t="s">
+        <v>185</v>
+      </c>
+      <c r="G26" t="s">
+        <v>185</v>
+      </c>
+      <c r="H26" t="s">
+        <v>185</v>
+      </c>
+      <c r="I26" t="s">
+        <v>185</v>
+      </c>
+      <c r="J26" t="s">
+        <v>185</v>
+      </c>
+      <c r="K26" t="s">
+        <v>185</v>
+      </c>
+      <c r="L26" t="s">
+        <v>185</v>
+      </c>
+      <c r="M26" t="s">
+        <v>185</v>
+      </c>
+      <c r="N26" t="s">
+        <v>185</v>
+      </c>
+      <c r="O26" t="s">
+        <v>185</v>
+      </c>
+      <c r="P26" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>185</v>
+      </c>
+      <c r="R26" t="s">
+        <v>185</v>
+      </c>
+      <c r="S26" t="s">
+        <v>185</v>
+      </c>
+      <c r="T26" t="s">
+        <v>185</v>
+      </c>
+      <c r="U26" t="s">
+        <v>185</v>
+      </c>
+      <c r="V26" t="s">
+        <v>185</v>
+      </c>
+      <c r="W26" t="s">
+        <v>185</v>
+      </c>
+      <c r="X26" t="s">
+        <v>185</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z26" t="s">
         <v>390</v>
       </c>
-      <c r="B26" s="10" t="s">
-        <v>377</v>
-      </c>
-      <c r="C26" t="s">
-        <v>374</v>
-      </c>
-      <c r="D26" t="s">
-        <v>185</v>
-      </c>
-      <c r="E26" t="s">
-        <v>185</v>
-      </c>
-      <c r="F26" t="s">
-        <v>185</v>
-      </c>
-      <c r="G26" t="s">
-        <v>185</v>
-      </c>
-      <c r="H26" t="s">
-        <v>185</v>
-      </c>
-      <c r="I26" t="s">
-        <v>185</v>
-      </c>
-      <c r="J26" t="s">
-        <v>185</v>
-      </c>
-      <c r="K26" t="s">
-        <v>185</v>
-      </c>
-      <c r="L26" t="s">
-        <v>185</v>
-      </c>
-      <c r="M26" t="s">
-        <v>185</v>
-      </c>
-      <c r="N26" t="s">
-        <v>185</v>
-      </c>
-      <c r="O26" t="s">
-        <v>185</v>
-      </c>
-      <c r="P26" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>185</v>
-      </c>
-      <c r="R26" t="s">
-        <v>185</v>
-      </c>
-      <c r="S26" t="s">
-        <v>185</v>
-      </c>
-      <c r="T26" t="s">
-        <v>185</v>
-      </c>
-      <c r="U26" t="s">
-        <v>185</v>
-      </c>
-      <c r="V26" t="s">
-        <v>185</v>
-      </c>
-      <c r="W26" t="s">
-        <v>185</v>
-      </c>
-      <c r="X26" t="s">
-        <v>185</v>
-      </c>
-      <c r="Y26" t="s">
-        <v>185</v>
-      </c>
-      <c r="Z26" t="s">
+      <c r="AA26" t="s">
         <v>391</v>
-      </c>
-      <c r="AA26" t="s">
-        <v>392</v>
       </c>
       <c r="AB26" t="s">
         <v>185</v>
@@ -13425,7 +13422,7 @@
     </row>
     <row r="27" spans="1:33">
       <c r="A27" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B27" t="s">
         <v>185</v>
@@ -13526,13 +13523,13 @@
     </row>
     <row r="28" spans="1:33">
       <c r="A28" t="s">
+        <v>393</v>
+      </c>
+      <c r="B28" t="s">
         <v>394</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>395</v>
-      </c>
-      <c r="C28" t="s">
-        <v>396</v>
       </c>
       <c r="D28" s="13">
         <v>13000</v>
@@ -13627,25 +13624,25 @@
     </row>
     <row r="29" spans="1:33">
       <c r="A29" t="s">
+        <v>396</v>
+      </c>
+      <c r="B29" s="10" t="s">
         <v>397</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="C29" s="10" t="s">
         <v>398</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>399</v>
       </c>
       <c r="D29">
         <v>2031.05</v>
       </c>
       <c r="E29" t="s">
+        <v>399</v>
+      </c>
+      <c r="F29" t="s">
         <v>400</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>401</v>
-      </c>
-      <c r="G29" t="s">
-        <v>402</v>
       </c>
       <c r="H29">
         <v>-19.41</v>
@@ -13657,7 +13654,7 @@
         <v>145.67</v>
       </c>
       <c r="K29" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="L29">
         <v>-34.76</v>
@@ -13669,7 +13666,7 @@
         <v>39.75</v>
       </c>
       <c r="O29" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="P29">
         <v>-139.32</v>
@@ -13681,34 +13678,34 @@
         <v>42.09</v>
       </c>
       <c r="S29" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="T29">
         <v>24.4</v>
       </c>
       <c r="U29" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="V29">
         <v>15.72</v>
       </c>
       <c r="W29" t="s">
+        <v>406</v>
+      </c>
+      <c r="X29" t="s">
+        <v>185</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z29" t="s">
         <v>407</v>
-      </c>
-      <c r="X29" t="s">
-        <v>185</v>
-      </c>
-      <c r="Y29" t="s">
-        <v>185</v>
-      </c>
-      <c r="Z29" t="s">
-        <v>408</v>
       </c>
       <c r="AA29">
         <v>3.44</v>
       </c>
       <c r="AB29" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="AC29">
         <v>4.79</v>
@@ -32683,28 +32680,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
+        <v>409</v>
+      </c>
+      <c r="B1" t="s">
         <v>410</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>411</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>412</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>413</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>414</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>415</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>416</v>
-      </c>
-      <c r="H1" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -32715,13 +32712,13 @@
         <v>20191011</v>
       </c>
       <c r="C2" t="s">
+        <v>417</v>
+      </c>
+      <c r="D2" t="s">
         <v>418</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>419</v>
-      </c>
-      <c r="E2" t="s">
-        <v>420</v>
       </c>
       <c r="F2">
         <v>8</v>
@@ -32730,7 +32727,7 @@
         <v>185</v>
       </c>
       <c r="H2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -32741,13 +32738,13 @@
         <v>20191211</v>
       </c>
       <c r="C3" t="s">
+        <v>421</v>
+      </c>
+      <c r="D3" t="s">
         <v>422</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>423</v>
-      </c>
-      <c r="E3" t="s">
-        <v>424</v>
       </c>
       <c r="F3">
         <v>3</v>
@@ -32756,111 +32753,111 @@
         <v>185</v>
       </c>
       <c r="H3" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B4" t="s">
         <v>165</v>
       </c>
       <c r="C4" t="s">
+        <v>426</v>
+      </c>
+      <c r="D4" t="s">
         <v>427</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>428</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>429</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>430</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>431</v>
-      </c>
-      <c r="H4" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B5" t="s">
+        <v>432</v>
+      </c>
+      <c r="C5" t="s">
         <v>433</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>434</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
+        <v>423</v>
+      </c>
+      <c r="F5" t="s">
         <v>435</v>
       </c>
-      <c r="E5" t="s">
-        <v>424</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>436</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>437</v>
-      </c>
-      <c r="H5" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
+        <v>438</v>
+      </c>
+      <c r="B6" t="s">
         <v>439</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D6" t="s">
+        <v>185</v>
+      </c>
+      <c r="E6" t="s">
+        <v>185</v>
+      </c>
+      <c r="F6" t="s">
+        <v>185</v>
+      </c>
+      <c r="G6" t="s">
+        <v>185</v>
+      </c>
+      <c r="H6" t="s">
         <v>440</v>
-      </c>
-      <c r="C6" t="s">
-        <v>185</v>
-      </c>
-      <c r="D6" t="s">
-        <v>185</v>
-      </c>
-      <c r="E6" t="s">
-        <v>185</v>
-      </c>
-      <c r="F6" t="s">
-        <v>185</v>
-      </c>
-      <c r="G6" t="s">
-        <v>185</v>
-      </c>
-      <c r="H6" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="7" ht="201.6" customHeight="1" spans="1:8">
       <c r="A7" t="s">
+        <v>441</v>
+      </c>
+      <c r="B7" t="s">
         <v>442</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>443</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>444</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
+        <v>423</v>
+      </c>
+      <c r="F7" t="s">
+        <v>185</v>
+      </c>
+      <c r="G7" t="s">
+        <v>185</v>
+      </c>
+      <c r="H7" s="9" t="s">
         <v>445</v>
-      </c>
-      <c r="E7" t="s">
-        <v>424</v>
-      </c>
-      <c r="F7" t="s">
-        <v>185</v>
-      </c>
-      <c r="G7" t="s">
-        <v>185</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="8" ht="43.2" customHeight="1" spans="1:8">
@@ -32871,13 +32868,13 @@
         <v>20191222</v>
       </c>
       <c r="C8" t="s">
+        <v>443</v>
+      </c>
+      <c r="D8" t="s">
         <v>444</v>
       </c>
-      <c r="D8" t="s">
-        <v>445</v>
-      </c>
       <c r="E8" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F8" t="s">
         <v>185</v>
@@ -32886,137 +32883,137 @@
         <v>185</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B9" t="s">
+        <v>447</v>
+      </c>
+      <c r="C9" t="s">
+        <v>185</v>
+      </c>
+      <c r="D9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E9" t="s">
+        <v>185</v>
+      </c>
+      <c r="F9" t="s">
+        <v>185</v>
+      </c>
+      <c r="G9" t="s">
+        <v>185</v>
+      </c>
+      <c r="H9" t="s">
         <v>448</v>
-      </c>
-      <c r="C9" t="s">
-        <v>185</v>
-      </c>
-      <c r="D9" t="s">
-        <v>185</v>
-      </c>
-      <c r="E9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F9" t="s">
-        <v>185</v>
-      </c>
-      <c r="G9" t="s">
-        <v>185</v>
-      </c>
-      <c r="H9" t="s">
-        <v>449</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
+        <v>449</v>
+      </c>
+      <c r="B10" t="s">
         <v>450</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
+        <v>185</v>
+      </c>
+      <c r="D10" t="s">
+        <v>185</v>
+      </c>
+      <c r="E10" t="s">
+        <v>185</v>
+      </c>
+      <c r="F10" t="s">
+        <v>185</v>
+      </c>
+      <c r="G10" t="s">
+        <v>185</v>
+      </c>
+      <c r="H10" t="s">
         <v>451</v>
-      </c>
-      <c r="C10" t="s">
-        <v>185</v>
-      </c>
-      <c r="D10" t="s">
-        <v>185</v>
-      </c>
-      <c r="E10" t="s">
-        <v>185</v>
-      </c>
-      <c r="F10" t="s">
-        <v>185</v>
-      </c>
-      <c r="G10" t="s">
-        <v>185</v>
-      </c>
-      <c r="H10" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
+        <v>452</v>
+      </c>
+      <c r="B11" t="s">
+        <v>394</v>
+      </c>
+      <c r="C11" t="s">
+        <v>185</v>
+      </c>
+      <c r="D11" t="s">
+        <v>185</v>
+      </c>
+      <c r="E11" t="s">
+        <v>185</v>
+      </c>
+      <c r="F11" t="s">
+        <v>185</v>
+      </c>
+      <c r="G11" t="s">
+        <v>185</v>
+      </c>
+      <c r="H11" t="s">
         <v>453</v>
-      </c>
-      <c r="B11" t="s">
-        <v>395</v>
-      </c>
-      <c r="C11" t="s">
-        <v>185</v>
-      </c>
-      <c r="D11" t="s">
-        <v>185</v>
-      </c>
-      <c r="E11" t="s">
-        <v>185</v>
-      </c>
-      <c r="F11" t="s">
-        <v>185</v>
-      </c>
-      <c r="G11" t="s">
-        <v>185</v>
-      </c>
-      <c r="H11" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
+        <v>454</v>
+      </c>
+      <c r="B12" t="s">
         <v>455</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
+        <v>185</v>
+      </c>
+      <c r="D12" t="s">
+        <v>185</v>
+      </c>
+      <c r="E12" t="s">
+        <v>185</v>
+      </c>
+      <c r="F12" t="s">
+        <v>185</v>
+      </c>
+      <c r="G12" t="s">
+        <v>185</v>
+      </c>
+      <c r="H12" t="s">
         <v>456</v>
-      </c>
-      <c r="C12" t="s">
-        <v>185</v>
-      </c>
-      <c r="D12" t="s">
-        <v>185</v>
-      </c>
-      <c r="E12" t="s">
-        <v>185</v>
-      </c>
-      <c r="F12" t="s">
-        <v>185</v>
-      </c>
-      <c r="G12" t="s">
-        <v>185</v>
-      </c>
-      <c r="H12" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
+        <v>457</v>
+      </c>
+      <c r="B13" t="s">
+        <v>455</v>
+      </c>
+      <c r="C13" t="s">
+        <v>185</v>
+      </c>
+      <c r="D13" t="s">
+        <v>185</v>
+      </c>
+      <c r="E13" t="s">
+        <v>185</v>
+      </c>
+      <c r="F13" t="s">
+        <v>185</v>
+      </c>
+      <c r="G13" t="s">
+        <v>185</v>
+      </c>
+      <c r="H13" t="s">
         <v>458</v>
-      </c>
-      <c r="B13" t="s">
-        <v>456</v>
-      </c>
-      <c r="C13" t="s">
-        <v>185</v>
-      </c>
-      <c r="D13" t="s">
-        <v>185</v>
-      </c>
-      <c r="E13" t="s">
-        <v>185</v>
-      </c>
-      <c r="F13" t="s">
-        <v>185</v>
-      </c>
-      <c r="G13" t="s">
-        <v>185</v>
-      </c>
-      <c r="H13" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -33027,7 +33024,7 @@
         <v>20200105</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
   </sheetData>
@@ -33055,110 +33052,110 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="2" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2"/>
       <c r="B2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="3" spans="2:2">
       <c r="B3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="4" spans="2:2">
       <c r="B4" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="2" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="C11" t="s">
         <v>467</v>
-      </c>
-      <c r="C11" t="s">
-        <v>468</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="13" spans="2:2">
       <c r="B13" s="3" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="14" spans="2:2">
       <c r="B14" s="3" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="15" spans="2:2">
       <c r="B15" s="3" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B16" s="3"/>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="20" spans="2:2">
       <c r="B20" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="23" spans="2:2">
       <c r="B23" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="24" spans="2:13">
       <c r="B24" s="4" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C24" s="4"/>
       <c r="F24" s="4" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="G24" s="5"/>
       <c r="J24" s="4" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
@@ -33166,7 +33163,7 @@
     </row>
     <row r="25" spans="2:13">
       <c r="B25" s="6" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C25" s="7"/>
       <c r="F25" s="4"/>
@@ -33175,12 +33172,12 @@
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
       <c r="M25" s="5" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="26" spans="2:14">
       <c r="B26" s="6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>1</v>
@@ -33189,106 +33186,106 @@
         <v>363</v>
       </c>
       <c r="G26" s="6" t="s">
+        <v>483</v>
+      </c>
+      <c r="H26" s="6" t="s">
         <v>484</v>
       </c>
-      <c r="H26" s="6" t="s">
+      <c r="J26" s="8" t="s">
         <v>485</v>
       </c>
-      <c r="J26" s="8" t="s">
+      <c r="K26" s="8" t="s">
         <v>486</v>
-      </c>
-      <c r="K26" s="8" t="s">
-        <v>487</v>
       </c>
       <c r="L26" s="8"/>
       <c r="M26" s="6" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="N26" s="6"/>
     </row>
     <row r="27" spans="2:14">
       <c r="B27" s="6" t="s">
+        <v>488</v>
+      </c>
+      <c r="C27" s="6" t="s">
         <v>489</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>490</v>
       </c>
       <c r="F27" s="8"/>
       <c r="G27" s="6" t="s">
+        <v>490</v>
+      </c>
+      <c r="H27" s="6" t="s">
         <v>491</v>
       </c>
-      <c r="H27" s="6" t="s">
+      <c r="J27" s="8" t="s">
         <v>492</v>
       </c>
-      <c r="J27" s="8" t="s">
+      <c r="K27" s="8" t="s">
         <v>493</v>
-      </c>
-      <c r="K27" s="8" t="s">
-        <v>494</v>
       </c>
       <c r="L27" s="8"/>
       <c r="M27" s="6" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="N27" s="6" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="28" spans="2:13">
       <c r="B28" s="6" t="s">
+        <v>495</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>493</v>
+      </c>
+      <c r="M28" t="s">
         <v>496</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>494</v>
-      </c>
-      <c r="M28" t="s">
-        <v>497</v>
       </c>
     </row>
     <row r="29" spans="2:13">
       <c r="B29" s="6" t="s">
+        <v>497</v>
+      </c>
+      <c r="C29" s="6" t="s">
         <v>498</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="M29" t="s">
         <v>499</v>
-      </c>
-      <c r="M29" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="34" spans="2:2">
       <c r="B34" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="35" spans="2:2">
       <c r="B35" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="36" spans="2:2">
       <c r="B36" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="37" spans="2:2">
       <c r="B37" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rename HSI to 100.HSI, avoid get current price for HSI got exception: 'NoneType' object is not iterable. because cols obj list is None.
</commit_message>
<xml_diff>
--- a/fund/Jelly_model.xlsx
+++ b/fund/Jelly_model.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22368" windowHeight="9420" activeTab="1"/>
+    <workbookView windowWidth="22368" windowHeight="9420" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="基金" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1725" uniqueCount="515">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1725" uniqueCount="514">
   <si>
     <t>编号</t>
   </si>
@@ -1146,9 +1146,6 @@
   </si>
   <si>
     <t>320007</t>
-  </si>
-  <si>
-    <t>HSI</t>
   </si>
   <si>
     <t>恒生指数组合</t>
@@ -1588,10 +1585,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
     <numFmt numFmtId="177" formatCode="0.00_ "/>
     <numFmt numFmtId="178" formatCode="yyyy/m/d;@"/>
@@ -1631,13 +1628,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -1645,61 +1635,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1714,7 +1650,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1722,7 +1673,30 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1744,23 +1718,46 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1805,13 +1802,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1823,31 +1916,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1859,67 +1970,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1931,61 +1982,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2018,60 +2015,6 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -2094,11 +2037,39 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2106,8 +2077,34 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2119,10 +2116,10 @@
     <xf numFmtId="42" fontId="3" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="5">
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="5">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0">
@@ -2131,16 +2128,16 @@
     <xf numFmtId="41" fontId="3" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0">
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
@@ -2149,97 +2146,94 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="7">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0">
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="6">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="4">
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="5">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="5">
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="8">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="3">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0">
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="37" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0">
+    <xf numFmtId="0" fontId="5" fillId="36" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="36" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="35" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0">
@@ -2248,16 +2242,19 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0">
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0">
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -7857,7 +7854,7 @@
   <sheetPr/>
   <dimension ref="A1:CS41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -12884,8 +12881,8 @@
   <sheetPr/>
   <dimension ref="A1:AG37"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="Z3" sqref="Z3"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="Z2" sqref="Z2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -13087,28 +13084,28 @@
         <v>154</v>
       </c>
       <c r="Z2" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="AA2" t="s">
         <v>376</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>377</v>
       </c>
       <c r="AB2" s="10" t="s">
         <v>268</v>
       </c>
       <c r="AC2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="AD2" s="10" t="s">
         <v>266</v>
       </c>
       <c r="AE2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="AF2" s="10" t="s">
         <v>252</v>
       </c>
       <c r="AG2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="3" spans="1:33">
@@ -13422,7 +13419,7 @@
         <v>20190909</v>
       </c>
       <c r="C6" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D6" t="s">
         <v>70</v>
@@ -13624,7 +13621,7 @@
         <v>20191008</v>
       </c>
       <c r="C8" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D8" t="s">
         <v>70</v>
@@ -13826,7 +13823,7 @@
         <v>142</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D10" t="s">
         <v>70</v>
@@ -14025,10 +14022,10 @@
         <v>12</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D12" t="s">
         <v>70</v>
@@ -14230,7 +14227,7 @@
         <v>179</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D14">
         <v>13000</v>
@@ -14432,7 +14429,7 @@
         <v>256</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D16" t="s">
         <v>70</v>
@@ -14631,10 +14628,10 @@
         <v>18</v>
       </c>
       <c r="B18" s="10" t="s">
+        <v>383</v>
+      </c>
+      <c r="C18" s="10" t="s">
         <v>384</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>385</v>
       </c>
       <c r="D18" t="s">
         <v>70</v>
@@ -14729,7 +14726,7 @@
     </row>
     <row r="19" spans="1:33">
       <c r="A19" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B19" t="s">
         <v>70</v>
@@ -14830,34 +14827,34 @@
     </row>
     <row r="20" spans="1:33">
       <c r="A20" t="s">
+        <v>386</v>
+      </c>
+      <c r="B20" t="s">
         <v>387</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
+        <v>380</v>
+      </c>
+      <c r="D20" t="s">
+        <v>70</v>
+      </c>
+      <c r="E20" t="s">
+        <v>70</v>
+      </c>
+      <c r="F20" t="s">
+        <v>70</v>
+      </c>
+      <c r="G20" t="s">
+        <v>70</v>
+      </c>
+      <c r="H20" t="s">
         <v>388</v>
-      </c>
-      <c r="C20" t="s">
-        <v>381</v>
-      </c>
-      <c r="D20" t="s">
-        <v>70</v>
-      </c>
-      <c r="E20" t="s">
-        <v>70</v>
-      </c>
-      <c r="F20" t="s">
-        <v>70</v>
-      </c>
-      <c r="G20" t="s">
-        <v>70</v>
-      </c>
-      <c r="H20" t="s">
-        <v>389</v>
       </c>
       <c r="I20">
         <v>2.2221</v>
       </c>
       <c r="J20" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="K20">
         <v>2.184</v>
@@ -14931,7 +14928,7 @@
     </row>
     <row r="21" spans="1:33">
       <c r="A21" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B21" t="s">
         <v>70</v>
@@ -15032,13 +15029,13 @@
     </row>
     <row r="22" spans="1:33">
       <c r="A22" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B22" t="s">
         <v>175</v>
       </c>
       <c r="C22" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D22" t="s">
         <v>70</v>
@@ -15071,19 +15068,19 @@
         <v>70</v>
       </c>
       <c r="N22" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="O22">
         <v>1.244</v>
       </c>
       <c r="P22" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="Q22">
         <v>1.022</v>
       </c>
       <c r="R22" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="S22">
         <v>1.8156</v>
@@ -15133,7 +15130,7 @@
     </row>
     <row r="23" spans="1:33">
       <c r="A23" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B23" t="s">
         <v>70</v>
@@ -15234,13 +15231,13 @@
     </row>
     <row r="24" spans="1:33">
       <c r="A24" t="s">
+        <v>394</v>
+      </c>
+      <c r="B24" s="10" t="s">
         <v>395</v>
       </c>
-      <c r="B24" s="10" t="s">
-        <v>396</v>
-      </c>
       <c r="C24" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D24" t="s">
         <v>70</v>
@@ -15267,7 +15264,7 @@
         <v>70</v>
       </c>
       <c r="L24" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="M24">
         <v>1.282</v>
@@ -15436,85 +15433,85 @@
     </row>
     <row r="26" spans="1:33">
       <c r="A26" t="s">
+        <v>396</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>383</v>
+      </c>
+      <c r="C26" t="s">
+        <v>380</v>
+      </c>
+      <c r="D26" t="s">
+        <v>70</v>
+      </c>
+      <c r="E26" t="s">
+        <v>70</v>
+      </c>
+      <c r="F26" t="s">
+        <v>70</v>
+      </c>
+      <c r="G26" t="s">
+        <v>70</v>
+      </c>
+      <c r="H26" t="s">
+        <v>70</v>
+      </c>
+      <c r="I26" t="s">
+        <v>70</v>
+      </c>
+      <c r="J26" t="s">
+        <v>70</v>
+      </c>
+      <c r="K26" t="s">
+        <v>70</v>
+      </c>
+      <c r="L26" t="s">
+        <v>70</v>
+      </c>
+      <c r="M26" t="s">
+        <v>70</v>
+      </c>
+      <c r="N26" t="s">
+        <v>70</v>
+      </c>
+      <c r="O26" t="s">
+        <v>70</v>
+      </c>
+      <c r="P26" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>70</v>
+      </c>
+      <c r="R26" t="s">
+        <v>70</v>
+      </c>
+      <c r="S26" t="s">
+        <v>70</v>
+      </c>
+      <c r="T26" t="s">
+        <v>70</v>
+      </c>
+      <c r="U26" t="s">
+        <v>70</v>
+      </c>
+      <c r="V26" t="s">
+        <v>70</v>
+      </c>
+      <c r="W26" t="s">
+        <v>70</v>
+      </c>
+      <c r="X26" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z26" t="s">
         <v>397</v>
       </c>
-      <c r="B26" s="10" t="s">
-        <v>384</v>
-      </c>
-      <c r="C26" t="s">
-        <v>381</v>
-      </c>
-      <c r="D26" t="s">
-        <v>70</v>
-      </c>
-      <c r="E26" t="s">
-        <v>70</v>
-      </c>
-      <c r="F26" t="s">
-        <v>70</v>
-      </c>
-      <c r="G26" t="s">
-        <v>70</v>
-      </c>
-      <c r="H26" t="s">
-        <v>70</v>
-      </c>
-      <c r="I26" t="s">
-        <v>70</v>
-      </c>
-      <c r="J26" t="s">
-        <v>70</v>
-      </c>
-      <c r="K26" t="s">
-        <v>70</v>
-      </c>
-      <c r="L26" t="s">
-        <v>70</v>
-      </c>
-      <c r="M26" t="s">
-        <v>70</v>
-      </c>
-      <c r="N26" t="s">
-        <v>70</v>
-      </c>
-      <c r="O26" t="s">
-        <v>70</v>
-      </c>
-      <c r="P26" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>70</v>
-      </c>
-      <c r="R26" t="s">
-        <v>70</v>
-      </c>
-      <c r="S26" t="s">
-        <v>70</v>
-      </c>
-      <c r="T26" t="s">
-        <v>70</v>
-      </c>
-      <c r="U26" t="s">
-        <v>70</v>
-      </c>
-      <c r="V26" t="s">
-        <v>70</v>
-      </c>
-      <c r="W26" t="s">
-        <v>70</v>
-      </c>
-      <c r="X26" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y26" t="s">
-        <v>70</v>
-      </c>
-      <c r="Z26" t="s">
+      <c r="AA26" t="s">
         <v>398</v>
-      </c>
-      <c r="AA26" t="s">
-        <v>399</v>
       </c>
       <c r="AB26" t="s">
         <v>70</v>
@@ -15537,7 +15534,7 @@
     </row>
     <row r="27" spans="1:33">
       <c r="A27" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B27" t="s">
         <v>70</v>
@@ -15638,13 +15635,13 @@
     </row>
     <row r="28" spans="1:33">
       <c r="A28" t="s">
+        <v>400</v>
+      </c>
+      <c r="B28" t="s">
         <v>401</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>402</v>
-      </c>
-      <c r="C28" t="s">
-        <v>403</v>
       </c>
       <c r="D28" s="13">
         <v>13000</v>
@@ -15739,25 +15736,25 @@
     </row>
     <row r="29" spans="1:33">
       <c r="A29" t="s">
+        <v>403</v>
+      </c>
+      <c r="B29" s="10" t="s">
         <v>404</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="C29" s="10" t="s">
         <v>405</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>406</v>
       </c>
       <c r="D29">
         <v>2031.05</v>
       </c>
       <c r="E29" t="s">
+        <v>406</v>
+      </c>
+      <c r="F29" t="s">
         <v>407</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>408</v>
-      </c>
-      <c r="G29" t="s">
-        <v>409</v>
       </c>
       <c r="H29">
         <v>-19.41</v>
@@ -15769,7 +15766,7 @@
         <v>145.67</v>
       </c>
       <c r="K29" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="L29">
         <v>-34.76</v>
@@ -15781,7 +15778,7 @@
         <v>39.75</v>
       </c>
       <c r="O29" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="P29">
         <v>-139.32</v>
@@ -15793,34 +15790,34 @@
         <v>42.09</v>
       </c>
       <c r="S29" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="T29">
         <v>24.4</v>
       </c>
       <c r="U29" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="V29">
         <v>15.72</v>
       </c>
       <c r="W29" t="s">
+        <v>413</v>
+      </c>
+      <c r="X29" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z29" t="s">
         <v>414</v>
-      </c>
-      <c r="X29" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y29" t="s">
-        <v>70</v>
-      </c>
-      <c r="Z29" t="s">
-        <v>415</v>
       </c>
       <c r="AA29">
         <v>3.44</v>
       </c>
       <c r="AB29" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="AC29">
         <v>4.79</v>
@@ -28050,16 +28047,16 @@
     <cfRule type="cellIs" dxfId="7" priority="1864" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6217" stopIfTrue="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6217" stopIfTrue="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6217" stopIfTrue="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6217" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="6218" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="6218" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6218" stopIfTrue="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="6218" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="2019" stopIfTrue="1" operator="greaterThan">
@@ -28068,7 +28065,7 @@
     <cfRule type="cellIs" dxfId="7" priority="2020" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6217" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="6218" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="7" priority="2188" stopIfTrue="1" operator="lessThan">
@@ -28277,19 +28274,19 @@
     <cfRule type="cellIs" dxfId="7" priority="1866" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6217" stopIfTrue="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6217" stopIfTrue="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6217" stopIfTrue="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6217" stopIfTrue="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6217" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="6218" stopIfTrue="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="6218" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6218" stopIfTrue="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="6218" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6218" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="2021" stopIfTrue="1" operator="greaterThan">
@@ -28988,22 +28985,22 @@
     <cfRule type="cellIs" dxfId="7" priority="1796" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6217" stopIfTrue="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6217" stopIfTrue="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6217" stopIfTrue="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6217" stopIfTrue="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6217" stopIfTrue="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6217" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="6218" stopIfTrue="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="6218" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6218" stopIfTrue="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="6218" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6218" stopIfTrue="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="6218" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="1919" stopIfTrue="1" operator="greaterThan">
@@ -29230,22 +29227,22 @@
     <cfRule type="cellIs" dxfId="7" priority="1798" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6217" stopIfTrue="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6217" stopIfTrue="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6217" stopIfTrue="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6217" stopIfTrue="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6217" stopIfTrue="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6217" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="6218" stopIfTrue="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="6218" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6218" stopIfTrue="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="6218" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6218" stopIfTrue="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="6218" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="1921" stopIfTrue="1" operator="greaterThan">
@@ -29466,22 +29463,22 @@
     <cfRule type="cellIs" dxfId="7" priority="1812" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6217" stopIfTrue="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6217" stopIfTrue="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6217" stopIfTrue="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6217" stopIfTrue="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6217" stopIfTrue="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6217" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="6218" stopIfTrue="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="6218" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6218" stopIfTrue="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="6218" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6218" stopIfTrue="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="6218" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="1943" stopIfTrue="1" operator="greaterThan">
@@ -30192,16 +30189,16 @@
     <cfRule type="cellIs" dxfId="7" priority="1822" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6217" stopIfTrue="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6217" stopIfTrue="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6217" stopIfTrue="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6217" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="6218" stopIfTrue="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="6218" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6218" stopIfTrue="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="6218" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="1957" stopIfTrue="1" operator="greaterThan">
@@ -30434,16 +30431,16 @@
     <cfRule type="cellIs" dxfId="7" priority="1828" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6217" stopIfTrue="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6217" stopIfTrue="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6217" stopIfTrue="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6217" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="6218" stopIfTrue="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="6218" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6218" stopIfTrue="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="6218" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="1967" stopIfTrue="1" operator="greaterThan">
@@ -30676,16 +30673,16 @@
     <cfRule type="cellIs" dxfId="7" priority="1830" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6217" stopIfTrue="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6217" stopIfTrue="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6217" stopIfTrue="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6217" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="6218" stopIfTrue="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="6218" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6218" stopIfTrue="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="6218" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="1969" stopIfTrue="1" operator="greaterThan">
@@ -30915,19 +30912,19 @@
     <cfRule type="cellIs" dxfId="7" priority="1836" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6217" stopIfTrue="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6217" stopIfTrue="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6217" stopIfTrue="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6217" stopIfTrue="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6217" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="6218" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6218" stopIfTrue="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="6218" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6218" stopIfTrue="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="6218" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="1979" stopIfTrue="1" operator="greaterThan">
@@ -31154,22 +31151,22 @@
     <cfRule type="cellIs" dxfId="7" priority="1838" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6217" stopIfTrue="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6217" stopIfTrue="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6217" stopIfTrue="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6217" stopIfTrue="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6217" stopIfTrue="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6217" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="6218" stopIfTrue="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="6218" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6218" stopIfTrue="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="6218" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6218" stopIfTrue="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="6218" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="1981" stopIfTrue="1" operator="greaterThan">
@@ -31396,22 +31393,22 @@
     <cfRule type="cellIs" dxfId="7" priority="1804" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6217" stopIfTrue="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6217" stopIfTrue="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6217" stopIfTrue="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6217" stopIfTrue="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6217" stopIfTrue="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6217" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="6218" stopIfTrue="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="6218" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6218" stopIfTrue="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="6218" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6218" stopIfTrue="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="6218" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="1931" stopIfTrue="1" operator="greaterThan">
@@ -31638,22 +31635,22 @@
     <cfRule type="cellIs" dxfId="7" priority="1806" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6217" stopIfTrue="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6217" stopIfTrue="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6217" stopIfTrue="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6217" stopIfTrue="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6217" stopIfTrue="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6217" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="6218" stopIfTrue="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="6218" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6218" stopIfTrue="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="6218" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6218" stopIfTrue="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="6218" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="1933" stopIfTrue="1" operator="greaterThan">
@@ -33172,10 +33169,10 @@
     <cfRule type="cellIs" dxfId="7" priority="1808" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6217" stopIfTrue="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6217" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="6218" stopIfTrue="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="6218" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -33374,16 +33371,16 @@
     <cfRule type="cellIs" dxfId="7" priority="1816" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6217" stopIfTrue="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6217" stopIfTrue="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6217" stopIfTrue="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6217" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="6218" stopIfTrue="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="6218" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6218" stopIfTrue="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="6218" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -33493,13 +33490,13 @@
     <cfRule type="cellIs" dxfId="7" priority="1818" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6217" stopIfTrue="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6217" stopIfTrue="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6217" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="6218" stopIfTrue="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6218" stopIfTrue="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="6218" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -33588,10 +33585,10 @@
     <cfRule type="cellIs" dxfId="7" priority="1824" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6217" stopIfTrue="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6217" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="6218" stopIfTrue="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="6218" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -33683,7 +33680,7 @@
     <cfRule type="cellIs" dxfId="7" priority="1826" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6217" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="6218" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -33769,13 +33766,13 @@
     <cfRule type="cellIs" dxfId="7" priority="1832" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6217" stopIfTrue="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6217" stopIfTrue="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6217" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="6218" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6218" stopIfTrue="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="6218" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -33861,13 +33858,13 @@
     <cfRule type="cellIs" dxfId="7" priority="1834" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6217" stopIfTrue="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6217" stopIfTrue="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6217" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="6218" stopIfTrue="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="6218" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6218" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -33950,16 +33947,16 @@
     <cfRule type="cellIs" dxfId="7" priority="1840" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6217" stopIfTrue="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6217" stopIfTrue="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6217" stopIfTrue="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6217" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="6218" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="6218" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6218" stopIfTrue="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="6218" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -34039,19 +34036,19 @@
     <cfRule type="cellIs" dxfId="7" priority="1842" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6217" stopIfTrue="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6217" stopIfTrue="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6217" stopIfTrue="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6217" stopIfTrue="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6217" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="6218" stopIfTrue="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="6218" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6218" stopIfTrue="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="6218" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6218" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -34692,10 +34689,10 @@
     <cfRule type="cellIs" dxfId="7" priority="1876" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6217" stopIfTrue="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6217" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="6218" stopIfTrue="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6218" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -34787,7 +34784,7 @@
     <cfRule type="cellIs" dxfId="7" priority="1878" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6217" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="6218" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -34855,28 +34852,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
+        <v>416</v>
+      </c>
+      <c r="B1" t="s">
         <v>417</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>418</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>419</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>420</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>421</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>422</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>423</v>
-      </c>
-      <c r="H1" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -34887,13 +34884,13 @@
         <v>20191011</v>
       </c>
       <c r="C2" t="s">
+        <v>424</v>
+      </c>
+      <c r="D2" t="s">
         <v>425</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>426</v>
-      </c>
-      <c r="E2" t="s">
-        <v>427</v>
       </c>
       <c r="F2">
         <v>8</v>
@@ -34902,7 +34899,7 @@
         <v>70</v>
       </c>
       <c r="H2" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -34913,13 +34910,13 @@
         <v>20191211</v>
       </c>
       <c r="C3" t="s">
+        <v>428</v>
+      </c>
+      <c r="D3" t="s">
         <v>429</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>430</v>
-      </c>
-      <c r="E3" t="s">
-        <v>431</v>
       </c>
       <c r="F3">
         <v>3</v>
@@ -34928,111 +34925,111 @@
         <v>70</v>
       </c>
       <c r="H3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B4" t="s">
         <v>166</v>
       </c>
       <c r="C4" t="s">
+        <v>433</v>
+      </c>
+      <c r="D4" t="s">
         <v>434</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>435</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>436</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>437</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>438</v>
-      </c>
-      <c r="H4" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B5" t="s">
+        <v>439</v>
+      </c>
+      <c r="C5" t="s">
         <v>440</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>441</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
+        <v>430</v>
+      </c>
+      <c r="F5" t="s">
         <v>442</v>
       </c>
-      <c r="E5" t="s">
-        <v>431</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>443</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>444</v>
-      </c>
-      <c r="H5" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
+        <v>445</v>
+      </c>
+      <c r="B6" t="s">
         <v>446</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6" t="s">
+        <v>70</v>
+      </c>
+      <c r="G6" t="s">
+        <v>70</v>
+      </c>
+      <c r="H6" t="s">
         <v>447</v>
-      </c>
-      <c r="C6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D6" t="s">
-        <v>70</v>
-      </c>
-      <c r="E6" t="s">
-        <v>70</v>
-      </c>
-      <c r="F6" t="s">
-        <v>70</v>
-      </c>
-      <c r="G6" t="s">
-        <v>70</v>
-      </c>
-      <c r="H6" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="7" ht="201.6" customHeight="1" spans="1:8">
       <c r="A7" t="s">
+        <v>448</v>
+      </c>
+      <c r="B7" t="s">
         <v>449</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>450</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>451</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
+        <v>430</v>
+      </c>
+      <c r="F7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G7" t="s">
+        <v>70</v>
+      </c>
+      <c r="H7" s="9" t="s">
         <v>452</v>
-      </c>
-      <c r="E7" t="s">
-        <v>431</v>
-      </c>
-      <c r="F7" t="s">
-        <v>70</v>
-      </c>
-      <c r="G7" t="s">
-        <v>70</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="8" ht="43.2" customHeight="1" spans="1:8">
@@ -35043,13 +35040,13 @@
         <v>20191222</v>
       </c>
       <c r="C8" t="s">
+        <v>450</v>
+      </c>
+      <c r="D8" t="s">
         <v>451</v>
       </c>
-      <c r="D8" t="s">
-        <v>452</v>
-      </c>
       <c r="E8" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F8" t="s">
         <v>70</v>
@@ -35058,137 +35055,137 @@
         <v>70</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B9" t="s">
+        <v>454</v>
+      </c>
+      <c r="C9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" t="s">
+        <v>70</v>
+      </c>
+      <c r="G9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H9" t="s">
         <v>455</v>
-      </c>
-      <c r="C9" t="s">
-        <v>70</v>
-      </c>
-      <c r="D9" t="s">
-        <v>70</v>
-      </c>
-      <c r="E9" t="s">
-        <v>70</v>
-      </c>
-      <c r="F9" t="s">
-        <v>70</v>
-      </c>
-      <c r="G9" t="s">
-        <v>70</v>
-      </c>
-      <c r="H9" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
+        <v>456</v>
+      </c>
+      <c r="B10" t="s">
         <v>457</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F10" t="s">
+        <v>70</v>
+      </c>
+      <c r="G10" t="s">
+        <v>70</v>
+      </c>
+      <c r="H10" t="s">
         <v>458</v>
-      </c>
-      <c r="C10" t="s">
-        <v>70</v>
-      </c>
-      <c r="D10" t="s">
-        <v>70</v>
-      </c>
-      <c r="E10" t="s">
-        <v>70</v>
-      </c>
-      <c r="F10" t="s">
-        <v>70</v>
-      </c>
-      <c r="G10" t="s">
-        <v>70</v>
-      </c>
-      <c r="H10" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
+        <v>459</v>
+      </c>
+      <c r="B11" t="s">
+        <v>401</v>
+      </c>
+      <c r="C11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" t="s">
+        <v>70</v>
+      </c>
+      <c r="H11" t="s">
         <v>460</v>
-      </c>
-      <c r="B11" t="s">
-        <v>402</v>
-      </c>
-      <c r="C11" t="s">
-        <v>70</v>
-      </c>
-      <c r="D11" t="s">
-        <v>70</v>
-      </c>
-      <c r="E11" t="s">
-        <v>70</v>
-      </c>
-      <c r="F11" t="s">
-        <v>70</v>
-      </c>
-      <c r="G11" t="s">
-        <v>70</v>
-      </c>
-      <c r="H11" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
+        <v>461</v>
+      </c>
+      <c r="B12" t="s">
         <v>462</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12" t="s">
+        <v>70</v>
+      </c>
+      <c r="G12" t="s">
+        <v>70</v>
+      </c>
+      <c r="H12" t="s">
         <v>463</v>
-      </c>
-      <c r="C12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E12" t="s">
-        <v>70</v>
-      </c>
-      <c r="F12" t="s">
-        <v>70</v>
-      </c>
-      <c r="G12" t="s">
-        <v>70</v>
-      </c>
-      <c r="H12" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
+        <v>464</v>
+      </c>
+      <c r="B13" t="s">
+        <v>462</v>
+      </c>
+      <c r="C13" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" t="s">
+        <v>70</v>
+      </c>
+      <c r="E13" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" t="s">
+        <v>70</v>
+      </c>
+      <c r="G13" t="s">
+        <v>70</v>
+      </c>
+      <c r="H13" t="s">
         <v>465</v>
-      </c>
-      <c r="B13" t="s">
-        <v>463</v>
-      </c>
-      <c r="C13" t="s">
-        <v>70</v>
-      </c>
-      <c r="D13" t="s">
-        <v>70</v>
-      </c>
-      <c r="E13" t="s">
-        <v>70</v>
-      </c>
-      <c r="F13" t="s">
-        <v>70</v>
-      </c>
-      <c r="G13" t="s">
-        <v>70</v>
-      </c>
-      <c r="H13" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -35214,7 +35211,7 @@
         <v>70</v>
       </c>
       <c r="H14" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
   </sheetData>
@@ -35242,110 +35239,110 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="2" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2"/>
       <c r="B2" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="3" spans="2:2">
       <c r="B3" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="4" spans="2:2">
       <c r="B4" s="3" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="C11" t="s">
         <v>474</v>
-      </c>
-      <c r="C11" t="s">
-        <v>475</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="13" spans="2:2">
       <c r="B13" s="3" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="14" spans="2:2">
       <c r="B14" s="3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="15" spans="2:2">
       <c r="B15" s="3" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B16" s="3"/>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="20" spans="2:2">
       <c r="B20" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="23" spans="2:2">
       <c r="B23" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="24" spans="2:13">
       <c r="B24" s="4" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C24" s="4"/>
       <c r="F24" s="4" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G24" s="5"/>
       <c r="J24" s="4" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
@@ -35353,7 +35350,7 @@
     </row>
     <row r="25" spans="2:13">
       <c r="B25" s="6" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C25" s="7"/>
       <c r="F25" s="4"/>
@@ -35362,12 +35359,12 @@
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
       <c r="M25" s="5" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="26" spans="2:14">
       <c r="B26" s="6" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>1</v>
@@ -35376,106 +35373,106 @@
         <v>370</v>
       </c>
       <c r="G26" s="6" t="s">
+        <v>490</v>
+      </c>
+      <c r="H26" s="6" t="s">
         <v>491</v>
       </c>
-      <c r="H26" s="6" t="s">
+      <c r="J26" s="8" t="s">
         <v>492</v>
       </c>
-      <c r="J26" s="8" t="s">
+      <c r="K26" s="8" t="s">
         <v>493</v>
-      </c>
-      <c r="K26" s="8" t="s">
-        <v>494</v>
       </c>
       <c r="L26" s="8"/>
       <c r="M26" s="6" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="N26" s="6"/>
     </row>
     <row r="27" spans="2:14">
       <c r="B27" s="6" t="s">
+        <v>495</v>
+      </c>
+      <c r="C27" s="6" t="s">
         <v>496</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>497</v>
       </c>
       <c r="F27" s="8"/>
       <c r="G27" s="6" t="s">
+        <v>497</v>
+      </c>
+      <c r="H27" s="6" t="s">
         <v>498</v>
       </c>
-      <c r="H27" s="6" t="s">
+      <c r="J27" s="8" t="s">
         <v>499</v>
       </c>
-      <c r="J27" s="8" t="s">
+      <c r="K27" s="8" t="s">
         <v>500</v>
-      </c>
-      <c r="K27" s="8" t="s">
-        <v>501</v>
       </c>
       <c r="L27" s="8"/>
       <c r="M27" s="6" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="N27" s="6" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="28" spans="2:13">
       <c r="B28" s="6" t="s">
+        <v>502</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>500</v>
+      </c>
+      <c r="M28" t="s">
         <v>503</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>501</v>
-      </c>
-      <c r="M28" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="29" spans="2:13">
       <c r="B29" s="6" t="s">
+        <v>504</v>
+      </c>
+      <c r="C29" s="6" t="s">
         <v>505</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="M29" t="s">
         <v>506</v>
-      </c>
-      <c r="M29" t="s">
-        <v>507</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="34" spans="2:2">
       <c r="B34" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="35" spans="2:2">
       <c r="B35" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="36" spans="2:2">
       <c r="B36" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="37" spans="2:2">
       <c r="B37" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change excel history trend from unit worth to ac worth.
</commit_message>
<xml_diff>
--- a/fund/Jelly_model.xlsx
+++ b/fund/Jelly_model.xlsx
@@ -1742,7 +1742,7 @@
       </c>
       <c r="D2" s="0" t="inlineStr">
         <is>
-          <t>1.9786, 1.9708, 1.9662, 2.0156, 2.016, 2.0069, 1.9292, 1.8758, 1.9094, 1.9462, 1.9415, 1.9334, 1.9657, 2.0333, 2.0368, 2.0594, 2.0833, 2.1021, 2.1619, 2.1357, 2.1591, 2.1756, 2.2221, 2.2334, 2.2205, 2.2061, 2.1742, 2.1436, 2.1972, 2.2256, 2.2204, 2.1711, 2.1752, 2.1792, 2.2168, 2.203, 2.2107, 2.2143, 2.1871, 2.2483, 2.2799, 2.3195, 2.2982, 2.3311, 2.351, 2.3749, 2.4625, 2.44, 2.4958, 2.4445, 2.2939, 2.393, 2.4071, 2.4697, 2.5209, 2.5221, 2.5459, 2.5921, 2.6019, 2.6219</t>
+          <t>1.9662, 2.0156, 2.016, 2.0069, 1.9292, 1.8758, 1.9094, 1.9462, 1.9415, 1.9334, 1.9657, 2.0333, 2.0368, 2.0594, 2.0833, 2.1021, 2.1619, 2.1357, 2.1591, 2.1756, 2.2221, 2.2334, 2.2205, 2.2061, 2.1742, 2.1436, 2.1972, 2.2256, 2.2204, 2.1711, 2.1752, 2.1792, 2.2168, 2.203, 2.2107, 2.2143, 2.1871, 2.2483, 2.2799, 2.3195, 2.2982, 2.3311, 2.351, 2.3749, 2.4625, 2.44, 2.4958, 2.4445, 2.2939, 2.393, 2.4071, 2.4697, 2.5209, 2.5221, 2.5459, 2.5921, 2.6019, 2.6219, 2.6931, 2.7566</t>
         </is>
       </c>
       <c r="E2" s="24" t="inlineStr">
@@ -1759,23 +1759,23 @@
         <v>15</v>
       </c>
       <c r="I2" s="74" t="n">
-        <v>2.6219</v>
+        <v>2.7566</v>
       </c>
       <c r="J2" s="75" t="n">
-        <v>0.7686690495407209</v>
+        <v>2.357877538895709</v>
       </c>
       <c r="K2" s="76" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="L2" s="76" t="n">
-        <v>14.2987924495401</v>
+        <v>20.17088800732379</v>
       </c>
       <c r="M2" s="76" t="n">
-        <v>2.6219</v>
+        <v>2.7566</v>
       </c>
       <c r="N2" s="77" t="inlineStr">
         <is>
-          <t>2020-02-14</t>
+          <t>2020-02-18</t>
         </is>
       </c>
       <c r="O2" s="30">
@@ -1892,30 +1892,30 @@
       </c>
       <c r="D3" s="0" t="inlineStr">
         <is>
-          <t>1.146, 1.149, 1.133, 1.15, 1.135, 1.138, 1.099, 1.063, 1.086, 1.123, 1.121, 1.116, 1.145, 1.189, 1.195, 1.208, 1.239, 1.251, 1.284, 1.277, 1.29, 1.291, 1.312, 1.314, 1.326, 1.282, 1.264, 1.226, 1.265, 1.311, 1.288, 1.244, 1.244, 1.243, 1.275, 1.253, 1.249, 1.244, 1.235, 1.278, 1.313, 1.387, 1.354, 1.375, 1.376, 1.373, 1.43, 1.441, 1.487, 1.439, 1.317, 1.392, 1.393, 1.426, 1.471, 1.429, 1.457, 1.498, 1.548, 1.537</t>
+          <t>1.133, 1.15, 1.135, 1.138, 1.099, 1.063, 1.086, 1.123, 1.121, 1.116, 1.145, 1.189, 1.195, 1.208, 1.239, 1.251, 1.284, 1.277, 1.29, 1.291, 1.312, 1.314, 1.326, 1.282, 1.264, 1.226, 1.265, 1.311, 1.288, 1.244, 1.244, 1.243, 1.275, 1.253, 1.249, 1.244, 1.235, 1.278, 1.313, 1.387, 1.354, 1.375, 1.376, 1.373, 1.43, 1.441, 1.487, 1.439, 1.317, 1.392, 1.393, 1.426, 1.471, 1.429, 1.457, 1.498, 1.548, 1.537, 1.572, 1.627</t>
         </is>
       </c>
       <c r="H3" s="3" t="n">
         <v>15</v>
       </c>
       <c r="I3" s="74" t="n">
-        <v>1.537</v>
+        <v>1.627</v>
       </c>
       <c r="J3" s="75" t="n">
-        <v>-0.7105943152454859</v>
+        <v>3.498727735368953</v>
       </c>
       <c r="K3" s="76" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L3" s="76" t="n">
-        <v>-0.5519317611640804</v>
+        <v>4.540867810292638</v>
       </c>
       <c r="M3" s="76" t="n">
-        <v>1.982</v>
+        <v>2.072</v>
       </c>
       <c r="N3" s="77" t="inlineStr">
         <is>
-          <t>2020-02-14</t>
+          <t>2020-02-18</t>
         </is>
       </c>
       <c r="O3" s="30">
@@ -2034,30 +2034,30 @@
       </c>
       <c r="D4" s="0" t="inlineStr">
         <is>
-          <t>3.7299, 3.6813, 3.6526, 3.698, 3.6566, 3.6777, 3.5981, 3.4791, 3.5305, 3.6562, 3.6666, 3.6823, 3.7375, 3.7957, 3.8074, 3.8782, 3.9198, 3.927, 4.0568, 4.0206, 4.0601, 4.1019, 4.2549, 4.2962, 4.2832, 4.1795, 4.1366, 3.9861, 4.097, 4.1918, 4.1732, 4.0528, 4.0374, 4.0288, 4.2087, 4.2386, 4.2866, 4.2851, 4.174, 4.2587, 4.3341, 4.4817, 4.5077, 4.5983, 4.6206, 4.6398, 4.8649, 4.8899, 5.1199, 5.0136, 4.6553, 4.8895, 4.9414, 5.0837, 5.2218, 5.1426, 5.2235, 5.3354, 5.3753, 5.4243</t>
+          <t>3.6526, 3.698, 3.6566, 3.6777, 3.5981, 3.4791, 3.5305, 3.6562, 3.6666, 3.6823, 3.7375, 3.7957, 3.8074, 3.8782, 3.9198, 3.927, 4.0568, 4.0206, 4.0601, 4.1019, 4.2549, 4.2962, 4.2832, 4.1795, 4.1366, 3.9861, 4.097, 4.1918, 4.1732, 4.0528, 4.0374, 4.0288, 4.2087, 4.2386, 4.2866, 4.2851, 4.174, 4.2587, 4.3341, 4.4817, 4.5077, 4.5983, 4.6206, 4.6398, 4.8649, 4.8899, 5.1199, 5.0136, 4.6553, 4.8895, 4.9414, 5.0837, 5.2218, 5.1426, 5.2235, 5.3354, 5.3753, 5.4243, 5.6002, 5.8071</t>
         </is>
       </c>
       <c r="H4" s="3" t="n">
         <v>5</v>
       </c>
       <c r="I4" s="74" t="n">
-        <v>5.4243</v>
+        <v>5.8071</v>
       </c>
       <c r="J4" s="75" t="n">
-        <v>0.9115770282588783</v>
+        <v>3.694510910324632</v>
       </c>
       <c r="K4" s="76" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L4" s="76" t="n">
-        <v>5.477773888694432</v>
+        <v>12.9214794073037</v>
       </c>
       <c r="M4" s="76" t="n">
-        <v>5.4243</v>
+        <v>5.8071</v>
       </c>
       <c r="N4" s="77" t="inlineStr">
         <is>
-          <t>2020-02-14</t>
+          <t>2020-02-18</t>
         </is>
       </c>
       <c r="O4" s="30">
@@ -2178,30 +2178,30 @@
       </c>
       <c r="D5" s="0" t="inlineStr">
         <is>
-          <t>1.4115, 1.405, 1.4044, 1.4379, 1.4363, 1.4366, 1.3776, 1.3389, 1.3573, 1.3817, 1.3824, 1.3756, 1.3968, 1.4373, 1.4445, 1.4642, 1.489, 1.5025, 1.551, 1.531, 1.5467, 1.5604, 1.5956, 1.6014, 1.5942, 1.5793, 1.5578, 1.5335, 1.5722, 1.5956, 1.5907, 1.5523, 1.5573, 1.5628, 1.592, 1.5822, 1.5893, 1.5914, 1.5712, 1.6147, 1.6356, 1.669, 1.6556, 1.6782, 1.6928, 1.7128, 1.7753, 1.758, 1.7993, 1.7584, 1.6472, 1.7278, 1.7458, 1.7983, 1.8437, 1.8405, 1.8513, 1.89, 1.8988, 1.9184</t>
+          <t>1.4044, 1.4379, 1.4363, 1.4366, 1.3776, 1.3389, 1.3573, 1.3817, 1.3824, 1.3756, 1.3968, 1.4373, 1.4445, 1.4642, 1.489, 1.5025, 1.551, 1.531, 1.5467, 1.5604, 1.5956, 1.6014, 1.5942, 1.5793, 1.5578, 1.5335, 1.5722, 1.5956, 1.5907, 1.5523, 1.5573, 1.5628, 1.592, 1.5822, 1.5893, 1.5914, 1.5712, 1.6147, 1.6356, 1.669, 1.6556, 1.6782, 1.6928, 1.7128, 1.7753, 1.758, 1.7993, 1.7584, 1.6472, 1.7278, 1.7458, 1.7983, 1.8437, 1.8405, 1.8513, 1.89, 1.8988, 1.9184, 1.9754, 2.035</t>
         </is>
       </c>
       <c r="H5" s="3" t="n">
         <v>5</v>
       </c>
       <c r="I5" s="74" t="n">
-        <v>1.9184</v>
+        <v>2.035</v>
       </c>
       <c r="J5" s="75" t="n">
-        <v>1.032230882662738</v>
+        <v>3.017110458641293</v>
       </c>
       <c r="K5" s="76" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L5" s="76" t="n">
-        <v>4.232545503939152</v>
+        <v>10.56778049443087</v>
       </c>
       <c r="M5" s="76" t="n">
-        <v>1.9184</v>
+        <v>2.035</v>
       </c>
       <c r="N5" s="77" t="inlineStr">
         <is>
-          <t>2020-02-14</t>
+          <t>2020-02-18</t>
         </is>
       </c>
       <c r="O5" s="30">
@@ -2320,7 +2320,7 @@
       </c>
       <c r="D6" s="0" t="inlineStr">
         <is>
-          <t>2.145, 2.094, 2.101, 2.144, 2.118, 2.103, 2.041, 2.003, 2.043, 2.041, 2.05, 2.036, 2.068, 2.084, 2.078, 2.103, 2.131, 2.148, 2.152, 2.112, 2.133, 2.136, 2.184, 2.229, 2.219, 2.202, 2.196, 2.116, 2.155, 2.198, 2.203, 2.164, 2.171, 2.196, 2.251, 2.243, 2.262, 2.317, 2.289, 2.321, 2.305, 2.363, 2.358, 2.357, 2.343, 2.361, 2.407, 2.373, 2.395, 2.273, 2.087, 2.157, 2.222, 2.295, 2.372, 2.383, 2.362, 2.422, 2.42, 2.44</t>
+          <t>2.101, 2.144, 2.118, 2.103, 2.041, 2.003, 2.043, 2.041, 2.05, 2.036, 2.068, 2.084, 2.078, 2.103, 2.131, 2.148, 2.152, 2.112, 2.133, 2.136, 2.184, 2.229, 2.219, 2.202, 2.196, 2.116, 2.155, 2.198, 2.203, 2.164, 2.171, 2.196, 2.251, 2.243, 2.262, 2.317, 2.289, 2.321, 2.305, 2.363, 2.358, 2.357, 2.343, 2.361, 2.407, 2.373, 2.395, 2.273, 2.087, 2.157, 2.222, 2.295, 2.372, 2.383, 2.362, 2.422, 2.42, 2.44, 2.522, 2.568</t>
         </is>
       </c>
       <c r="E6" s="0" t="inlineStr">
@@ -2332,23 +2332,23 @@
         <v>15</v>
       </c>
       <c r="I6" s="74" t="n">
-        <v>2.44</v>
+        <v>2.568</v>
       </c>
       <c r="J6" s="75" t="n">
-        <v>0.8264462809917362</v>
+        <v>1.82394924662967</v>
       </c>
       <c r="K6" s="76" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L6" s="76" t="n">
-        <v>0.8257279443719984</v>
+        <v>6.127770534550195</v>
       </c>
       <c r="M6" s="76" t="n">
-        <v>2.32</v>
+        <v>2.442</v>
       </c>
       <c r="N6" s="77" t="inlineStr">
         <is>
-          <t>2020-02-14</t>
+          <t>2020-02-18</t>
         </is>
       </c>
       <c r="O6" s="30">
@@ -2472,7 +2472,7 @@
       </c>
       <c r="D7" s="0" t="inlineStr">
         <is>
-          <t>1.1876, 1.177, 1.1841, 1.2157, 1.2194, 1.1982, 1.1561, 1.1391, 1.1423, 1.1292, 1.1279, 1.1065, 1.0957, 1.0971, 1.1028, 1.1169, 1.1227, 1.104, 1.1201, 1.1185, 1.1135, 1.1062, 1.119, 1.1277, 1.1111, 1.109, 1.0965, 1.0857, 1.0896, 1.0891, 1.0908, 1.0768, 1.0815, 1.1022, 1.1038, 1.0981, 1.0917, 1.1144, 1.1055, 1.1465, 1.1473, 1.1566, 1.1466, 1.1548, 1.169, 1.1797, 1.1911, 1.2034, 1.1944, 1.1711, 1.136, 1.1782, 1.2051, 1.2481, 1.2379, 1.2328, 1.2365, 1.2609, 1.2546, 1.2483</t>
+          <t>1.1841, 1.2157, 1.2194, 1.1982, 1.1561, 1.1391, 1.1423, 1.1292, 1.1279, 1.1065, 1.0957, 1.0971, 1.1028, 1.1169, 1.1227, 1.104, 1.1201, 1.1185, 1.1135, 1.1062, 1.119, 1.1277, 1.1111, 1.109, 1.0965, 1.0857, 1.0896, 1.0891, 1.0908, 1.0768, 1.0815, 1.1022, 1.1038, 1.0981, 1.0917, 1.1144, 1.1055, 1.1465, 1.1473, 1.1566, 1.1466, 1.1548, 1.169, 1.1797, 1.1911, 1.2034, 1.1944, 1.1711, 1.136, 1.1782, 1.2051, 1.2481, 1.2379, 1.2328, 1.2365, 1.2609, 1.2546, 1.2483, 1.2871, 1.2944</t>
         </is>
       </c>
       <c r="E7" s="26" t="inlineStr">
@@ -2489,23 +2489,23 @@
         <v>5</v>
       </c>
       <c r="I7" s="74" t="n">
-        <v>1.2483</v>
+        <v>1.2944</v>
       </c>
       <c r="J7" s="75" t="n">
-        <v>-0.5021520803443307</v>
+        <v>0.5671664983295848</v>
       </c>
       <c r="K7" s="76" t="n">
         <v>2</v>
       </c>
       <c r="L7" s="76" t="n">
-        <v>-1.000188714851874</v>
+        <v>3.698055661456364</v>
       </c>
       <c r="M7" s="76" t="n">
-        <v>0.5246</v>
+        <v>0.544</v>
       </c>
       <c r="N7" s="77" t="inlineStr">
         <is>
-          <t>2020-02-14</t>
+          <t>2020-02-18</t>
         </is>
       </c>
       <c r="O7" s="30">
@@ -2626,7 +2626,7 @@
       </c>
       <c r="D8" s="0" t="inlineStr">
         <is>
-          <t>1.6873, 1.6728, 1.671, 1.7046, 1.7004, 1.6698, 1.6047, 1.5899, 1.6046, 1.5896, 1.5956, 1.5578, 1.5421, 1.5451, 1.5607, 1.581, 1.594, 1.5636, 1.5832, 1.5825, 1.5853, 1.6122, 1.6105, 1.6167, 1.5937, 1.5863, 1.5692, 1.5659, 1.5675, 1.5697, 1.5777, 1.5704, 1.5775, 1.5971, 1.5973, 1.5803, 1.5686, 1.5998, 1.5972, 1.6535, 1.6539, 1.6725, 1.6581, 1.6817, 1.7073, 1.7254, 1.7513, 1.7561, 1.7484, 1.7006, 1.6286, 1.6837, 1.7158, 1.775, 1.7592, 1.7599, 1.7748, 1.7989, 1.7838, 1.7891</t>
+          <t>1.671, 1.7046, 1.7004, 1.6698, 1.6047, 1.5899, 1.6046, 1.5896, 1.5956, 1.5578, 1.5421, 1.5451, 1.5607, 1.581, 1.594, 1.5636, 1.5832, 1.5825, 1.5853, 1.6122, 1.6105, 1.6167, 1.5937, 1.5863, 1.5692, 1.5659, 1.5675, 1.5697, 1.5777, 1.5704, 1.5775, 1.5971, 1.5973, 1.5803, 1.5686, 1.5998, 1.5972, 1.6535, 1.6539, 1.6725, 1.6581, 1.6817, 1.7073, 1.7254, 1.7513, 1.7561, 1.7484, 1.7006, 1.6286, 1.6837, 1.7158, 1.775, 1.7592, 1.7599, 1.7748, 1.7989, 1.7838, 1.7891, 1.8337, 1.8309</t>
         </is>
       </c>
       <c r="E8" s="3" t="inlineStr">
@@ -2638,23 +2638,23 @@
         <v>5</v>
       </c>
       <c r="I8" s="74" t="n">
-        <v>1.7891</v>
+        <v>1.8309</v>
       </c>
       <c r="J8" s="75" t="n">
-        <v>0.2971185110438311</v>
+        <v>-0.152696733380604</v>
       </c>
       <c r="K8" s="76" t="n">
         <v>1</v>
       </c>
       <c r="L8" s="76" t="n">
-        <v>0.2971185110438311</v>
+        <v>-0.152696733380604</v>
       </c>
       <c r="M8" s="76" t="n">
-        <v>1.7891</v>
+        <v>1.8309</v>
       </c>
       <c r="N8" s="77" t="inlineStr">
         <is>
-          <t>2020-02-14</t>
+          <t>2020-02-18</t>
         </is>
       </c>
       <c r="O8" s="30">
@@ -2775,7 +2775,7 @@
       </c>
       <c r="D9" s="0" t="inlineStr">
         <is>
-          <t>1.241, 1.229, 1.214, 1.237, 1.221, 1.218, 1.182, 1.141, 1.145, 1.158, 1.17, 1.171, 1.181, 1.193, 1.186, 1.222, 1.249, 1.256, 1.27, 1.256, 1.263, 1.276, 1.311, 1.327, 1.318, 1.289, 1.272, 1.234, 1.259, 1.275, 1.272, 1.238, 1.238, 1.252, 1.3, 1.313, 1.324, 1.329, 1.293, 1.342, 1.364, 1.418, 1.405, 1.412, 1.41, 1.405, 1.467, 1.482, 1.536, 1.483, 1.363, 1.398, 1.411, 1.445, 1.47, 1.458, 1.491, 1.514, 1.518, 1.532</t>
+          <t>1.214, 1.237, 1.221, 1.218, 1.182, 1.141, 1.145, 1.158, 1.17, 1.171, 1.181, 1.193, 1.186, 1.222, 1.249, 1.256, 1.27, 1.256, 1.263, 1.276, 1.311, 1.327, 1.318, 1.289, 1.272, 1.234, 1.259, 1.275, 1.272, 1.238, 1.238, 1.252, 1.3, 1.313, 1.324, 1.329, 1.293, 1.342, 1.364, 1.418, 1.405, 1.412, 1.41, 1.405, 1.467, 1.482, 1.536, 1.483, 1.363, 1.398, 1.411, 1.445, 1.47, 1.458, 1.491, 1.514, 1.518, 1.532, 1.603, 1.622</t>
         </is>
       </c>
       <c r="E9" s="3" t="inlineStr">
@@ -2787,23 +2787,23 @@
         <v>4</v>
       </c>
       <c r="I9" s="74" t="n">
-        <v>1.532</v>
+        <v>1.622</v>
       </c>
       <c r="J9" s="75" t="n">
-        <v>0.9222661396574449</v>
+        <v>1.185277604491586</v>
       </c>
       <c r="K9" s="76" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L9" s="76" t="n">
-        <v>5.075445816186561</v>
+        <v>11.24828532235941</v>
       </c>
       <c r="M9" s="76" t="n">
-        <v>1.532</v>
+        <v>1.622</v>
       </c>
       <c r="N9" s="77" t="inlineStr">
         <is>
-          <t>2020-02-14</t>
+          <t>2020-02-18</t>
         </is>
       </c>
       <c r="O9" s="30">
@@ -2924,7 +2924,7 @@
       </c>
       <c r="D10" s="0" t="inlineStr">
         <is>
-          <t>1.4678, 1.4657, 1.4648, 1.5032, 1.4891, 1.4887, 1.4683, 1.4495, 1.4588, 1.4811, 1.4775, 1.4791, 1.4871, 1.4975, 1.5055, 1.518, 1.5225, 1.5257, 1.5338, 1.5191, 1.5153, 1.5364, 1.5617, 1.5784, 1.5779, 1.5782, 1.5614, 1.5454, 1.5875, 1.5954, 1.5974, 1.6028, 1.6091, 1.6206, 1.6645, 1.6935, 1.7343, 1.7419, 1.7236, 1.74, 1.7302, 1.7444, 1.7512, 1.7344, 1.7254, 1.7181, 1.7239, 1.711, 1.7341, 1.7011, 1.6122, 1.6534, 1.6935, 1.7373, 1.7429, 1.7719, 1.7808, 1.8377, 1.8261, 1.821</t>
+          <t>1.4648, 1.5032, 1.4891, 1.4887, 1.4683, 1.4495, 1.4588, 1.4811, 1.4775, 1.4791, 1.4871, 1.4975, 1.5055, 1.518, 1.5225, 1.5257, 1.5338, 1.5191, 1.5153, 1.5364, 1.5617, 1.5784, 1.5779, 1.5782, 1.5614, 1.5454, 1.5875, 1.5954, 1.5974, 1.6028, 1.6091, 1.6206, 1.6645, 1.6935, 1.7343, 1.7419, 1.7236, 1.74, 1.7302, 1.7444, 1.7512, 1.7344, 1.7254, 1.7181, 1.7239, 1.711, 1.7341, 1.7011, 1.6122, 1.6534, 1.6935, 1.7373, 1.7429, 1.7719, 1.7808, 1.8377, 1.8261, 1.821, 1.8763, 1.8836</t>
         </is>
       </c>
       <c r="E10" s="0" t="inlineStr">
@@ -2941,23 +2941,23 @@
         <v>3</v>
       </c>
       <c r="I10" s="74" t="n">
-        <v>1.821</v>
+        <v>1.8836</v>
       </c>
       <c r="J10" s="75" t="n">
-        <v>-0.27928371940201</v>
+        <v>0.3890635825827353</v>
       </c>
       <c r="K10" s="76" t="n">
         <v>2</v>
       </c>
       <c r="L10" s="76" t="n">
-        <v>-0.9087446264352145</v>
+        <v>3.43767160900604</v>
       </c>
       <c r="M10" s="76" t="n">
-        <v>1.821</v>
+        <v>1.8836</v>
       </c>
       <c r="N10" s="77" t="inlineStr">
         <is>
-          <t>2020-02-14</t>
+          <t>2020-02-18</t>
         </is>
       </c>
       <c r="O10" s="30">
@@ -3078,7 +3078,7 @@
       </c>
       <c r="D11" s="0" t="inlineStr">
         <is>
-          <t>1.0755, 1.0668, 1.0686, 1.0902, 1.0837, 1.0781, 1.0485, 1.0308, 1.0416, 1.0473, 1.0445, 1.0392, 1.0359, 1.0425, 1.0454, 1.065, 1.0728, 1.0665, 1.0808, 1.0744, 1.0731, 1.0914, 1.1116, 1.1268, 1.118, 1.1105, 1.0965, 1.0756, 1.0908, 1.0997, 1.1043, 1.0862, 1.0934, 1.1035, 1.1274, 1.1289, 1.138, 1.1435, 1.1326, 1.1605, 1.1671, 1.1945, 1.1888, 1.205, 1.2073, 1.2112, 1.2423, 1.2315, 1.2639, 1.2241, 1.1368, 1.1893, 1.2077, 1.2392, 1.2451, 1.246, 1.2574, 1.2826, 1.2727, 1.2727</t>
+          <t>1.0686, 1.0902, 1.0837, 1.0781, 1.0485, 1.0308, 1.0416, 1.0473, 1.0445, 1.0392, 1.0359, 1.0425, 1.0454, 1.065, 1.0728, 1.0665, 1.0808, 1.0744, 1.0731, 1.0914, 1.1116, 1.1268, 1.118, 1.1105, 1.0965, 1.0756, 1.0908, 1.0997, 1.1043, 1.0862, 1.0934, 1.1035, 1.1274, 1.1289, 1.138, 1.1435, 1.1326, 1.1605, 1.1671, 1.1945, 1.1888, 1.205, 1.2073, 1.2112, 1.2423, 1.2315, 1.2639, 1.2241, 1.1368, 1.1893, 1.2077, 1.2392, 1.2451, 1.246, 1.2574, 1.2826, 1.2727, 1.2727, 1.3147, 1.3253</t>
         </is>
       </c>
       <c r="E11" s="3" t="inlineStr">
@@ -3090,23 +3090,23 @@
         <v>3</v>
       </c>
       <c r="I11" s="74" t="n">
-        <v>1.2727</v>
+        <v>1.3253</v>
       </c>
       <c r="J11" s="75" t="n">
-        <v>0</v>
+        <v>0.8062675895641547</v>
       </c>
       <c r="K11" s="76" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L11" s="76" t="n">
-        <v>-0.7718696397941697</v>
+        <v>4.132945705979413</v>
       </c>
       <c r="M11" s="76" t="n">
-        <v>1.2727</v>
+        <v>1.3253</v>
       </c>
       <c r="N11" s="77" t="inlineStr">
         <is>
-          <t>2020-02-14</t>
+          <t>2020-02-18</t>
         </is>
       </c>
       <c r="O11" s="30">
@@ -3227,7 +3227,7 @@
       </c>
       <c r="D12" s="0" t="inlineStr">
         <is>
-          <t>1.3447, 1.3323, 1.3367, 1.3667, 1.3602, 1.3542, 1.3271, 1.2906, 1.3009, 1.3192, 1.3209, 1.3088, 1.3308, 1.3357, 1.348, 1.3841, 1.4134, 1.424, 1.4583, 1.4436, 1.4503, 1.4564, 1.4935, 1.5217, 1.5246, 1.508, 1.4893, 1.46, 1.4888, 1.5075, 1.5104, 1.4884, 1.4913, 1.5001, 1.544, 1.548, 1.5676, 1.5706, 1.5458, 1.5876, 1.5872, 1.6302, 1.6253, 1.6337, 1.6499, 1.6498, 1.7044, 1.683, 1.746, 1.6898, 1.5591, 1.6529, 1.6792, 1.7465, 1.7851, 1.7588, 1.7617, 1.7887, 1.7807, 1.7561</t>
+          <t>1.3367, 1.3667, 1.3602, 1.3542, 1.3271, 1.2906, 1.3009, 1.3192, 1.3209, 1.3088, 1.3308, 1.3357, 1.348, 1.3841, 1.4134, 1.424, 1.4583, 1.4436, 1.4503, 1.4564, 1.4935, 1.5217, 1.5246, 1.508, 1.4893, 1.46, 1.4888, 1.5075, 1.5104, 1.4884, 1.4913, 1.5001, 1.544, 1.548, 1.5676, 1.5706, 1.5458, 1.5876, 1.5872, 1.6302, 1.6253, 1.6337, 1.6499, 1.6498, 1.7044, 1.683, 1.746, 1.6898, 1.5591, 1.6529, 1.6792, 1.7465, 1.7851, 1.7588, 1.7617, 1.7887, 1.7807, 1.7561, 1.8229, 1.8464</t>
         </is>
       </c>
       <c r="E12" s="3" t="inlineStr">
@@ -3239,23 +3239,23 @@
         <v>3</v>
       </c>
       <c r="I12" s="74" t="n">
-        <v>1.7561</v>
+        <v>1.8464</v>
       </c>
       <c r="J12" s="75" t="n">
-        <v>-1.381479193575558</v>
+        <v>1.289154643699604</v>
       </c>
       <c r="K12" s="76" t="n">
         <v>2</v>
       </c>
       <c r="L12" s="76" t="n">
-        <v>-1.822552691899143</v>
+        <v>5.142076191560848</v>
       </c>
       <c r="M12" s="76" t="n">
-        <v>1.7561</v>
+        <v>1.8464</v>
       </c>
       <c r="N12" s="77" t="inlineStr">
         <is>
-          <t>2020-02-14</t>
+          <t>2020-02-18</t>
         </is>
       </c>
       <c r="O12" s="30">
@@ -3376,30 +3376,30 @@
       </c>
       <c r="D13" s="0" t="inlineStr">
         <is>
-          <t>2.392, 2.38, 2.388, 2.425, 2.433, 2.402, 2.313, 2.291, 2.303, 2.29, 2.291, 2.248, 2.223, 2.222, 2.236, 2.258, 2.268, 2.23, 2.249, 2.245, 2.254, 2.298, 2.308, 2.321, 2.286, 2.278, 2.252, 2.235, 2.238, 2.232, 2.245, 2.233, 2.236, 2.281, 2.289, 2.288, 2.271, 2.307, 2.29, 2.349, 2.358, 2.378, 2.352, 2.373, 2.403, 2.425, 2.456, 2.474, 2.457, 2.389, 2.286, 2.36, 2.421, 2.498, 2.463, 2.474, 2.479, 2.518, 2.493, 2.508</t>
+          <t>2.388, 2.425, 2.433, 2.402, 2.313, 2.291, 2.303, 2.29, 2.291, 2.248, 2.223, 2.222, 2.236, 2.258, 2.268, 2.23, 2.249, 2.245, 2.254, 2.298, 2.308, 2.321, 2.286, 2.278, 2.252, 2.235, 2.238, 2.232, 2.245, 2.233, 2.236, 2.281, 2.289, 2.288, 2.271, 2.307, 2.29, 2.349, 2.358, 2.378, 2.352, 2.373, 2.403, 2.425, 2.456, 2.474, 2.457, 2.389, 2.286, 2.36, 2.421, 2.498, 2.463, 2.474, 2.479, 2.518, 2.493, 2.508, 2.574, 2.576</t>
         </is>
       </c>
       <c r="H13" s="3" t="n">
         <v>5</v>
       </c>
       <c r="I13" s="74" t="n">
-        <v>2.508</v>
+        <v>2.576</v>
       </c>
       <c r="J13" s="75" t="n">
-        <v>0.6016847172081879</v>
+        <v>0.0777000777000864</v>
       </c>
       <c r="K13" s="76" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L13" s="76" t="n">
-        <v>0.5699088145896535</v>
+        <v>3.153495440729473</v>
       </c>
       <c r="M13" s="76" t="n">
-        <v>2.647</v>
+        <v>2.715</v>
       </c>
       <c r="N13" s="77" t="inlineStr">
         <is>
-          <t>2020-02-14</t>
+          <t>2020-02-18</t>
         </is>
       </c>
       <c r="O13" s="30">
@@ -3518,7 +3518,7 @@
       </c>
       <c r="D14" s="0" t="inlineStr">
         <is>
-          <t>5.5334, 5.4922, 5.4984, 5.5653, 5.5537, 5.5118, 4.8745, 4.851, 4.8865, 4.8578, 4.8471, 4.7459, 4.7341, 4.7245, 4.748, 4.7673, 4.8305, 4.7867, 4.8021, 4.7974, 4.7769, 4.8731, 4.8619, 4.8923, 4.868, 4.8449, 4.8361, 4.8142, 4.8313, 4.7994, 4.8552, 4.8483, 4.9114, 4.9607, 4.9348, 4.8767, 4.7873, 4.8272, 4.8134, 4.9049, 4.9685, 5.0368, 4.9983, 5.0017, 5.0181, 5.0197, 5.0262, 4.9916, 4.975, 4.8404, 4.5302, 4.5848, 4.7141, 4.838, 4.824, 4.861, 4.9281, 4.9444, 4.917, 4.9622</t>
+          <t>5.4984, 5.5653, 5.5537, 5.5118, 4.8745, 4.851, 4.8865, 4.8578, 4.8471, 4.7459, 4.7341, 4.7245, 4.748, 4.7673, 4.8305, 4.7867, 4.8021, 4.7974, 4.7769, 4.8731, 4.8619, 4.8923, 4.868, 4.8449, 4.8361, 4.8142, 4.8313, 4.7994, 4.8552, 4.8483, 4.9114, 4.9607, 4.9348, 4.8767, 4.7873, 4.8272, 4.8134, 4.9049, 4.9685, 5.0368, 4.9983, 5.0017, 5.0181, 5.0197, 5.0262, 4.9916, 4.975, 4.8404, 4.5302, 4.5848, 4.7141, 4.838, 4.824, 4.861, 4.9281, 4.9444, 4.917, 4.9622, 4.9751, 4.9235</t>
         </is>
       </c>
       <c r="E14" s="3" t="inlineStr">
@@ -3530,23 +3530,23 @@
         <v>14</v>
       </c>
       <c r="I14" s="74" t="n">
-        <v>4.9622</v>
+        <v>4.9235</v>
       </c>
       <c r="J14" s="75" t="n">
-        <v>0.9192597112060271</v>
+        <v>-1.037165082108913</v>
       </c>
       <c r="K14" s="76" t="n">
         <v>1</v>
       </c>
       <c r="L14" s="76" t="n">
-        <v>0.7783709316342252</v>
+        <v>-0.8797803959011721</v>
       </c>
       <c r="M14" s="76" t="n">
-        <v>5.8522</v>
+        <v>5.8135</v>
       </c>
       <c r="N14" s="77" t="inlineStr">
         <is>
-          <t>2020-02-14</t>
+          <t>2020-02-18</t>
         </is>
       </c>
       <c r="O14" s="30">
@@ -3670,7 +3670,7 @@
       </c>
       <c r="D15" s="0" t="inlineStr">
         <is>
-          <t>1.0158, 1.0093, 1.0048, 1.0131, 1.0184, 1.0167, 0.9896, 0.9869, 0.9964, 0.9999, 0.9939, 0.9686, 0.9686, 0.9641, 0.9697, 0.9686, 0.9889, 0.9833, 0.9836, 0.9733, 0.9654, 0.9803, 0.9649, 0.9761, 0.9807, 0.9735, 0.9698, 0.9635, 0.9676, 0.9566, 0.9637, 0.9734, 1.0068, 1.0073, 0.9966, 0.9857, 0.9779, 0.988, 0.9896, 1.01, 1.0337, 1.0486, 1.0332, 1.0381, 1.04, 1.0401, 1.0295, 1.0006, 1.0043, 0.9675, 0.8865, 0.8809, 0.8926, 0.9014, 0.9091, 0.9112, 0.9324, 0.935, 0.928, 0.9257</t>
+          <t>1.0048, 1.0131, 1.0184, 1.0167, 0.9896, 0.9869, 0.9964, 0.9999, 0.9939, 0.9686, 0.9686, 0.9641, 0.9697, 0.9686, 0.9889, 0.9833, 0.9836, 0.9733, 0.9654, 0.9803, 0.9649, 0.9761, 0.9807, 0.9735, 0.9698, 0.9635, 0.9676, 0.9566, 0.9637, 0.9734, 1.0068, 1.0073, 0.9966, 0.9857, 0.9779, 0.988, 0.9896, 1.01, 1.0337, 1.0486, 1.0332, 1.0381, 1.04, 1.0401, 1.0295, 1.0006, 1.0043, 0.9675, 0.8865, 0.8809, 0.8926, 0.9014, 0.9091, 0.9112, 0.9324, 0.935, 0.928, 0.9257, 0.9331, 0.9283</t>
         </is>
       </c>
       <c r="E15" s="28" t="inlineStr">
@@ -3682,23 +3682,23 @@
         <v>3</v>
       </c>
       <c r="I15" s="74" t="n">
-        <v>0.9257</v>
+        <v>0.9283</v>
       </c>
       <c r="J15" s="75" t="n">
-        <v>-0.2478448275862155</v>
+        <v>-0.5144143178651834</v>
       </c>
       <c r="K15" s="76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L15" s="76" t="n">
-        <v>-0.4512153704332679</v>
+        <v>-0.2331002331002505</v>
       </c>
       <c r="M15" s="76" t="n">
-        <v>2.0518</v>
+        <v>2.0544</v>
       </c>
       <c r="N15" s="77" t="inlineStr">
         <is>
-          <t>2020-02-14</t>
+          <t>2020-02-18</t>
         </is>
       </c>
       <c r="O15" s="30">
@@ -3819,7 +3819,7 @@
       </c>
       <c r="D16" s="0" t="inlineStr">
         <is>
-          <t>1.878, 1.858, 1.862, 1.908, 1.91, 1.877, 1.787, 1.76, 1.773, 1.761, 1.772, 1.726, 1.707, 1.702, 1.718, 1.739, 1.754, 1.713, 1.732, 1.73, 1.726, 1.764, 1.765, 1.772, 1.739, 1.729, 1.712, 1.706, 1.711, 1.709, 1.715, 1.705, 1.706, 1.733, 1.727, 1.715, 1.699, 1.733, 1.727, 1.789, 1.798, 1.814, 1.794, 1.823, 1.853, 1.876, 1.915, 1.917, 1.919, 1.865, 1.774, 1.846, 1.87, 1.934, 1.912, 1.921, 1.935, 1.97, 1.953, 1.965</t>
+          <t>1.862, 1.908, 1.91, 1.877, 1.787, 1.76, 1.773, 1.761, 1.772, 1.726, 1.707, 1.702, 1.718, 1.739, 1.754, 1.713, 1.732, 1.73, 1.726, 1.764, 1.765, 1.772, 1.739, 1.729, 1.712, 1.706, 1.711, 1.709, 1.715, 1.705, 1.706, 1.733, 1.727, 1.715, 1.699, 1.733, 1.727, 1.789, 1.798, 1.814, 1.794, 1.823, 1.853, 1.876, 1.915, 1.917, 1.919, 1.865, 1.774, 1.846, 1.87, 1.934, 1.912, 1.921, 1.935, 1.97, 1.953, 1.965, 2.016, 2.007</t>
         </is>
       </c>
       <c r="E16" s="24" t="inlineStr">
@@ -3836,23 +3836,23 @@
         <v>15</v>
       </c>
       <c r="I16" s="74" t="n">
-        <v>1.965</v>
+        <v>2.007</v>
       </c>
       <c r="J16" s="75" t="n">
-        <v>0.614439324116744</v>
+        <v>-0.4464285714285663</v>
       </c>
       <c r="K16" s="76" t="n">
         <v>1</v>
       </c>
       <c r="L16" s="76" t="n">
-        <v>0.5917159763313614</v>
+        <v>-0.4304160688665873</v>
       </c>
       <c r="M16" s="76" t="n">
-        <v>2.04</v>
+        <v>2.082</v>
       </c>
       <c r="N16" s="77" t="inlineStr">
         <is>
-          <t>2020-02-14</t>
+          <t>2020-02-18</t>
         </is>
       </c>
       <c r="O16" s="30">
@@ -3973,7 +3973,7 @@
       </c>
       <c r="D17" s="0" t="inlineStr">
         <is>
-          <t>1.8341, 1.8157, 1.8188, 1.8605, 1.8682, 1.8275, 1.7434, 1.7228, 1.7321, 1.7125, 1.7214, 1.6762, 1.6551, 1.6533, 1.6719, 1.6955, 1.7107, 1.6733, 1.6936, 1.6934, 1.6944, 1.7286, 1.726, 1.7313, 1.6992, 1.6892, 1.671, 1.6652, 1.6706, 1.6734, 1.6803, 1.67, 1.6783, 1.7051, 1.7031, 1.6944, 1.6826, 1.7221, 1.7157, 1.7829, 1.7836, 1.8001, 1.7809, 1.8068, 1.8401, 1.8616, 1.888, 1.8958, 1.8887, 1.8384, 1.7604, 1.8216, 1.8625, 1.921, 1.9091, 1.9107, 1.9362, 1.9697, 1.9542, 1.9526</t>
+          <t>1.8188, 1.8605, 1.8682, 1.8275, 1.7434, 1.7228, 1.7321, 1.7125, 1.7214, 1.6762, 1.6551, 1.6533, 1.6719, 1.6955, 1.7107, 1.6733, 1.6936, 1.6934, 1.6944, 1.7286, 1.726, 1.7313, 1.6992, 1.6892, 1.671, 1.6652, 1.6706, 1.6734, 1.6803, 1.67, 1.6783, 1.7051, 1.7031, 1.6944, 1.6826, 1.7221, 1.7157, 1.7829, 1.7836, 1.8001, 1.7809, 1.8068, 1.8401, 1.8616, 1.888, 1.8958, 1.8887, 1.8384, 1.7604, 1.8216, 1.8625, 1.921, 1.9091, 1.9107, 1.9362, 1.9697, 1.9542, 1.9526, 1.9972, 1.9988</t>
         </is>
       </c>
       <c r="E17" s="3" t="inlineStr">
@@ -3990,23 +3990,23 @@
         <v>5</v>
       </c>
       <c r="I17" s="74" t="n">
-        <v>1.9526</v>
+        <v>1.9988</v>
       </c>
       <c r="J17" s="75" t="n">
-        <v>-0.08187493603520858</v>
+        <v>0.08011215701981894</v>
       </c>
       <c r="K17" s="76" t="n">
         <v>2</v>
       </c>
       <c r="L17" s="76" t="n">
-        <v>-0.8681525105346051</v>
+        <v>2.366076001229132</v>
       </c>
       <c r="M17" s="76" t="n">
-        <v>1.9526</v>
+        <v>1.9988</v>
       </c>
       <c r="N17" s="77" t="inlineStr">
         <is>
-          <t>2020-02-14</t>
+          <t>2020-02-18</t>
         </is>
       </c>
       <c r="O17" s="30">
@@ -4127,7 +4127,7 @@
       </c>
       <c r="D18" s="0" t="inlineStr">
         <is>
-          <t>1.6737, 1.6646, 1.665, 1.7066, 1.7058, 1.6791, 1.5942, 1.577, 1.6024, 1.5964, 1.6024, 1.5521, 1.5316, 1.5392, 1.5577, 1.582, 1.5959, 1.561, 1.5798, 1.5718, 1.5727, 1.6094, 1.6056, 1.6183, 1.5962, 1.5828, 1.563, 1.5493, 1.5532, 1.5582, 1.5611, 1.5432, 1.5446, 1.5693, 1.5706, 1.5547, 1.5403, 1.566, 1.5558, 1.6241, 1.6349, 1.6584, 1.6409, 1.6638, 1.6859, 1.7106, 1.738, 1.7398, 1.7496, 1.7044, 1.6276, 1.6889, 1.7306, 1.7809, 1.7523, 1.7603, 1.7693, 1.7924, 1.7771, 1.7835</t>
+          <t>1.665, 1.7066, 1.7058, 1.6791, 1.5942, 1.577, 1.6024, 1.5964, 1.6024, 1.5521, 1.5316, 1.5392, 1.5577, 1.582, 1.5959, 1.561, 1.5798, 1.5718, 1.5727, 1.6094, 1.6056, 1.6183, 1.5962, 1.5828, 1.563, 1.5493, 1.5532, 1.5582, 1.5611, 1.5432, 1.5446, 1.5693, 1.5706, 1.5547, 1.5403, 1.566, 1.5558, 1.6241, 1.6349, 1.6584, 1.6409, 1.6638, 1.6859, 1.7106, 1.738, 1.7398, 1.7496, 1.7044, 1.6276, 1.6889, 1.7306, 1.7809, 1.7523, 1.7603, 1.7693, 1.7924, 1.7771, 1.7835, 1.8545, 1.8541</t>
         </is>
       </c>
       <c r="E18" s="24" t="inlineStr">
@@ -4144,23 +4144,23 @@
         <v>5</v>
       </c>
       <c r="I18" s="74" t="n">
-        <v>1.7835</v>
+        <v>1.8541</v>
       </c>
       <c r="J18" s="75" t="n">
-        <v>0.3601373023465299</v>
+        <v>-0.02156915610676495</v>
       </c>
       <c r="K18" s="76" t="n">
         <v>1</v>
       </c>
       <c r="L18" s="76" t="n">
-        <v>0.3601373023465299</v>
+        <v>-0.02156915610676495</v>
       </c>
       <c r="M18" s="76" t="n">
-        <v>1.7835</v>
+        <v>1.8541</v>
       </c>
       <c r="N18" s="77" t="inlineStr">
         <is>
-          <t>2020-02-14</t>
+          <t>2020-02-18</t>
         </is>
       </c>
       <c r="O18" s="30">
@@ -4279,7 +4279,7 @@
       </c>
       <c r="D19" s="0" t="inlineStr">
         <is>
-          <t>1.1197, 1.1204, 1.1357, 1.1355, 1.1164, 1.1135, 1.1097, 1.1218, 1.1154, 1.1163, 1.1123, 1.106, 1.1066, 1.1103, 1.1049, 1.11, 1.1111, 1.1097, 1.1061, 1.1176, 1.1149, 1.1351, 1.1099, 1.1249, 1.1258, 1.1277, 1.1277, 1.1164, 1.1228, 1.1181, 1.1261, 1.1273, 1.1266, 1.1261, 1.143, 1.1458, 1.1385, 1.1436, 1.1265, 1.1321, 1.1319, 1.1347, 1.1322, 1.1205, 1.114, 1.1149, 1.1214, 1.107, 1.1067, 1.0836, 1.0166, 1.0373, 1.0375, 1.0442, 1.0404, 1.0366, 1.047, 1.0493, 1.0424, 1.0507</t>
+          <t>1.1357, 1.1355, 1.1164, 1.1135, 1.1097, 1.1218, 1.1154, 1.1163, 1.1123, 1.106, 1.1066, 1.1103, 1.1049, 1.11, 1.1111, 1.1097, 1.1061, 1.1176, 1.1149, 1.1351, 1.1099, 1.1249, 1.1258, 1.1277, 1.1277, 1.1164, 1.1228, 1.1181, 1.1261, 1.1273, 1.1266, 1.1261, 1.143, 1.1458, 1.1385, 1.1436, 1.1265, 1.1321, 1.1319, 1.1347, 1.1322, 1.1205, 1.114, 1.1149, 1.1214, 1.107, 1.1067, 1.0836, 1.0166, 1.0373, 1.0375, 1.0442, 1.0404, 1.0366, 1.047, 1.0493, 1.0424, 1.0507, 1.0686, 1.06</t>
         </is>
       </c>
       <c r="E19" s="3" t="inlineStr">
@@ -4291,23 +4291,23 @@
         <v>2</v>
       </c>
       <c r="I19" s="76" t="n">
-        <v>1.0507</v>
+        <v>1.06</v>
       </c>
       <c r="J19" s="78" t="n">
-        <v>0.7962394474290075</v>
+        <v>-0.8047913157402155</v>
       </c>
       <c r="K19" s="76" t="n">
         <v>1</v>
       </c>
       <c r="L19" s="76" t="n">
-        <v>0.7232485186476101</v>
+        <v>-0.7326631453399166</v>
       </c>
       <c r="M19" s="76" t="n">
-        <v>1.1559</v>
+        <v>1.1652</v>
       </c>
       <c r="N19" s="76" t="inlineStr">
         <is>
-          <t>2020-02-14</t>
+          <t>2020-02-18</t>
         </is>
       </c>
       <c r="O19" s="30">
@@ -4428,7 +4428,7 @@
       </c>
       <c r="D20" s="0" t="inlineStr">
         <is>
-          <t>1.819, 1.816, 1.816, 1.866, 1.848, 1.847, 1.821, 1.797, 1.81, 1.84, 1.835, 1.837, 1.847, 1.86, 1.871, 1.889, 1.894, 1.897, 1.908, 1.889, 1.884, 1.91, 1.942, 1.963, 1.963, 1.963, 1.941, 1.918, 1.974, 1.984, 1.987, 1.994, 2.002, 2.017, 2.072, 2.111, 2.164, 2.173, 2.149, 2.171, 2.159, 2.179, 2.189, 2.166, 2.153, 2.142, 2.152, 2.133, 2.166, 2.116, 1.984, 2.037, 2.092, 2.15, 2.156, 2.194, 2.206, 2.278, 2.263, 2.257</t>
+          <t>1.816, 1.866, 1.848, 1.847, 1.821, 1.797, 1.81, 1.84, 1.835, 1.837, 1.847, 1.86, 1.871, 1.889, 1.894, 1.897, 1.908, 1.889, 1.884, 1.91, 1.942, 1.963, 1.963, 1.963, 1.941, 1.918, 1.974, 1.984, 1.987, 1.994, 2.002, 2.017, 2.072, 2.111, 2.164, 2.173, 2.149, 2.171, 2.159, 2.179, 2.189, 2.166, 2.153, 2.142, 2.152, 2.133, 2.166, 2.116, 1.984, 2.037, 2.092, 2.15, 2.156, 2.194, 2.206, 2.278, 2.263, 2.257, 2.328, 2.338</t>
         </is>
       </c>
       <c r="E20" s="3" t="inlineStr">
@@ -4440,23 +4440,23 @@
         <v>3</v>
       </c>
       <c r="I20" s="76" t="n">
-        <v>2.257</v>
+        <v>2.338</v>
       </c>
       <c r="J20" s="78" t="n">
-        <v>-0.2651347768448866</v>
+        <v>0.4295532646048209</v>
       </c>
       <c r="K20" s="76" t="n">
         <v>2</v>
       </c>
       <c r="L20" s="76" t="n">
-        <v>-0.9218612818261593</v>
+        <v>3.588834736375718</v>
       </c>
       <c r="M20" s="76" t="n">
-        <v>2.257</v>
+        <v>2.338</v>
       </c>
       <c r="N20" s="76" t="inlineStr">
         <is>
-          <t>2020-02-14</t>
+          <t>2020-02-18</t>
         </is>
       </c>
       <c r="O20" s="30">
@@ -4577,30 +4577,30 @@
       </c>
       <c r="D21" s="0" t="inlineStr">
         <is>
-          <t>0.9038, 0.8946, 0.9066, 0.9137, 0.8999, 0.9003, 0.8975, 0.902, 0.9025, 0.8952, 0.8947, 0.8983, 0.9044, 0.9102, 0.9075, 0.9211, 0.925, 0.9236, 0.9218, 0.9231, 0.9179, 0.9508, 0.9654, 0.9905, 0.9934, 0.9887, 0.9923, 0.9687, 0.9782, 0.9796, 1.004, 0.9835, 1.0372, 1.0333, 1.0395, 1.0382, 1.0389, 1.0457, 1.0141, 1.0291, 1.0305, 1.0433, 1.0308, 1.0263, 1.0208, 1.0247, 1.0402, 1.0218, 1.0295, 0.9886, 0.8991, 0.8979, 0.9094, 0.9323, 0.9349, 0.9442, 0.9422, 0.9563, 0.941, 0.9581</t>
+          <t>0.9066, 0.9137, 0.8999, 0.9003, 0.8975, 0.902, 0.9025, 0.8952, 0.8947, 0.8983, 0.9044, 0.9102, 0.9075, 0.9211, 0.925, 0.9236, 0.9218, 0.9231, 0.9179, 0.9508, 0.9654, 0.9905, 0.9934, 0.9887, 0.9923, 0.9687, 0.9782, 0.9796, 1.004, 0.9835, 1.0372, 1.0333, 1.0395, 1.0382, 1.0389, 1.0457, 1.0141, 1.0291, 1.0305, 1.0433, 1.0308, 1.0263, 1.0208, 1.0247, 1.0402, 1.0218, 1.0295, 0.9886, 0.8991, 0.8979, 0.9094, 0.9323, 0.9349, 0.9442, 0.9422, 0.9563, 0.941, 0.9581, 1.0038, 0.9989</t>
         </is>
       </c>
       <c r="H21" s="3" t="n">
         <v>104</v>
       </c>
       <c r="I21" s="76" t="n">
-        <v>0.9581</v>
+        <v>0.9989</v>
       </c>
       <c r="J21" s="78" t="n">
-        <v>1.817215727948991</v>
+        <v>-0.4881450488145064</v>
       </c>
       <c r="K21" s="76" t="n">
         <v>1</v>
       </c>
       <c r="L21" s="76" t="n">
-        <v>1.817215727948991</v>
+        <v>-0.4881450488145064</v>
       </c>
       <c r="M21" s="76" t="n">
-        <v>0.9581</v>
+        <v>0.9989</v>
       </c>
       <c r="N21" s="76" t="inlineStr">
         <is>
-          <t>2020-02-14</t>
+          <t>2020-02-18</t>
         </is>
       </c>
       <c r="O21" s="30">
@@ -4726,30 +4726,30 @@
       </c>
       <c r="D22" s="0" t="inlineStr">
         <is>
-          <t>2.577, 2.579, 2.596, 2.597, 2.6, 2.588, 2.586, 2.591, 2.623, 2.625, 2.643, 2.64, 2.629, 2.6, 2.582, 2.6, 2.61, 2.631, 2.621, 2.619, 2.633, 2.647, 2.65, 2.664, 2.667, 2.668, 2.688, 2.699, 2.709, 2.709, 2.708, 2.722, 2.723, 2.703, 2.709, 2.744, 2.724, 2.74, 2.738, 2.748, 2.772, 2.76, 2.786, 2.764, 2.76, 2.784, 2.8, 2.792, 2.788, 2.802, 2.811, 2.8, 2.881, 2.893, 2.922, 2.902, 2.937, 2.938, 2.956, 2.955</t>
+          <t>2.596, 2.597, 2.6, 2.588, 2.586, 2.591, 2.623, 2.625, 2.643, 2.64, 2.629, 2.6, 2.582, 2.6, 2.61, 2.631, 2.621, 2.619, 2.633, 2.647, 2.65, 2.664, 2.667, 2.668, 2.688, 2.699, 2.709, 2.709, 2.708, 2.722, 2.723, 2.703, 2.709, 2.744, 2.724, 2.74, 2.738, 2.748, 2.772, 2.76, 2.786, 2.764, 2.76, 2.784, 2.8, 2.792, 2.788, 2.802, 2.811, 2.8, 2.881, 2.893, 2.922, 2.902, 2.937, 2.938, 2.956, 2.955, 2.963, 2.961</t>
         </is>
       </c>
       <c r="H22" s="3" t="n">
         <v>113</v>
       </c>
       <c r="I22" s="76" t="n">
-        <v>2.955</v>
+        <v>2.961</v>
       </c>
       <c r="J22" s="78" t="n">
-        <v>-0.03382949932340629</v>
+        <v>-0.0674991562605543</v>
       </c>
       <c r="K22" s="76" t="n">
         <v>1</v>
       </c>
       <c r="L22" s="76" t="n">
-        <v>-0.03382949932340629</v>
+        <v>-0.0674991562605543</v>
       </c>
       <c r="M22" s="76" t="n">
-        <v>2.955</v>
+        <v>2.961</v>
       </c>
       <c r="N22" s="76" t="inlineStr">
         <is>
-          <t>2020-02-13</t>
+          <t>2020-02-17</t>
         </is>
       </c>
       <c r="O22" s="30">
@@ -4868,30 +4868,30 @@
       </c>
       <c r="D23" s="0" t="inlineStr">
         <is>
-          <t>0.9701, 0.9605, 0.9733, 0.9812, 0.9661, 0.9666, 0.964, 0.9691, 0.9702, 0.9626, 0.9619, 0.9656, 0.9723, 0.9786, 0.9759, 0.9908, 0.9949, 0.9936, 0.9921, 0.9932, 0.9877, 1.0227, 1.0376, 1.064, 1.0659, 1.0619, 1.067, 1.0416, 1.0508, 1.0517, 1.0779, 1.0568, 1.1154, 1.1105, 1.1178, 1.1158, 1.1159, 1.1234, 1.091, 1.1058, 1.107, 1.1219, 1.1091, 1.104, 1.0983, 1.1025, 1.1192, 1.0998, 1.1071, 1.0629, 0.9641, 0.963, 0.9756, 0.998, 1.0008, 1.0104, 1.0089, 1.0218, 1.0065, 1.0217</t>
+          <t>0.9605, 0.9733, 0.9812, 0.9661, 0.9666, 0.964, 0.9691, 0.9702, 0.9626, 0.9619, 0.9656, 0.9723, 0.9786, 0.9759, 0.9908, 0.9949, 0.9936, 0.9921, 0.9932, 0.9877, 1.0227, 1.0376, 1.064, 1.0659, 1.0619, 1.067, 1.0416, 1.0508, 1.0517, 1.0779, 1.0568, 1.1154, 1.1105, 1.1178, 1.1158, 1.1159, 1.1234, 1.091, 1.1058, 1.107, 1.1219, 1.1091, 1.104, 1.0983, 1.1025, 1.1192, 1.0998, 1.1071, 1.0629, 0.9641, 0.963, 0.9756, 0.998, 1.0008, 1.0104, 1.0089, 1.0218, 1.0065, 1.0217, 1.0705</t>
         </is>
       </c>
       <c r="H23" s="3" t="n">
         <v>4</v>
       </c>
       <c r="I23" s="76" t="n">
-        <v>1.0217</v>
+        <v>1.0705</v>
       </c>
       <c r="J23" s="78" t="n">
-        <v>1.510183805265783</v>
+        <v>4.776353136928644</v>
       </c>
       <c r="K23" s="76" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L23" s="76" t="n">
-        <v>1.510183805265783</v>
+        <v>6.358668653750627</v>
       </c>
       <c r="M23" s="76" t="n">
-        <v>1.0217</v>
+        <v>1.0705</v>
       </c>
       <c r="N23" s="76" t="inlineStr">
         <is>
-          <t>2020-02-14</t>
+          <t>2020-02-17</t>
         </is>
       </c>
       <c r="O23" s="30">
@@ -5012,30 +5012,30 @@
       </c>
       <c r="D24" s="0" t="inlineStr">
         <is>
-          <t>1.504, 1.504, 1.497, 1.521, 1.516, 1.512, 1.496, 1.483, 1.51, 1.527, 1.526, 1.519, 1.532, 1.545, 1.549, 1.566, 1.584, 1.592, 1.604, 1.581, 1.581, 1.626, 1.657, 1.67, 1.649, 1.62, 1.618, 1.59, 1.606, 1.604, 1.609, 1.58, 1.597, 1.609, 1.642, 1.634, 1.65, 1.651, 1.632, 1.665, 1.67, 1.705, 1.709, 1.716, 1.715, 1.709, 1.755, 1.735, 1.784, 1.731, 1.604, 1.661, 1.67, 1.707, 1.699, 1.725, 1.743, 1.783, 1.775, 1.788</t>
+          <t>1.497, 1.521, 1.516, 1.512, 1.496, 1.483, 1.51, 1.527, 1.526, 1.519, 1.532, 1.545, 1.549, 1.566, 1.584, 1.592, 1.604, 1.581, 1.581, 1.626, 1.657, 1.67, 1.649, 1.62, 1.618, 1.59, 1.606, 1.604, 1.609, 1.58, 1.597, 1.609, 1.642, 1.634, 1.65, 1.651, 1.632, 1.665, 1.67, 1.705, 1.709, 1.716, 1.715, 1.709, 1.755, 1.735, 1.784, 1.731, 1.604, 1.661, 1.67, 1.707, 1.699, 1.725, 1.743, 1.783, 1.775, 1.788, 1.857, 1.895</t>
         </is>
       </c>
       <c r="H24" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I24" s="76" t="n">
-        <v>1.788</v>
+        <v>1.895</v>
       </c>
       <c r="J24" s="78" t="n">
-        <v>0.73239436619719</v>
+        <v>2.046311254711903</v>
       </c>
       <c r="K24" s="76" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L24" s="76" t="n">
-        <v>0.5816554809843555</v>
+        <v>5.369127516778528</v>
       </c>
       <c r="M24" s="76" t="n">
-        <v>2.248</v>
+        <v>2.355</v>
       </c>
       <c r="N24" s="76" t="inlineStr">
         <is>
-          <t>2020-02-14</t>
+          <t>2020-02-18</t>
         </is>
       </c>
       <c r="O24" s="0">
@@ -5156,30 +5156,30 @@
       </c>
       <c r="D25" s="0" t="inlineStr">
         <is>
-          <t>1.6932, 1.683, 1.6798, 1.719, 1.7163, 1.7134, 1.6409, 1.5957, 1.6259, 1.6451, 1.6407, 1.6363, 1.6574, 1.7108, 1.7164, 1.7361, 1.7637, 1.7824, 1.8359, 1.8088, 1.8309, 1.8497, 1.8954, 1.9017, 1.8895, 1.8703, 1.8415, 1.8062, 1.864, 1.8918, 1.8817, 1.8308, 1.8379, 1.8454, 1.8824, 1.8705, 1.8822, 1.8826, 1.8552, 1.9101, 1.9396, 1.982, 1.9654, 1.9967, 2.0032, 2.0143, 2.0945, 2.0749, 2.129, 2.0843, 1.9474, 2.034, 2.0439, 2.1053, 2.1487, 2.1539, 2.1677, 2.2087, 2.2184, 2.2406</t>
+          <t>1.6798, 1.719, 1.7163, 1.7134, 1.6409, 1.5957, 1.6259, 1.6451, 1.6407, 1.6363, 1.6574, 1.7108, 1.7164, 1.7361, 1.7637, 1.7824, 1.8359, 1.8088, 1.8309, 1.8497, 1.8954, 1.9017, 1.8895, 1.8703, 1.8415, 1.8062, 1.864, 1.8918, 1.8817, 1.8308, 1.8379, 1.8454, 1.8824, 1.8705, 1.8822, 1.8826, 1.8552, 1.9101, 1.9396, 1.982, 1.9654, 1.9967, 2.0032, 2.0143, 2.0945, 2.0749, 2.129, 2.0843, 1.9474, 2.034, 2.0439, 2.1053, 2.1487, 2.1539, 2.1677, 2.2087, 2.2184, 2.2406, 2.3069, 2.376</t>
         </is>
       </c>
       <c r="H25" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I25" s="76" t="n">
-        <v>2.2406</v>
+        <v>2.376</v>
       </c>
       <c r="J25" s="78" t="n">
-        <v>1.000721240533728</v>
+        <v>2.995361740864351</v>
       </c>
       <c r="K25" s="76" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="L25" s="76" t="n">
-        <v>14.715920497892</v>
+        <v>21.51174462959244</v>
       </c>
       <c r="M25" s="76" t="n">
-        <v>2.2856</v>
+        <v>2.421</v>
       </c>
       <c r="N25" s="76" t="inlineStr">
         <is>
-          <t>2020-02-14</t>
+          <t>2020-02-18</t>
         </is>
       </c>
       <c r="O25" s="0">
@@ -5300,30 +5300,30 @@
       </c>
       <c r="D26" s="0" t="inlineStr">
         <is>
-          <t>2.026, 2.013, 2.01, 2.056, 2.037, 2.045, 2.006, 1.946, 1.966, 2.017, 2.015, 2.019, 2.055, 2.078, 2.072, 2.131, 2.164, 2.178, 2.226, 2.203, 2.23, 2.262, 2.352, 2.379, 2.383, 2.356, 2.319, 2.249, 2.304, 2.349, 2.35, 2.298, 2.312, 2.308, 2.383, 2.398, 2.434, 2.454, 2.414, 2.471, 2.484, 2.558, 2.546, 2.577, 2.586, 2.592, 2.674, 2.649, 2.739, 2.646, 2.435, 2.523, 2.564, 2.649, 2.714, 2.732, 2.736, 2.826, 2.817, 2.829</t>
+          <t>2.01, 2.056, 2.037, 2.045, 2.006, 1.946, 1.966, 2.017, 2.015, 2.019, 2.055, 2.078, 2.072, 2.131, 2.164, 2.178, 2.226, 2.203, 2.23, 2.262, 2.352, 2.379, 2.383, 2.356, 2.319, 2.249, 2.304, 2.349, 2.35, 2.298, 2.312, 2.308, 2.383, 2.398, 2.434, 2.454, 2.414, 2.471, 2.484, 2.558, 2.546, 2.577, 2.586, 2.592, 2.674, 2.649, 2.739, 2.646, 2.435, 2.523, 2.564, 2.649, 2.714, 2.732, 2.736, 2.826, 2.817, 2.829, 2.954, 3.028</t>
         </is>
       </c>
       <c r="H26" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I26" s="76" t="n">
-        <v>2.829</v>
+        <v>3.028</v>
       </c>
       <c r="J26" s="78" t="n">
-        <v>0.4259850905218321</v>
+        <v>2.505077860528092</v>
       </c>
       <c r="K26" s="76" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L26" s="76" t="n">
-        <v>0.4168113928447382</v>
+        <v>7.328933657519968</v>
       </c>
       <c r="M26" s="76" t="n">
-        <v>2.891</v>
+        <v>3.09</v>
       </c>
       <c r="N26" s="76" t="inlineStr">
         <is>
-          <t>2020-02-14</t>
+          <t>2020-02-18</t>
         </is>
       </c>
       <c r="O26" s="0">
@@ -5444,30 +5444,30 @@
       </c>
       <c r="D27" s="0" t="inlineStr">
         <is>
-          <t>1.1219, 1.1127, 1.1209, 1.1348, 1.1289, 1.1244, 1.1164, 1.1142, 1.1171, 1.1176, 1.1149, 1.1086, 1.1122, 1.1144, 1.1165, 1.1276, 1.1346, 1.1362, 1.1447, 1.1471, 1.1512, 1.1643, 1.1761, 1.1839, 1.1826, 1.1762, 1.1691, 1.1609, 1.173, 1.1797, 1.1846, 1.1787, 1.1897, 1.1982, 1.2174, 1.2225, 1.2272, 1.2349, 1.2271, 1.2388, 1.2347, 1.2452, 1.2487, 1.2422, 1.2368, 1.24, 1.26, 1.2557, 1.2639, 1.2383, 1.1689, 1.2131, 1.2282, 1.255, 1.2568, 1.2658, 1.2673, 1.2927, 1.2876, 1.2879</t>
+          <t>1.1209, 1.1348, 1.1289, 1.1244, 1.1164, 1.1142, 1.1171, 1.1176, 1.1149, 1.1086, 1.1122, 1.1144, 1.1165, 1.1276, 1.1346, 1.1362, 1.1447, 1.1471, 1.1512, 1.1643, 1.1761, 1.1839, 1.1826, 1.1762, 1.1691, 1.1609, 1.173, 1.1797, 1.1846, 1.1787, 1.1897, 1.1982, 1.2174, 1.2225, 1.2272, 1.2349, 1.2271, 1.2388, 1.2347, 1.2452, 1.2487, 1.2422, 1.2368, 1.24, 1.26, 1.2557, 1.2639, 1.2383, 1.1689, 1.2131, 1.2282, 1.255, 1.2568, 1.2658, 1.2673, 1.2927, 1.2876, 1.2879, 1.3212, 1.335</t>
         </is>
       </c>
       <c r="H27" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I27" s="76" t="n">
-        <v>1.2879</v>
+        <v>1.335</v>
       </c>
       <c r="J27" s="78" t="n">
-        <v>0.02329916123019314</v>
+        <v>1.044504995458676</v>
       </c>
       <c r="K27" s="76" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L27" s="76" t="n">
-        <v>0.02329916123019314</v>
+        <v>3.681267474370914</v>
       </c>
       <c r="M27" s="76" t="n">
-        <v>1.2879</v>
+        <v>1.335</v>
       </c>
       <c r="N27" s="76" t="inlineStr">
         <is>
-          <t>2020-02-14</t>
+          <t>2020-02-18</t>
         </is>
       </c>
       <c r="O27" s="0">
@@ -5588,30 +5588,30 @@
       </c>
       <c r="D28" s="0" t="inlineStr">
         <is>
-          <t>0.9503, 0.9297, 0.954, 0.9697, 0.9387, 0.9394, 0.9333, 0.9427, 0.9436, 0.9273, 0.9261, 0.9342, 0.947, 0.9593, 0.9536, 0.9831, 0.9912, 0.9876, 0.9837, 0.9859, 0.9746, 1.0475, 1.0772, 1.1303, 1.1348, 1.1244, 1.1315, 1.0805, 1.1006, 1.1029, 1.1536, 1.1092, 1.2243, 1.2154, 1.2283, 1.2258, 1.2266, 1.2403, 1.1714, 1.2046, 1.2077, 1.2351, 1.208, 1.1977, 1.1858, 1.1941, 1.2261, 1.186, 1.2016, 1.1115, 0.9104, 0.9076, 0.9339, 0.983, 0.9885, 1.0069, 1.0022, 1.0312, 0.9983, 1.0348</t>
+          <t>0.954, 0.9697, 0.9387, 0.9394, 0.9333, 0.9427, 0.9436, 0.9273, 0.9261, 0.9342, 0.947, 0.9593, 0.9536, 0.9831, 0.9912, 0.9876, 0.9837, 0.9859, 0.9746, 1.0475, 1.0772, 1.1303, 1.1348, 1.1244, 1.1315, 1.0805, 1.1006, 1.1029, 1.1536, 1.1092, 1.2243, 1.2154, 1.2283, 1.2258, 1.2266, 1.2403, 1.1714, 1.2046, 1.2077, 1.2351, 1.208, 1.1977, 1.1858, 1.1941, 1.2261, 1.186, 1.2016, 1.1115, 0.9104, 0.9076, 0.9339, 0.983, 0.9885, 1.0069, 1.0022, 1.0312, 0.9983, 1.0348, 1.1292, 1.1173</t>
         </is>
       </c>
       <c r="H28" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I28" s="76" t="n">
-        <v>1.0348</v>
+        <v>1.1173</v>
       </c>
       <c r="J28" s="78" t="n">
-        <v>3.656215566462985</v>
+        <v>-1.053843428976268</v>
       </c>
       <c r="K28" s="76" t="n">
         <v>1</v>
       </c>
       <c r="L28" s="76" t="n">
-        <v>0.6130268199233679</v>
+        <v>-0.1502629601803198</v>
       </c>
       <c r="M28" s="76" t="n">
-        <v>0.1313</v>
+        <v>0.1329</v>
       </c>
       <c r="N28" s="76" t="inlineStr">
         <is>
-          <t>2020-02-14</t>
+          <t>2020-02-18</t>
         </is>
       </c>
       <c r="O28" s="0">
@@ -5732,30 +5732,30 @@
       </c>
       <c r="D29" s="0" t="inlineStr">
         <is>
-          <t>1, 0.985, 0.991, 1.03, 1.028, 1.032, 1.04, 1.036, 1.06, 1.07, 1.067, 1.062, 1.058, 1.066, 1.073, 1.094, 1.105, 1.099, 1.097, 1.079, 1.076, 1.085, 1.1, 1.132, 1.12, 1.122, 1.122, 1.12, 1.175, 1.19, 1.195, 1.186, 1.206, 1.206, 1.219, 1.231, 1.278, 1.27, 1.274, 1.289, 1.285, 1.31, 1.332, 1.309, 1.309, 1.306, 1.34, 1.32, 1.375, 1.345, 1.251, 1.339, 1.385, 1.413, 1.372, 1.433, 1.426, 1.477, 1.464, 1.45</t>
+          <t>0.991, 1.03, 1.028, 1.032, 1.04, 1.036, 1.06, 1.07, 1.067, 1.062, 1.058, 1.066, 1.073, 1.094, 1.105, 1.099, 1.097, 1.079, 1.076, 1.085, 1.1, 1.132, 1.12, 1.122, 1.122, 1.12, 1.175, 1.19, 1.195, 1.186, 1.206, 1.206, 1.219, 1.231, 1.278, 1.27, 1.274, 1.289, 1.285, 1.31, 1.332, 1.309, 1.309, 1.306, 1.34, 1.32, 1.375, 1.345, 1.251, 1.339, 1.385, 1.413, 1.372, 1.433, 1.426, 1.477, 1.464, 1.45, 1.496, 1.509</t>
         </is>
       </c>
       <c r="H29" s="0" t="n">
         <v>100</v>
       </c>
       <c r="I29" s="76" t="n">
-        <v>1.45</v>
+        <v>1.509</v>
       </c>
       <c r="J29" s="78" t="n">
-        <v>-0.9562841530054653</v>
+        <v>0.8689839572192447</v>
       </c>
       <c r="K29" s="76" t="n">
         <v>2</v>
       </c>
       <c r="L29" s="76" t="n">
-        <v>-1.708542713567841</v>
+        <v>3.783231083844573</v>
       </c>
       <c r="M29" s="76" t="n">
-        <v>0.978</v>
+        <v>1.015</v>
       </c>
       <c r="N29" s="76" t="inlineStr">
         <is>
-          <t>2020-02-14</t>
+          <t>2020-02-18</t>
         </is>
       </c>
       <c r="O29" s="0">
@@ -5872,30 +5872,30 @@
       </c>
       <c r="D30" s="0" t="inlineStr">
         <is>
-          <t>1.823, 1.8148, 1.8259, 1.8422, 1.8237, 1.8085, 1.7809, 1.7907, 1.7907, 1.7898, 1.7839, 1.7542, 1.7555, 1.7626, 1.7641, 1.7722, 1.7847, 1.775, 1.7794, 1.7841, 1.7774, 1.8144, 1.8057, 1.8216, 1.8156, 1.8097, 1.8065, 1.7942, 1.7721, 1.7641, 1.778, 1.7856, 1.802, 1.808, 1.8266, 1.8226, 1.8043, 1.8185, 1.8006, 1.8201, 1.8233, 1.8414, 1.8286, 1.8242, 1.8186, 1.8235, 1.8314, 1.8017, 1.8043, 1.7538, 1.6446, 1.6912, 1.7048, 1.7352, 1.7306, 1.7254, 1.7459, 1.7522, 1.7386, 1.7487</t>
+          <t>1.8259, 1.8422, 1.8237, 1.8085, 1.7809, 1.7907, 1.7907, 1.7898, 1.7839, 1.7542, 1.7555, 1.7626, 1.7641, 1.7722, 1.7847, 1.775, 1.7794, 1.7841, 1.7774, 1.8144, 1.8057, 1.8216, 1.8156, 1.8097, 1.8065, 1.7942, 1.7721, 1.7641, 1.778, 1.7856, 1.802, 1.808, 1.8266, 1.8226, 1.8043, 1.8185, 1.8006, 1.8201, 1.8233, 1.8414, 1.8286, 1.8242, 1.8186, 1.8235, 1.8314, 1.8017, 1.8043, 1.7538, 1.6446, 1.6912, 1.7048, 1.7352, 1.7306, 1.7254, 1.7459, 1.7522, 1.7386, 1.7487, 1.7698, 1.7532</t>
         </is>
       </c>
       <c r="H30" s="0" t="n">
         <v>10</v>
       </c>
       <c r="I30" s="76" t="n">
-        <v>1.7487</v>
+        <v>1.7532</v>
       </c>
       <c r="J30" s="78" t="n">
-        <v>0.5809271827907512</v>
+        <v>-0.9379590914227567</v>
       </c>
       <c r="K30" s="76" t="n">
         <v>1</v>
       </c>
       <c r="L30" s="76" t="n">
-        <v>0.2775792887374264</v>
+        <v>-0.4523407270150948</v>
       </c>
       <c r="M30" s="76" t="n">
-        <v>3.6487</v>
+        <v>3.6532</v>
       </c>
       <c r="N30" s="76" t="inlineStr">
         <is>
-          <t>2020-02-14</t>
+          <t>2020-02-18</t>
         </is>
       </c>
       <c r="O30" s="0">
@@ -6016,30 +6016,30 @@
       </c>
       <c r="D31" s="0" t="inlineStr">
         <is>
-          <t>2.6147, 2.6155, 2.6331, 2.6354, 2.6381, 2.6253, 2.6238, 2.6289, 2.6617, 2.6644, 2.6821, 2.6794, 2.6681, 2.6388, 2.6207, 2.6387, 2.6477, 2.6701, 2.6595, 2.6576, 2.6715, 2.6862, 2.6894, 2.7055, 2.7086, 2.7095, 2.7286, 2.7398, 2.7489, 2.7497, 2.7478, 2.7629, 2.7632, 2.7424, 2.7479, 2.7864, 2.7642, 2.7818, 2.7804, 2.7923, 2.8172, 2.8047, 2.8335, 2.8115, 2.8078, 2.8327, 2.8494, 2.8418, 2.8371, 2.8507, 2.8592, 2.8425, 2.9278, 2.94, 2.9716, 2.9499, 2.9892, 2.9893, 3.0119, 3.0082</t>
+          <t>2.6331, 2.6354, 2.6381, 2.6253, 2.6238, 2.6289, 2.6617, 2.6644, 2.6821, 2.6794, 2.6681, 2.6388, 2.6207, 2.6387, 2.6477, 2.6701, 2.6595, 2.6576, 2.6715, 2.6862, 2.6894, 2.7055, 2.7086, 2.7095, 2.7286, 2.7398, 2.7489, 2.7497, 2.7478, 2.7629, 2.7632, 2.7424, 2.7479, 2.7864, 2.7642, 2.7818, 2.7804, 2.7923, 2.8172, 2.8047, 2.8335, 2.8115, 2.8078, 2.8327, 2.8494, 2.8418, 2.8371, 2.8507, 2.8592, 2.8425, 2.9278, 2.94, 2.9716, 2.9499, 2.9892, 2.9893, 3.0119, 3.0082, 3.018, 3.0158</t>
         </is>
       </c>
       <c r="H31" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I31" s="76" t="n">
-        <v>3.0082</v>
+        <v>3.0158</v>
       </c>
       <c r="J31" s="78" t="n">
-        <v>-0.1228460440253599</v>
+        <v>-0.07289595758779847</v>
       </c>
       <c r="K31" s="76" t="n">
         <v>1</v>
       </c>
       <c r="L31" s="76" t="n">
-        <v>-0.1127395715896223</v>
+        <v>-0.06690997566909239</v>
       </c>
       <c r="M31" s="76" t="n">
-        <v>3.2782</v>
+        <v>3.2858</v>
       </c>
       <c r="N31" s="76" t="inlineStr">
         <is>
-          <t>2020-02-13</t>
+          <t>2020-02-17</t>
         </is>
       </c>
       <c r="O31" s="0">
@@ -6148,30 +6148,30 @@
       </c>
       <c r="D32" s="0" t="inlineStr">
         <is>
-          <t>0.874, 0.87, 0.857, 0.874, 0.869, 0.864, 0.831, 0.808, 0.819, 0.836, 0.839, 0.837, 0.854, 0.864, 0.874, 0.892, 0.91, 0.928, 0.951, 0.946, 0.951, 0.962, 1.006, 1.017, 1.022, 1.006, 0.991, 0.951, 0.974, 0.996, 0.988, 0.957, 0.96, 0.957, 0.976, 0.965, 0.968, 0.98, 0.962, 1.004, 1.016, 1.046, 1.05, 1.072, 1.093, 1.108, 1.136, 1.129, 1.179, 1.141, 1.04, 1.114, 1.143, 1.18, 1.213, 1.176, 1.181, 1.221, 1.219, 1.211</t>
+          <t>0.857, 0.874, 0.869, 0.864, 0.831, 0.808, 0.819, 0.836, 0.839, 0.837, 0.854, 0.864, 0.874, 0.892, 0.91, 0.928, 0.951, 0.946, 0.951, 0.962, 1.006, 1.017, 1.022, 1.006, 0.991, 0.951, 0.974, 0.996, 0.988, 0.957, 0.96, 0.957, 0.976, 0.965, 0.968, 0.98, 0.962, 1.004, 1.016, 1.046, 1.05, 1.072, 1.093, 1.108, 1.136, 1.129, 1.179, 1.141, 1.04, 1.114, 1.143, 1.18, 1.213, 1.176, 1.181, 1.221, 1.219, 1.211, 1.246, 1.292</t>
         </is>
       </c>
       <c r="H32" s="0" t="n">
         <v>10</v>
       </c>
       <c r="I32" s="76" t="n">
-        <v>1.211</v>
+        <v>1.292</v>
       </c>
       <c r="J32" s="78" t="n">
-        <v>-0.6562756357670227</v>
+        <v>3.691813804173358</v>
       </c>
       <c r="K32" s="76" t="n">
         <v>2</v>
       </c>
       <c r="L32" s="76" t="n">
-        <v>-0.3154574132492046</v>
+        <v>2.563291139240505</v>
       </c>
       <c r="M32" s="76" t="n">
-        <v>3.16</v>
+        <v>3.241</v>
       </c>
       <c r="N32" s="76" t="inlineStr">
         <is>
-          <t>2020-02-14</t>
+          <t>2020-02-18</t>
         </is>
       </c>
       <c r="O32" s="0">
@@ -6292,30 +6292,30 @@
       </c>
       <c r="D33" s="0" t="inlineStr">
         <is>
-          <t>1.8636, 1.856, 1.8537, 1.9026, 1.9009, 1.8976, 1.8177, 1.768, 1.8006, 1.8194, 1.8181, 1.8128, 1.8346, 1.892, 1.8968, 1.9188, 1.9443, 1.9634, 2.021, 1.9917, 2.0176, 2.0428, 2.0965, 2.1055, 2.0867, 2.0683, 2.031, 1.9883, 2.0558, 2.0847, 2.0682, 2.0081, 2.0205, 2.031, 2.0743, 2.0578, 2.0787, 2.0751, 2.0351, 2.1002, 2.1392, 2.188, 2.1672, 2.2078, 2.2102, 2.2243, 2.3164, 2.294, 2.3611, 2.3208, 2.169, 2.2652, 2.2853, 2.3499, 2.3926, 2.3979, 2.4137, 2.4626, 2.4709, 2.4955</t>
+          <t>1.8537, 1.9026, 1.9009, 1.8976, 1.8177, 1.768, 1.8006, 1.8194, 1.8181, 1.8128, 1.8346, 1.892, 1.8968, 1.9188, 1.9443, 1.9634, 2.021, 1.9917, 2.0176, 2.0428, 2.0965, 2.1055, 2.0867, 2.0683, 2.031, 1.9883, 2.0558, 2.0847, 2.0682, 2.0081, 2.0205, 2.031, 2.0743, 2.0578, 2.0787, 2.0751, 2.0351, 2.1002, 2.1392, 2.188, 2.1672, 2.2078, 2.2102, 2.2243, 2.3164, 2.294, 2.3611, 2.3208, 2.169, 2.2652, 2.2853, 2.3499, 2.3926, 2.3979, 2.4137, 2.4626, 2.4709, 2.4955, 2.5689, 2.6463</t>
         </is>
       </c>
       <c r="H33" s="0" t="n">
         <v>5</v>
       </c>
       <c r="I33" s="76" t="n">
-        <v>2.4955</v>
+        <v>2.6463</v>
       </c>
       <c r="J33" s="78" t="n">
-        <v>0.9955886519082099</v>
+        <v>3.012962746700919</v>
       </c>
       <c r="K33" s="76" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="L33" s="76" t="n">
-        <v>7.244286665187492</v>
+        <v>10.5901930330597</v>
       </c>
       <c r="M33" s="76" t="n">
-        <v>4.8335</v>
+        <v>4.9843</v>
       </c>
       <c r="N33" s="76" t="inlineStr">
         <is>
-          <t>2020-02-14</t>
+          <t>2020-02-18</t>
         </is>
       </c>
       <c r="O33" s="0">
@@ -6432,30 +6432,30 @@
       </c>
       <c r="D34" s="0" t="inlineStr">
         <is>
-          <t>1.2812, 1.2709, 1.2751, 1.2951, 1.2779, 1.2758, 1.2489, 1.2055, 1.2185, 1.2555, 1.2529, 1.2591, 1.2845, 1.3128, 1.3214, 1.3439, 1.3735, 1.3891, 1.4311, 1.4166, 1.4534, 1.4525, 1.4835, 1.4761, 1.4765, 1.4415, 1.4303, 1.3849, 1.4227, 1.4876, 1.4754, 1.4345, 1.4418, 1.4379, 1.4891, 1.487, 1.4992, 1.4905, 1.4571, 1.4964, 1.5418, 1.6194, 1.6067, 1.6429, 1.6427, 1.6377, 1.7166, 1.718, 1.7997, 1.7785, 1.6634, 1.7211, 1.7295, 1.7679, 1.8224, 1.7854, 1.8022, 1.8508, 1.9104, 1.9366</t>
+          <t>1.2751, 1.2951, 1.2779, 1.2758, 1.2489, 1.2055, 1.2185, 1.2555, 1.2529, 1.2591, 1.2845, 1.3128, 1.3214, 1.3439, 1.3735, 1.3891, 1.4311, 1.4166, 1.4534, 1.4525, 1.4835, 1.4761, 1.4765, 1.4415, 1.4303, 1.3849, 1.4227, 1.4876, 1.4754, 1.4345, 1.4418, 1.4379, 1.4891, 1.487, 1.4992, 1.4905, 1.4571, 1.4964, 1.5418, 1.6194, 1.6067, 1.6429, 1.6427, 1.6377, 1.7166, 1.718, 1.7997, 1.7785, 1.6634, 1.7211, 1.7295, 1.7679, 1.8224, 1.7854, 1.8022, 1.8508, 1.9104, 1.9366, 1.9868, 2.0561</t>
         </is>
       </c>
       <c r="H34" s="0" t="n">
         <v>5</v>
       </c>
       <c r="I34" s="76" t="n">
-        <v>1.9366</v>
+        <v>2.0561</v>
       </c>
       <c r="J34" s="82" t="n">
-        <v>1.3714405360134</v>
+        <v>3.488020938192064</v>
       </c>
       <c r="K34" s="76" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L34" s="76" t="n">
-        <v>8.468690489526157</v>
+        <v>15.16186848885402</v>
       </c>
       <c r="M34" s="76" t="n">
-        <v>1.9366</v>
+        <v>2.0561</v>
       </c>
       <c r="N34" s="76" t="inlineStr">
         <is>
-          <t>2020-02-14</t>
+          <t>2020-02-18</t>
         </is>
       </c>
       <c r="O34" s="0">
@@ -6572,30 +6572,30 @@
       </c>
       <c r="D35" s="0" t="inlineStr">
         <is>
-          <t>0.822, 0.813, 0.817, 0.838, 0.834, 0.831, 0.815, 0.806, 0.814, 0.813, 0.813, 0.808, 0.81, 0.813, 0.812, 0.829, 0.837, 0.833, 0.839, 0.832, 0.834, 0.851, 0.863, 0.872, 0.867, 0.866, 0.858, 0.842, 0.857, 0.864, 0.868, 0.855, 0.865, 0.869, 0.885, 0.885, 0.897, 0.912, 0.898, 0.922, 0.918, 0.933, 0.927, 0.928, 0.93, 0.931, 0.954, 0.948, 0.961, 0.93, 0.869, 0.912, 0.938, 0.972, 0.972, 0.985, 0.978, 1.004, 0.994, 0.996</t>
+          <t>0.817, 0.838, 0.834, 0.831, 0.815, 0.806, 0.814, 0.813, 0.813, 0.808, 0.81, 0.813, 0.812, 0.829, 0.837, 0.833, 0.839, 0.832, 0.834, 0.851, 0.863, 0.872, 0.867, 0.866, 0.858, 0.842, 0.857, 0.864, 0.868, 0.855, 0.865, 0.869, 0.885, 0.885, 0.897, 0.912, 0.898, 0.922, 0.918, 0.933, 0.927, 0.928, 0.93, 0.931, 0.954, 0.948, 0.961, 0.93, 0.869, 0.912, 0.938, 0.972, 0.972, 0.985, 0.978, 1.004, 0.994, 0.996, 1.031, 1.043</t>
         </is>
       </c>
       <c r="H35" s="0" t="n">
         <v>5</v>
       </c>
       <c r="I35" s="76" t="n">
-        <v>0.996</v>
+        <v>1.043</v>
       </c>
       <c r="J35" s="78" t="n">
-        <v>0.2012072434607648</v>
+        <v>1.163918525703202</v>
       </c>
       <c r="K35" s="76" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L35" s="76" t="n">
-        <v>0.08873114463175598</v>
+        <v>2.173913043478258</v>
       </c>
       <c r="M35" s="76" t="n">
-        <v>2.256</v>
+        <v>2.303</v>
       </c>
       <c r="N35" s="76" t="inlineStr">
         <is>
-          <t>2020-02-14</t>
+          <t>2020-02-18</t>
         </is>
       </c>
       <c r="O35" s="0">
@@ -6712,30 +6712,30 @@
       </c>
       <c r="D36" s="0" t="inlineStr">
         <is>
-          <t>1.7457, 1.745, 1.7589, 1.7615, 1.7652, 1.7562, 1.7507, 1.7507, 1.7763, 1.7761, 1.7857, 1.7838, 1.7787, 1.7547, 1.7396, 1.7493, 1.759, 1.7741, 1.7664, 1.7664, 1.7778, 1.7929, 1.8013, 1.81, 1.8084, 1.8072, 1.8205, 1.8303, 1.8378, 1.8383, 1.837, 1.8425, 1.8447, 1.8326, 1.8375, 1.8636, 1.8466, 1.8522, 1.8497, 1.8619, 1.8831, 1.8759, 1.8971, 1.8787, 1.8771, 1.9006, 1.9153, 1.9095, 1.9062, 1.9186, 1.9279, 1.9119, 1.9736, 1.9855, 2.0068, 1.9844, 2.011, 2.0056, 2.0214, 2.0176</t>
+          <t>1.7589, 1.7615, 1.7652, 1.7562, 1.7507, 1.7507, 1.7763, 1.7761, 1.7857, 1.7838, 1.7787, 1.7547, 1.7396, 1.7493, 1.759, 1.7741, 1.7664, 1.7664, 1.7778, 1.7929, 1.8013, 1.81, 1.8084, 1.8072, 1.8205, 1.8303, 1.8378, 1.8383, 1.837, 1.8425, 1.8447, 1.8326, 1.8375, 1.8636, 1.8466, 1.8522, 1.8497, 1.8619, 1.8831, 1.8759, 1.8971, 1.8787, 1.8771, 1.9006, 1.9153, 1.9095, 1.9062, 1.9186, 1.9279, 1.9119, 1.9736, 1.9855, 2.0068, 1.9844, 2.011, 2.0056, 2.0214, 2.0176, 2.0275, 2.026</t>
         </is>
       </c>
       <c r="H36" s="0" t="n">
         <v>5</v>
       </c>
       <c r="I36" s="76" t="n">
-        <v>2.0176</v>
+        <v>2.026</v>
       </c>
       <c r="J36" s="78" t="n">
-        <v>-0.1879885228059773</v>
+        <v>-0.07398273736128518</v>
       </c>
       <c r="K36" s="76" t="n">
         <v>1</v>
       </c>
       <c r="L36" s="76" t="n">
-        <v>-0.1879885228059773</v>
+        <v>-0.07398273736128518</v>
       </c>
       <c r="M36" s="76" t="n">
-        <v>2.0176</v>
+        <v>2.026</v>
       </c>
       <c r="N36" s="76" t="inlineStr">
         <is>
-          <t>2020-02-13</t>
+          <t>2020-02-17</t>
         </is>
       </c>
       <c r="O36" s="0">
@@ -6852,30 +6852,30 @@
       </c>
       <c r="D37" s="0" t="inlineStr">
         <is>
-          <t>1.128, 1.119, 1.112, 1.136, 1.135, 1.132, 1.125, 1.103, 1.109, 1.13, 1.13, 1.133, 1.142, 1.16, 1.154, 1.174, 1.194, 1.189, 1.205, 1.197, 1.203, 1.221, 1.24, 1.247, 1.244, 1.236, 1.224, 1.201, 1.225, 1.246, 1.238, 1.221, 1.239, 1.24, 1.262, 1.262, 1.283, 1.283, 1.281, 1.31, 1.311, 1.351, 1.335, 1.345, 1.352, 1.35, 1.389, 1.375, 1.402, 1.347, 1.233, 1.299, 1.315, 1.341, 1.344, 1.364, 1.371, 1.383, 1.379, 1.377</t>
+          <t>1.112, 1.136, 1.135, 1.132, 1.125, 1.103, 1.109, 1.13, 1.13, 1.133, 1.142, 1.16, 1.154, 1.174, 1.194, 1.189, 1.205, 1.197, 1.203, 1.221, 1.24, 1.247, 1.244, 1.236, 1.224, 1.201, 1.225, 1.246, 1.238, 1.221, 1.239, 1.24, 1.262, 1.262, 1.283, 1.283, 1.281, 1.31, 1.311, 1.351, 1.335, 1.345, 1.352, 1.35, 1.389, 1.375, 1.402, 1.347, 1.233, 1.299, 1.315, 1.341, 1.344, 1.364, 1.371, 1.383, 1.379, 1.377, 1.426, 1.445</t>
         </is>
       </c>
       <c r="H37" s="0" t="n">
         <v>10</v>
       </c>
       <c r="I37" s="76" t="n">
-        <v>1.377</v>
+        <v>1.445</v>
       </c>
       <c r="J37" s="78" t="n">
-        <v>-0.1450326323422771</v>
+        <v>1.332398316970556</v>
       </c>
       <c r="K37" s="76" t="n">
         <v>2</v>
       </c>
       <c r="L37" s="76" t="n">
-        <v>-0.4338394793926251</v>
+        <v>4.938271604938276</v>
       </c>
       <c r="M37" s="76" t="n">
-        <v>1.377</v>
+        <v>1.445</v>
       </c>
       <c r="N37" s="76" t="inlineStr">
         <is>
-          <t>2020-02-14</t>
+          <t>2020-02-18</t>
         </is>
       </c>
       <c r="O37" s="0">
@@ -6996,30 +6996,30 @@
       </c>
       <c r="D38" s="0" t="inlineStr">
         <is>
-          <t>1.2768, 1.2664, 1.2711, 1.2911, 1.2738, 1.2717, 1.2449, 1.2015, 1.2146, 1.2514, 1.2488, 1.255, 1.2803, 1.3085, 1.317, 1.3394, 1.3687, 1.3842, 1.426, 1.4116, 1.4482, 1.4473, 1.4782, 1.4708, 1.4711, 1.4363, 1.4251, 1.3799, 1.4175, 1.4822, 1.47, 1.4293, 1.4365, 1.4326, 1.4836, 1.4815, 1.4936, 1.4849, 1.4517, 1.4908, 1.536, 1.6133, 1.6006, 1.6367, 1.6365, 1.6314, 1.7101, 1.7114, 1.7928, 1.7716, 1.6569, 1.7143, 1.7227, 1.7609, 1.8152, 1.7783, 1.7951, 1.8434, 1.9028, 1.9289</t>
+          <t>1.2711, 1.2911, 1.2738, 1.2717, 1.2449, 1.2015, 1.2146, 1.2514, 1.2488, 1.255, 1.2803, 1.3085, 1.317, 1.3394, 1.3687, 1.3842, 1.426, 1.4116, 1.4482, 1.4473, 1.4782, 1.4708, 1.4711, 1.4363, 1.4251, 1.3799, 1.4175, 1.4822, 1.47, 1.4293, 1.4365, 1.4326, 1.4836, 1.4815, 1.4936, 1.4849, 1.4517, 1.4908, 1.536, 1.6133, 1.6006, 1.6367, 1.6365, 1.6314, 1.7101, 1.7114, 1.7928, 1.7716, 1.6569, 1.7143, 1.7227, 1.7609, 1.8152, 1.7783, 1.7951, 1.8434, 1.9028, 1.9289, 1.9788, 2.0478</t>
         </is>
       </c>
       <c r="H38" s="0" t="n">
         <v>10</v>
       </c>
       <c r="I38" s="76" t="n">
-        <v>1.9289</v>
+        <v>2.0478</v>
       </c>
       <c r="J38" s="82" t="n">
-        <v>1.371662812697079</v>
+        <v>3.486961795027298</v>
       </c>
       <c r="K38" s="76" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L38" s="76" t="n">
-        <v>8.468762301074063</v>
+        <v>15.15492324129787</v>
       </c>
       <c r="M38" s="76" t="n">
-        <v>1.9289</v>
+        <v>2.0478</v>
       </c>
       <c r="N38" s="76" t="inlineStr">
         <is>
-          <t>2020-02-14</t>
+          <t>2020-02-18</t>
         </is>
       </c>
       <c r="O38" s="0">
@@ -7253,30 +7253,30 @@
       </c>
       <c r="D40" s="0" t="inlineStr">
         <is>
-          <t>1.2161, 1.2084, 1.2211, 1.2346, 1.2237, 1.2186, 1.2058, 1.2128, 1.2141, 1.2094, 1.2053, 1.1931, 1.1971, 1.2015, 1.2013, 1.2115, 1.2188, 1.2185, 1.222, 1.2239, 1.2197, 1.2441, 1.2484, 1.2631, 1.2592, 1.258, 1.2553, 1.2408, 1.2489, 1.2486, 1.2577, 1.2589, 1.277, 1.2824, 1.2999, 1.2971, 1.2906, 1.2992, 1.285, 1.3021, 1.3023, 1.3132, 1.3075, 1.3017, 1.2986, 1.3007, 1.3108, 1.2888, 1.2967, 1.2591, 1.1679, 1.2075, 1.2197, 1.2419, 1.2415, 1.2453, 1.257, 1.2682, 1.2643, 1.272</t>
+          <t>1.2211, 1.2346, 1.2237, 1.2186, 1.2058, 1.2128, 1.2141, 1.2094, 1.2053, 1.1931, 1.1971, 1.2015, 1.2013, 1.2115, 1.2188, 1.2185, 1.222, 1.2239, 1.2197, 1.2441, 1.2484, 1.2631, 1.2592, 1.258, 1.2553, 1.2408, 1.2489, 1.2486, 1.2577, 1.2589, 1.277, 1.2824, 1.2999, 1.2971, 1.2906, 1.2992, 1.285, 1.3021, 1.3023, 1.3132, 1.3075, 1.3017, 1.2986, 1.3007, 1.3108, 1.2888, 1.2967, 1.2591, 1.1679, 1.2075, 1.2197, 1.2419, 1.2415, 1.2453, 1.257, 1.2682, 1.2643, 1.272, 1.3008, 1.2964</t>
         </is>
       </c>
       <c r="H40" s="0" t="n">
         <v>115</v>
       </c>
       <c r="I40" s="76" t="n">
-        <v>1.272</v>
+        <v>1.2964</v>
       </c>
       <c r="J40" s="78" t="n">
-        <v>0.6090326662975591</v>
+        <v>-0.3382533825338223</v>
       </c>
       <c r="K40" s="76" t="n">
         <v>1</v>
       </c>
       <c r="L40" s="76" t="n">
-        <v>0.6090326662975591</v>
+        <v>-0.3382533825338223</v>
       </c>
       <c r="M40" s="76" t="n">
-        <v>1.272</v>
+        <v>1.2964</v>
       </c>
       <c r="N40" s="76" t="inlineStr">
         <is>
-          <t>2020-02-14</t>
+          <t>2020-02-18</t>
         </is>
       </c>
       <c r="O40" s="0">
@@ -7393,30 +7393,30 @@
       </c>
       <c r="D41" s="0" t="inlineStr">
         <is>
-          <t>1.4557, 1.4409, 1.4495, 1.4711, 1.4565, 1.4497, 1.4261, 1.4321, 1.4448, 1.4361, 1.4333, 1.4221, 1.4244, 1.4315, 1.4324, 1.4468, 1.4563, 1.4505, 1.4539, 1.446, 1.4437, 1.4724, 1.4886, 1.5122, 1.5088, 1.5095, 1.5056, 1.4836, 1.4949, 1.4982, 1.51, 1.5044, 1.5257, 1.5363, 1.5617, 1.5606, 1.5569, 1.5732, 1.5612, 1.5906, 1.5884, 1.6079, 1.5989, 1.5949, 1.5924, 1.5936, 1.6115, 1.5838, 1.5987, 1.5427, 1.4206, 1.474, 1.5008, 1.5356, 1.5263, 1.5417, 1.5576, 1.5714, 1.5623, 1.5737</t>
+          <t>1.4495, 1.4711, 1.4565, 1.4497, 1.4261, 1.4321, 1.4448, 1.4361, 1.4333, 1.4221, 1.4244, 1.4315, 1.4324, 1.4468, 1.4563, 1.4505, 1.4539, 1.446, 1.4437, 1.4724, 1.4886, 1.5122, 1.5088, 1.5095, 1.5056, 1.4836, 1.4949, 1.4982, 1.51, 1.5044, 1.5257, 1.5363, 1.5617, 1.5606, 1.5569, 1.5732, 1.5612, 1.5906, 1.5884, 1.6079, 1.5989, 1.5949, 1.5924, 1.5936, 1.6115, 1.5838, 1.5987, 1.5427, 1.4206, 1.474, 1.5008, 1.5356, 1.5263, 1.5417, 1.5576, 1.5714, 1.5623, 1.5737, 1.6104, 1.6061</t>
         </is>
       </c>
       <c r="H41" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I41" s="76" t="n">
-        <v>1.5737</v>
+        <v>1.6061</v>
       </c>
       <c r="J41" s="78" t="n">
-        <v>0.7296934007553016</v>
+        <v>-0.2670144063586668</v>
       </c>
       <c r="K41" s="76" t="n">
         <v>1</v>
       </c>
       <c r="L41" s="76" t="n">
-        <v>0.7296934007553016</v>
+        <v>-0.2670144063586668</v>
       </c>
       <c r="M41" s="76" t="n">
-        <v>1.5737</v>
+        <v>1.6061</v>
       </c>
       <c r="N41" s="76" t="inlineStr">
         <is>
-          <t>2020-02-14</t>
+          <t>2020-02-18</t>
         </is>
       </c>
       <c r="O41" s="0">
@@ -7533,30 +7533,30 @@
       </c>
       <c r="D42" s="0" t="inlineStr">
         <is>
-          <t>1.0973, 1.0896, 1.0974, 1.1075, 1.0979, 1.0941, 1.084, 1.0908, 1.0933, 1.0895, 1.0857, 1.0772, 1.0789, 1.0817, 1.08, 1.0888, 1.0963, 1.0951, 1.0971, 1.0974, 1.0943, 1.1139, 1.1209, 1.1347, 1.1321, 1.1307, 1.1271, 1.1135, 1.1217, 1.1225, 1.1314, 1.1298, 1.1457, 1.1501, 1.1636, 1.1615, 1.1593, 1.1681, 1.1546, 1.1699, 1.1696, 1.1816, 1.177, 1.1726, 1.1698, 1.1704, 1.1799, 1.1628, 1.1695, 1.1356, 1.0534, 1.0813, 1.0961, 1.1169, 1.1179, 1.1238, 1.1305, 1.1408, 1.1345, 1.1405</t>
+          <t>1.0974, 1.1075, 1.0979, 1.0941, 1.084, 1.0908, 1.0933, 1.0895, 1.0857, 1.0772, 1.0789, 1.0817, 1.08, 1.0888, 1.0963, 1.0951, 1.0971, 1.0974, 1.0943, 1.1139, 1.1209, 1.1347, 1.1321, 1.1307, 1.1271, 1.1135, 1.1217, 1.1225, 1.1314, 1.1298, 1.1457, 1.1501, 1.1636, 1.1615, 1.1593, 1.1681, 1.1546, 1.1699, 1.1696, 1.1816, 1.177, 1.1726, 1.1698, 1.1704, 1.1799, 1.1628, 1.1695, 1.1356, 1.0534, 1.0813, 1.0961, 1.1169, 1.1179, 1.1238, 1.1305, 1.1408, 1.1345, 1.1405, 1.1655, 1.1628</t>
         </is>
       </c>
       <c r="H42" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I42" s="76" t="n">
-        <v>1.1405</v>
+        <v>1.1628</v>
       </c>
       <c r="J42" s="82" t="n">
-        <v>0.5288673424416046</v>
+        <v>-0.2316602316602252</v>
       </c>
       <c r="K42" s="76" t="n">
         <v>1</v>
       </c>
       <c r="L42" s="76" t="n">
-        <v>0.5288673424416046</v>
+        <v>-0.2316602316602252</v>
       </c>
       <c r="M42" s="76" t="n">
-        <v>1.1405</v>
+        <v>1.1628</v>
       </c>
       <c r="N42" s="76" t="inlineStr">
         <is>
-          <t>2020-02-14</t>
+          <t>2020-02-18</t>
         </is>
       </c>
       <c r="O42" s="0">
@@ -7673,30 +7673,30 @@
       </c>
       <c r="D43" s="0" t="inlineStr">
         <is>
-          <t>2.109, 2.091, 2.109, 2.131, 2.11, 2.097, 2.07, 2.085, 2.093, 2.085, 2.079, 2.061, 2.069, 2.078, 2.078, 2.091, 2.102, 2.1, 2.095, 2.103, 2.095, 2.131, 2.136, 2.16, 2.153, 2.147, 2.142, 2.115, 2.126, 2.131, 2.147, 2.144, 2.174, 2.184, 2.218, 2.207, 2.199, 2.219, 2.187, 2.219, 2.226, 2.254, 2.247, 2.243, 2.236, 2.24, 2.26, 2.223, 2.236, 2.172, 2.001, 2.056, 2.071, 2.106, 2.107, 2.118, 2.14, 2.152, 2.143, 2.155</t>
+          <t>2.109, 2.131, 2.11, 2.097, 2.07, 2.085, 2.093, 2.085, 2.079, 2.061, 2.069, 2.078, 2.078, 2.091, 2.102, 2.1, 2.095, 2.103, 2.095, 2.131, 2.136, 2.16, 2.153, 2.147, 2.142, 2.115, 2.126, 2.131, 2.147, 2.144, 2.174, 2.184, 2.218, 2.207, 2.199, 2.219, 2.187, 2.219, 2.226, 2.254, 2.247, 2.243, 2.236, 2.24, 2.26, 2.223, 2.236, 2.172, 2.001, 2.056, 2.071, 2.106, 2.107, 2.118, 2.14, 2.152, 2.143, 2.155, 2.203, 2.188</t>
         </is>
       </c>
       <c r="H43" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I43" s="76" t="n">
-        <v>2.155</v>
+        <v>2.188</v>
       </c>
       <c r="J43" s="78" t="n">
-        <v>0.5599626691553902</v>
+        <v>-0.6808896958692547</v>
       </c>
       <c r="K43" s="76" t="n">
         <v>1</v>
       </c>
       <c r="L43" s="76" t="n">
-        <v>0.4832863471606931</v>
+        <v>-0.589854502556041</v>
       </c>
       <c r="M43" s="76" t="n">
-        <v>2.495</v>
+        <v>2.528</v>
       </c>
       <c r="N43" s="76" t="inlineStr">
         <is>
-          <t>2020-02-14</t>
+          <t>2020-02-18</t>
         </is>
       </c>
       <c r="O43" s="0">
@@ -7813,30 +7813,30 @@
       </c>
       <c r="D44" s="0" t="inlineStr">
         <is>
-          <t>1.606, 1.591, 1.607, 1.623, 1.611, 1.609, 1.603, 1.623, 1.62, 1.612, 1.607, 1.604, 1.609, 1.615, 1.608, 1.615, 1.617, 1.624, 1.623, 1.633, 1.635, 1.647, 1.655, 1.665, 1.66, 1.664, 1.658, 1.638, 1.647, 1.645, 1.662, 1.66, 1.68, 1.69, 1.712, 1.711, 1.706, 1.719, 1.7, 1.72, 1.714, 1.725, 1.727, 1.719, 1.71, 1.711, 1.713, 1.684, 1.689, 1.648, 1.512, 1.542, 1.558, 1.576, 1.581, 1.603, 1.609, 1.619, 1.61, 1.621</t>
+          <t>1.607, 1.623, 1.611, 1.609, 1.603, 1.623, 1.62, 1.612, 1.607, 1.604, 1.609, 1.615, 1.608, 1.615, 1.617, 1.624, 1.623, 1.633, 1.635, 1.647, 1.655, 1.665, 1.66, 1.664, 1.658, 1.638, 1.647, 1.645, 1.662, 1.66, 1.68, 1.69, 1.712, 1.711, 1.706, 1.719, 1.7, 1.72, 1.714, 1.725, 1.727, 1.719, 1.71, 1.711, 1.713, 1.684, 1.689, 1.648, 1.512, 1.542, 1.558, 1.576, 1.581, 1.603, 1.609, 1.619, 1.61, 1.621, 1.653, 1.657</t>
         </is>
       </c>
       <c r="H44" s="0" t="n">
         <v>100</v>
       </c>
       <c r="I44" s="80" t="n">
-        <v>1.621</v>
+        <v>1.657</v>
       </c>
       <c r="J44" s="78" t="n">
-        <v>0.6832298136645899</v>
+        <v>0.2419842710223837</v>
       </c>
       <c r="K44" s="80" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L44" s="80" t="n">
-        <v>0.6832298136645899</v>
+        <v>2.919254658385089</v>
       </c>
       <c r="M44" s="80" t="n">
-        <v>1.621</v>
+        <v>1.657</v>
       </c>
       <c r="N44" s="80" t="inlineStr">
         <is>
-          <t>2020-02-14</t>
+          <t>2020-02-18</t>
         </is>
       </c>
       <c r="O44" s="0">
@@ -8466,23 +8466,23 @@
         <v>0</v>
       </c>
       <c r="F2" s="12" t="n">
-        <v>2917.0077</v>
+        <v>2984.9716</v>
       </c>
       <c r="G2" s="12" t="n">
-        <v>0.3762533879476946</v>
+        <v>0.04522019944613819</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I2" s="12" t="n">
-        <v>0.3762533879476946</v>
+        <v>2.714938214742328</v>
       </c>
       <c r="J2" s="12" t="n">
-        <v>3.080803687</v>
+        <v>3.749985626</v>
       </c>
       <c r="K2" s="0" t="inlineStr">
         <is>
-          <t>20200215 09:38:12</t>
+          <t>20200218 16:29:42</t>
         </is>
       </c>
       <c r="L2" s="45">
@@ -8607,23 +8607,23 @@
         <v>0</v>
       </c>
       <c r="F3" s="12" t="n">
-        <v>10916.3117</v>
+        <v>11306.4863</v>
       </c>
       <c r="G3" s="12" t="n">
-        <v>0.4785342246201026</v>
+        <v>0.5780990441372975</v>
       </c>
       <c r="H3" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I3" s="12" t="n">
-        <v>0.4785342246201026</v>
+        <v>4.06987285410221</v>
       </c>
       <c r="J3" s="12" t="n">
-        <v>5.048924645</v>
+        <v>6.249475121000001</v>
       </c>
       <c r="K3" s="0" t="inlineStr">
         <is>
-          <t>20200214</t>
+          <t>20200218</t>
         </is>
       </c>
       <c r="L3" s="0">
@@ -8743,23 +8743,23 @@
         <v>0</v>
       </c>
       <c r="F4" s="12" t="n">
-        <v>2069.219</v>
+        <v>2170.949</v>
       </c>
       <c r="G4" s="12" t="n">
-        <v>0.2239178996762586</v>
+        <v>1.154238443520732</v>
       </c>
       <c r="H4" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I4" s="12" t="n">
-        <v>0.2239373173128891</v>
+        <v>5.151294519856575</v>
       </c>
       <c r="J4" s="12" t="n">
-        <v>1.892438915</v>
+        <v>2.322640254</v>
       </c>
       <c r="K4" s="0" t="inlineStr">
         <is>
-          <t>20200215 09:38:13</t>
+          <t>20200218 16:29:42</t>
         </is>
       </c>
       <c r="L4" s="45">
@@ -8879,23 +8879,23 @@
         <v>3</v>
       </c>
       <c r="F5" s="12" t="n">
-        <v>2895.0644</v>
+        <v>2924.3981</v>
       </c>
       <c r="G5" s="12" t="n">
-        <v>0.6811038187232374</v>
+        <v>-0.8702098889250073</v>
       </c>
       <c r="H5" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I5" s="12" t="n">
-        <v>0.6811038187232374</v>
+        <v>-0.8702098889250073</v>
       </c>
       <c r="J5" s="12" t="n">
-        <v>0.532705082</v>
+        <v>0.608750963</v>
       </c>
       <c r="K5" s="0" t="inlineStr">
         <is>
-          <t>20200215 09:38:13</t>
+          <t>20200218 16:29:43</t>
         </is>
       </c>
       <c r="L5" s="45">
@@ -9015,23 +9015,23 @@
         <v>103</v>
       </c>
       <c r="F6" s="12" t="n">
-        <v>3987.7342</v>
+        <v>4057.5108</v>
       </c>
       <c r="G6" s="12" t="n">
-        <v>0.7024234941383131</v>
+        <v>-0.4883794158179465</v>
       </c>
       <c r="H6" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I6" s="12" t="n">
-        <v>0.7024234941383131</v>
+        <v>-0.4883794158179465</v>
       </c>
       <c r="J6" s="12" t="n">
-        <v>2.228950736</v>
+        <v>2.425525173</v>
       </c>
       <c r="K6" s="0" t="inlineStr">
         <is>
-          <t>20200215 09:38:13</t>
+          <t>20200218 16:29:43</t>
         </is>
       </c>
       <c r="L6" s="45">
@@ -9156,23 +9156,23 @@
         <v>3</v>
       </c>
       <c r="F7" s="12" t="n">
-        <v>4236.914</v>
+        <v>4333.747</v>
       </c>
       <c r="G7" s="12" t="n">
-        <v>0.7562699875770177</v>
+        <v>0.206899788868808</v>
       </c>
       <c r="H7" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I7" s="12" t="n">
-        <v>0.7562699875770177</v>
+        <v>3.059014837179134</v>
       </c>
       <c r="J7" s="12" t="n">
-        <v>0.296982909</v>
+        <v>0.344906732</v>
       </c>
       <c r="K7" s="0" t="inlineStr">
         <is>
-          <t>20200214</t>
+          <t>20200218</t>
         </is>
       </c>
       <c r="L7" s="45">
@@ -9288,23 +9288,23 @@
         <v>0</v>
       </c>
       <c r="F8" s="12" t="n">
-        <v>5420.8025</v>
+        <v>5660.8142</v>
       </c>
       <c r="G8" s="12" t="n">
-        <v>0.1470706200945986</v>
+        <v>1.186493024159033</v>
       </c>
       <c r="H8" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I8" s="12" t="n">
-        <v>0.1470706200945986</v>
+        <v>4.581186909988754</v>
       </c>
       <c r="J8" s="12" t="n">
-        <v>1.627420046</v>
+        <v>2.064285244</v>
       </c>
       <c r="K8" s="0" t="inlineStr">
         <is>
-          <t>20200215 09:38:13</t>
+          <t>20200218 16:29:43</t>
         </is>
       </c>
       <c r="L8" s="45">
@@ -9425,23 +9425,23 @@
         <v>0</v>
       </c>
       <c r="F9" s="12" t="n">
-        <v>9479.105</v>
+        <v>9593.825000000001</v>
       </c>
       <c r="G9" s="12" t="n">
-        <v>0.3164499693783703</v>
+        <v>-0.366772034310005</v>
       </c>
       <c r="H9" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I9" s="12" t="n">
-        <v>0.3164499693783703</v>
+        <v>-0.366772034310005</v>
       </c>
       <c r="J9" s="12" t="n">
-        <v>0.338064596</v>
+        <v>0.376880436</v>
       </c>
       <c r="K9" s="0" t="inlineStr">
         <is>
-          <t>20200214</t>
+          <t>20200218</t>
         </is>
       </c>
       <c r="L9" s="45">
@@ -9557,23 +9557,23 @@
         <v>0</v>
       </c>
       <c r="F10" s="12" t="n">
-        <v>15822.5993</v>
+        <v>15980.0738</v>
       </c>
       <c r="G10" s="12" t="n">
-        <v>0.8904362817496453</v>
+        <v>-0.469110335541926</v>
       </c>
       <c r="H10" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I10" s="12" t="n">
-        <v>0.8904362817496453</v>
+        <v>-0.469110335541926</v>
       </c>
       <c r="J10" s="12" t="n">
-        <v>0.263998935</v>
+        <v>0.245864055</v>
       </c>
       <c r="K10" s="0" t="inlineStr">
         <is>
-          <t>20200215 09:38:14</t>
+          <t>20200218 16:29:43</t>
         </is>
       </c>
       <c r="L10" s="45">
@@ -9693,23 +9693,23 @@
         <v>0</v>
       </c>
       <c r="F11" s="12" t="n">
-        <v>10868.3803</v>
+        <v>11109.2214</v>
       </c>
       <c r="G11" s="12" t="n">
-        <v>0.08202331733778204</v>
+        <v>0.09106673003029472</v>
       </c>
       <c r="H11" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I11" s="12" t="n">
-        <v>0.08202331733778204</v>
+        <v>2.299820626654723</v>
       </c>
       <c r="J11" s="12" t="n">
-        <v>0.71984879</v>
+        <v>0.8404359850000001</v>
       </c>
       <c r="K11" s="0" t="inlineStr">
         <is>
-          <t>20200215 09:38:14</t>
+          <t>20200218 16:29:43</t>
         </is>
       </c>
       <c r="L11" s="45">
@@ -9829,23 +9829,23 @@
         <v>0</v>
       </c>
       <c r="F12" s="12" t="n">
-        <v>11447.7785</v>
+        <v>11537.9981</v>
       </c>
       <c r="G12" s="12" t="n">
-        <v>0.1805393611774445</v>
+        <v>-0.6808852386980067</v>
       </c>
       <c r="H12" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I12" s="12" t="n">
-        <v>0.1805393611774445</v>
+        <v>-0.6808852386980067</v>
       </c>
       <c r="J12" s="12" t="n">
-        <v>0.204957588</v>
+        <v>0.207715513</v>
       </c>
       <c r="K12" s="0" t="inlineStr">
         <is>
-          <t>20200215 09:38:14</t>
+          <t>20200218 16:29:44</t>
         </is>
       </c>
       <c r="L12" s="45">
@@ -9969,23 +9969,23 @@
         <v>3</v>
       </c>
       <c r="F13" s="12" t="n">
-        <v>721.913</v>
+        <v>753.551</v>
       </c>
       <c r="G13" s="12" t="n">
-        <v>1.845286548453591</v>
+        <v>-0.6031994766027693</v>
       </c>
       <c r="H13" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I13" s="12" t="n">
-        <v>1.845243444403642</v>
+        <v>-0.6031994766027693</v>
       </c>
       <c r="J13" s="12" t="n">
-        <v>0.362194751</v>
+        <v>0.357507294</v>
       </c>
       <c r="K13" s="0" t="inlineStr">
         <is>
-          <t>20200215 09:38:14</t>
+          <t>20200218 16:29:44</t>
         </is>
       </c>
       <c r="L13" s="45">
@@ -10114,23 +10114,23 @@
         <v>2</v>
       </c>
       <c r="F14" s="12" t="n">
-        <v>6277.266</v>
+        <v>6324.635</v>
       </c>
       <c r="G14" s="12" t="n">
-        <v>0.8919161788769774</v>
+        <v>-1.007744536720815</v>
       </c>
       <c r="H14" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I14" s="12" t="n">
-        <v>0.8919161788769774</v>
+        <v>-1.007744536720815</v>
       </c>
       <c r="J14" s="12" t="n">
-        <v>0.102477621</v>
+        <v>0.119038156</v>
       </c>
       <c r="K14" s="0" t="inlineStr">
         <is>
-          <t>20200215 09:38:14</t>
+          <t>20200218 16:29:44</t>
         </is>
       </c>
       <c r="L14" s="45">
@@ -10255,23 +10255,23 @@
         <v>0</v>
       </c>
       <c r="F15" s="11" t="n">
-        <v>10464.051</v>
+        <v>10857.294</v>
       </c>
       <c r="G15" s="11" t="n">
-        <v>-0.5330448450817437</v>
+        <v>0.4801203840851924</v>
       </c>
       <c r="H15" s="0" t="n">
         <v>2</v>
       </c>
       <c r="I15" s="11" t="n">
-        <v>-1.051811095740889</v>
+        <v>3.758037876535583</v>
       </c>
       <c r="J15" s="11" t="n">
-        <v>0.149260195</v>
+        <v>0.171750425</v>
       </c>
       <c r="K15" s="0" t="inlineStr">
         <is>
-          <t>20200214</t>
+          <t>20200218</t>
         </is>
       </c>
       <c r="L15" s="45">
@@ -10393,23 +10393,23 @@
         <v>2</v>
       </c>
       <c r="F16" s="12" t="n">
-        <v>5494.2777</v>
+        <v>5543.5332</v>
       </c>
       <c r="G16" s="12" t="n">
-        <v>0.610808955169261</v>
+        <v>-0.8059763634233925</v>
       </c>
       <c r="H16" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I16" s="12" t="n">
-        <v>0.5258752490469459</v>
+        <v>-0.8548838607812362</v>
       </c>
       <c r="J16" s="12" t="n">
-        <v>0.305340939</v>
+        <v>0.392157644</v>
       </c>
       <c r="K16" s="0" t="inlineStr">
         <is>
-          <t>20200215 09:38:15</t>
+          <t>20200218 16:29:44</t>
         </is>
       </c>
       <c r="L16" s="45">
@@ -10534,17 +10534,17 @@
         <v>3</v>
       </c>
       <c r="F17" s="12" t="n">
-        <v>27815.6</v>
+        <v>27530.2</v>
       </c>
       <c r="G17" s="12" t="n">
-        <v>0.31</v>
+        <v>-1.54</v>
       </c>
       <c r="H17" s="0" t="inlineStr"/>
       <c r="I17" s="11" t="inlineStr"/>
       <c r="J17" s="11" t="inlineStr"/>
       <c r="K17" s="0" t="inlineStr">
         <is>
-          <t>20200215 09:38:15</t>
+          <t>20200218 16:29:44</t>
         </is>
       </c>
       <c r="L17" s="45">
@@ -10792,17 +10792,17 @@
         <v>100</v>
       </c>
       <c r="F19" s="12" t="n">
-        <v>9623.5805</v>
+        <v>9583.4041</v>
       </c>
       <c r="G19" s="12" t="n">
-        <v>0.29</v>
+        <v>-0.42</v>
       </c>
       <c r="H19" s="0" t="inlineStr"/>
       <c r="I19" s="11" t="inlineStr"/>
       <c r="J19" s="11" t="inlineStr"/>
       <c r="K19" s="0" t="inlineStr">
         <is>
-          <t>20200215 09:38:16</t>
+          <t>20200218 16:29:46</t>
         </is>
       </c>
       <c r="L19" s="45">
@@ -11050,23 +11050,23 @@
         <v>100</v>
       </c>
       <c r="F21" s="0" t="n">
-        <v>2466.959</v>
+        <v>2576.371</v>
       </c>
       <c r="G21" s="11" t="n">
-        <v>-1.003147325575845</v>
+        <v>0.9260670239049813</v>
       </c>
       <c r="H21" s="0" t="n">
         <v>2</v>
       </c>
       <c r="I21" s="11" t="n">
-        <v>-1.936810003486137</v>
+        <v>4.43509600281157</v>
       </c>
       <c r="J21" s="11" t="n">
-        <v>0.347055938</v>
+        <v>0.320498249</v>
       </c>
       <c r="K21" s="0" t="inlineStr">
         <is>
-          <t>20200214</t>
+          <t>20200218</t>
         </is>
       </c>
       <c r="L21" s="0">
@@ -11195,23 +11195,23 @@
         <v>0</v>
       </c>
       <c r="F22" s="0" t="n">
-        <v>8893.598</v>
+        <v>9465.575999999999</v>
       </c>
       <c r="G22" s="11" t="n">
-        <v>-0.05892901570789319</v>
+        <v>2.225827897820552</v>
       </c>
       <c r="H22" s="0" t="n">
         <v>2</v>
       </c>
       <c r="I22" s="11" t="n">
-        <v>-1.079741073917272</v>
+        <v>6.431345334025656</v>
       </c>
       <c r="J22" s="11" t="n">
-        <v>0.6154822010000001</v>
+        <v>0.760478558</v>
       </c>
       <c r="K22" s="0" t="inlineStr">
         <is>
-          <t>20200214</t>
+          <t>20200218</t>
         </is>
       </c>
       <c r="L22" s="0">
@@ -11340,23 +11340,23 @@
         <v>0</v>
       </c>
       <c r="F23" s="0" t="n">
-        <v>3956.302</v>
+        <v>4132.834</v>
       </c>
       <c r="G23" s="11" t="n">
-        <v>0.0001769332165589736</v>
+        <v>0.8701344313885867</v>
       </c>
       <c r="H23" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I23" s="11" t="n">
-        <v>0.0001769332165589736</v>
+        <v>4.46223044540409</v>
       </c>
       <c r="J23" s="11" t="n">
-        <v>0.698085985</v>
+        <v>0.836122881</v>
       </c>
       <c r="K23" s="0" t="inlineStr">
         <is>
-          <t>20200214</t>
+          <t>20200218</t>
         </is>
       </c>
       <c r="L23" s="0">
@@ -11616,23 +11616,23 @@
         <v>0</v>
       </c>
       <c r="F25" s="0" t="n">
-        <v>4667.8054</v>
+        <v>4813.5505</v>
       </c>
       <c r="G25" s="11" t="n">
-        <v>0.5238960517184752</v>
+        <v>0.2619697913760661</v>
       </c>
       <c r="H25" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I25" s="11" t="n">
-        <v>0.5238960517184752</v>
+        <v>3.662601294753526</v>
       </c>
       <c r="J25" s="11" t="n">
-        <v>2.129033164</v>
+        <v>2.383757086</v>
       </c>
       <c r="K25" s="0" t="inlineStr">
         <is>
-          <t>20200214</t>
+          <t>20200218</t>
         </is>
       </c>
       <c r="L25" s="0">
@@ -11756,23 +11756,23 @@
         <v>0</v>
       </c>
       <c r="F26" s="0" t="n">
-        <v>6121.5241</v>
+        <v>6257.2438</v>
       </c>
       <c r="G26" s="11" t="n">
-        <v>0.7364950025251807</v>
+        <v>-0.2612568686465158</v>
       </c>
       <c r="H26" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I26" s="11" t="n">
-        <v>0.7364950025251807</v>
+        <v>-0.2612568686465158</v>
       </c>
       <c r="J26" s="11" t="n">
-        <v>1.108890995</v>
+        <v>1.14244656</v>
       </c>
       <c r="K26" s="0" t="inlineStr">
         <is>
-          <t>20200214</t>
+          <t>20200218</t>
         </is>
       </c>
       <c r="L26" s="0">
@@ -12022,23 +12022,23 @@
         <v>0</v>
       </c>
       <c r="F28" s="0" t="n">
-        <v>3456.762</v>
+        <v>3519.609</v>
       </c>
       <c r="G28" s="11" t="n">
-        <v>0.3687797631923483</v>
+        <v>-0.3571686401630697</v>
       </c>
       <c r="H28" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I28" s="11" t="n">
-        <v>0.3687797631923483</v>
+        <v>-0.3571686401630697</v>
       </c>
       <c r="J28" s="11" t="n">
-        <v>0.147586429</v>
+        <v>0.15584575</v>
       </c>
       <c r="K28" s="0" t="inlineStr">
         <is>
-          <t>20200214</t>
+          <t>20200218</t>
         </is>
       </c>
       <c r="L28" s="0">
@@ -12159,23 +12159,23 @@
         <v>3</v>
       </c>
       <c r="F29" s="0" t="n">
-        <v>3049.712</v>
+        <v>3217.884</v>
       </c>
       <c r="G29" s="11" t="n">
-        <v>0.1727403904740857</v>
+        <v>1.618245206275426</v>
       </c>
       <c r="H29" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I29" s="11" t="n">
-        <v>0.1727403904740857</v>
+        <v>5.696622677374229</v>
       </c>
       <c r="J29" s="11" t="n">
-        <v>1.187110204</v>
+        <v>1.357565852</v>
       </c>
       <c r="K29" s="0" t="inlineStr">
         <is>
-          <t>20200214</t>
+          <t>20200218</t>
         </is>
       </c>
       <c r="L29" s="0">
@@ -12299,23 +12299,23 @@
         <v>3</v>
       </c>
       <c r="F30" s="0" t="n">
-        <v>3149.4799</v>
+        <v>3363.1807</v>
       </c>
       <c r="G30" s="11" t="n">
-        <v>0.4642598068592196</v>
+        <v>2.718827068386564</v>
       </c>
       <c r="H30" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I30" s="11" t="n">
-        <v>0.4642598068592196</v>
+        <v>7.281033805681587</v>
       </c>
       <c r="J30" s="11" t="n">
-        <v>1.038171342</v>
+        <v>1.316447224</v>
       </c>
       <c r="K30" s="0" t="inlineStr">
         <is>
-          <t>20200214</t>
+          <t>20200218</t>
         </is>
       </c>
       <c r="L30" s="0">
@@ -12439,23 +12439,23 @@
         <v>3</v>
       </c>
       <c r="F31" s="0" t="n">
-        <v>6743.6724</v>
+        <v>7200.1705</v>
       </c>
       <c r="G31" s="11" t="n">
-        <v>0.5251921303554345</v>
+        <v>2.643451054553089</v>
       </c>
       <c r="H31" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I31" s="11" t="n">
-        <v>0.5251921303554345</v>
+        <v>7.330024347537602</v>
       </c>
       <c r="J31" s="11" t="n">
-        <v>2.263568372</v>
+        <v>2.77097012</v>
       </c>
       <c r="K31" s="0" t="inlineStr">
         <is>
-          <t>20200214</t>
+          <t>20200218</t>
         </is>
       </c>
       <c r="L31" s="0">
@@ -12579,23 +12579,23 @@
         <v>0</v>
       </c>
       <c r="F32" s="0" t="n">
-        <v>3463.4166</v>
+        <v>3506.4467</v>
       </c>
       <c r="G32" s="11" t="n">
-        <v>1.470732613478791</v>
+        <v>-0.6615730998159643</v>
       </c>
       <c r="H32" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I32" s="11" t="n">
-        <v>1.470732613478791</v>
+        <v>-0.6615730998159643</v>
       </c>
       <c r="J32" s="11" t="n">
-        <v>0.172679227</v>
+        <v>0.153679767</v>
       </c>
       <c r="K32" s="0" t="inlineStr">
         <is>
-          <t>20200214</t>
+          <t>20200218</t>
         </is>
       </c>
       <c r="L32" s="0">
@@ -12711,23 +12711,23 @@
         <v>0</v>
       </c>
       <c r="F33" s="0" t="n">
-        <v>2287.1968</v>
+        <v>2425.2866</v>
       </c>
       <c r="G33" s="11" t="n">
-        <v>0.286139486411656</v>
+        <v>2.217197804541328</v>
       </c>
       <c r="H33" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I33" s="11" t="n">
-        <v>0.286139486411656</v>
+        <v>6.340928013769975</v>
       </c>
       <c r="J33" s="11" t="n">
-        <v>1.132505575</v>
+        <v>1.350950162</v>
       </c>
       <c r="K33" s="0" t="inlineStr">
         <is>
-          <t>20200214</t>
+          <t>20200218</t>
         </is>
       </c>
       <c r="L33" s="0">
@@ -12851,23 +12851,23 @@
         <v>5</v>
       </c>
       <c r="F34" s="0" t="n">
-        <v>9696.887699999999</v>
+        <v>9802.081200000001</v>
       </c>
       <c r="G34" s="11" t="n">
-        <v>0.8035289232396081</v>
+        <v>-0.7030956794433065</v>
       </c>
       <c r="H34" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I34" s="11" t="n">
-        <v>0.8035289232396081</v>
+        <v>-0.7030956794433065</v>
       </c>
       <c r="J34" s="11" t="n">
-        <v>0.286984785</v>
+        <v>0.322008653</v>
       </c>
       <c r="K34" s="0" t="inlineStr">
         <is>
-          <t>20200214</t>
+          <t>20200218</t>
         </is>
       </c>
       <c r="L34" s="0">
@@ -12991,23 +12991,23 @@
         <v>0</v>
       </c>
       <c r="F35" s="0" t="n">
-        <v>4769.0779</v>
+        <v>4874.8126</v>
       </c>
       <c r="G35" s="11" t="n">
-        <v>0.7364944699229503</v>
+        <v>-0.2612580315279783</v>
       </c>
       <c r="H35" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I35" s="11" t="n">
-        <v>0.7364944699229503</v>
+        <v>-0.2612580315279783</v>
       </c>
       <c r="J35" s="11" t="n">
-        <v>1.108890995</v>
+        <v>1.14244656</v>
       </c>
       <c r="K35" s="0" t="inlineStr">
         <is>
-          <t>20200214</t>
+          <t>20200218</t>
         </is>
       </c>
       <c r="L35" s="0">
@@ -13131,23 +13131,23 @@
         <v>0</v>
       </c>
       <c r="F36" s="0" t="n">
-        <v>3647.4363</v>
+        <v>3661.9615</v>
       </c>
       <c r="G36" s="11" t="n">
-        <v>2.221603603733874</v>
+        <v>-0.9463268702250989</v>
       </c>
       <c r="H36" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I36" s="11" t="n">
-        <v>2.221603603733874</v>
+        <v>-0.9463268702250989</v>
       </c>
       <c r="J36" s="11" t="n">
-        <v>0.187134834</v>
+        <v>0.149634025</v>
       </c>
       <c r="K36" s="0" t="inlineStr">
         <is>
-          <t>20200214</t>
+          <t>20200218</t>
         </is>
       </c>
       <c r="L36" s="0">
@@ -13268,23 +13268,23 @@
         <v>0</v>
       </c>
       <c r="F37" s="0" t="n">
-        <v>14261.341</v>
+        <v>14380.319</v>
       </c>
       <c r="G37" s="11" t="n">
-        <v>-0.1160394004472174</v>
+        <v>-0.3845431551533169</v>
       </c>
       <c r="H37" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I37" s="11" t="n">
-        <v>-1.349503207257726</v>
+        <v>-0.3845431551533169</v>
       </c>
       <c r="J37" s="11" t="n">
-        <v>0.146185045</v>
+        <v>0.178084129</v>
       </c>
       <c r="K37" s="0" t="inlineStr">
         <is>
-          <t>20200214</t>
+          <t>20200218</t>
         </is>
       </c>
       <c r="L37" s="0">
@@ -13413,23 +13413,23 @@
         <v>3</v>
       </c>
       <c r="F38" s="0" t="n">
-        <v>3553.374</v>
+        <v>3761.859</v>
       </c>
       <c r="G38" s="11" t="n">
-        <v>0.3047215037406256</v>
+        <v>2.471530533138871</v>
       </c>
       <c r="H38" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I38" s="11" t="n">
-        <v>4.833177019611148</v>
+        <v>10.98399168503439</v>
       </c>
       <c r="J38" s="11" t="n">
-        <v>0.851997259</v>
+        <v>0.939355761</v>
       </c>
       <c r="K38" s="0" t="inlineStr">
         <is>
-          <t>20200214</t>
+          <t>20200218</t>
         </is>
       </c>
       <c r="L38" s="0">
@@ -13558,23 +13558,23 @@
         <v>2</v>
       </c>
       <c r="F39" s="0" t="n">
-        <v>8112.761</v>
+        <v>8149.542</v>
       </c>
       <c r="G39" s="11" t="n">
-        <v>0.5548465814807088</v>
+        <v>-0.9029043160730502</v>
       </c>
       <c r="H39" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I39" s="11" t="n">
-        <v>9.135295566538918</v>
+        <v>-0.9029043160730502</v>
       </c>
       <c r="J39" s="11" t="n">
-        <v>0.084218076</v>
+        <v>0.09677662699999999</v>
       </c>
       <c r="K39" s="0" t="inlineStr">
         <is>
-          <t>20200214</t>
+          <t>20200218</t>
         </is>
       </c>
       <c r="L39" s="0">
@@ -13821,23 +13821,23 @@
         <v>2</v>
       </c>
       <c r="F41" s="0" t="n">
-        <v>8131.3124</v>
+        <v>8940.4638</v>
       </c>
       <c r="G41" s="11" t="n">
-        <v>0.1647734063246235</v>
+        <v>3.650591993295832</v>
       </c>
       <c r="H41" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I41" s="11" t="n">
-        <v>0.1647734063246235</v>
+        <v>10.13222547868754</v>
       </c>
       <c r="J41" s="11" t="n">
-        <v>0.161857231</v>
+        <v>0.269721146</v>
       </c>
       <c r="K41" s="0" t="inlineStr">
         <is>
-          <t>20200214</t>
+          <t>20200218</t>
         </is>
       </c>
       <c r="L41" s="0">
@@ -14384,19 +14384,19 @@
         <v>10000</v>
       </c>
       <c r="G3" s="0" t="n">
-        <v>0.9581</v>
+        <v>0.9989</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>10000</v>
       </c>
       <c r="I3" s="0" t="n">
-        <v>1.272</v>
+        <v>1.2964</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>10000</v>
       </c>
       <c r="K3" s="0" t="n">
-        <v>1.621</v>
+        <v>1.657</v>
       </c>
       <c r="L3" s="0" t="inlineStr"/>
       <c r="M3" s="0" t="inlineStr"/>
@@ -14452,13 +14452,13 @@
         <v>3000</v>
       </c>
       <c r="AE3" s="0" t="n">
-        <v>2.955</v>
+        <v>2.961</v>
       </c>
       <c r="AF3" s="0" t="n">
         <v>10000</v>
       </c>
       <c r="AG3" s="0" t="n">
-        <v>27815.6</v>
+        <v>27530.2</v>
       </c>
       <c r="AH3" s="0" t="n">
         <v>14000</v>
@@ -14476,10 +14476,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="11" t="n">
-        <v>1585.28326198874</v>
+        <v>2348.161475440668</v>
       </c>
       <c r="C4" s="11" t="n">
-        <v>3.68670526043893</v>
+        <v>5.460840640559693</v>
       </c>
       <c r="D4" s="11" t="n">
         <v>2049.08864954432</v>
@@ -14488,22 +14488,22 @@
         <v>15.7622203811102</v>
       </c>
       <c r="F4" s="11" t="n">
-        <v>276.7349565590468</v>
+        <v>714.3623297221924</v>
       </c>
       <c r="G4" s="11" t="n">
-        <v>2.767349565590468</v>
+        <v>7.143623297221923</v>
       </c>
       <c r="H4" s="11" t="n">
-        <v>242.3705612368147</v>
+        <v>438.8437072228037</v>
       </c>
       <c r="I4" s="11" t="n">
-        <v>2.423705612368147</v>
+        <v>4.388437072228037</v>
       </c>
       <c r="J4" s="11" t="n">
-        <v>285.5329949238574</v>
+        <v>513.9593908629439</v>
       </c>
       <c r="K4" s="11" t="n">
-        <v>2.855329949238574</v>
+        <v>5.139593908629439</v>
       </c>
       <c r="L4" s="11" t="inlineStr"/>
       <c r="M4" s="11" t="inlineStr"/>
@@ -14556,16 +14556,16 @@
         <v>0.523864959254955</v>
       </c>
       <c r="AD4" s="12" t="n">
-        <v>396.5517241379313</v>
+        <v>403.448275862069</v>
       </c>
       <c r="AE4" s="12" t="n">
-        <v>13.21839080459771</v>
+        <v>13.44827586206896</v>
       </c>
       <c r="AF4" s="12" t="n">
-        <v>384.0930251310898</v>
+        <v>277.5477717706593</v>
       </c>
       <c r="AG4" s="12" t="n">
-        <v>3.840930251310898</v>
+        <v>2.775477717706593</v>
       </c>
       <c r="AH4" s="0" t="n">
         <v>1053.2994269341</v>
@@ -14583,10 +14583,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="11" t="n">
-        <v>340.9329358114118</v>
+        <v>-214.4663907204111</v>
       </c>
       <c r="C5" s="11" t="n">
-        <v>0.7928672925846786</v>
+        <v>-0.4987590481870026</v>
       </c>
       <c r="D5" s="11" t="n">
         <v>85.45700135074129</v>
@@ -14595,22 +14595,22 @@
         <v>0.657361548851856</v>
       </c>
       <c r="F5" s="11" t="n">
-        <v>181.7215727948991</v>
+        <v>-48.81450488145064</v>
       </c>
       <c r="G5" s="11" t="n">
-        <v>1.817215727948991</v>
+        <v>-0.4881450488145064</v>
       </c>
       <c r="H5" s="11" t="n">
-        <v>60.90326662975592</v>
+        <v>-33.82533825338223</v>
       </c>
       <c r="I5" s="11" t="n">
-        <v>0.6090326662975591</v>
+        <v>-0.3382533825338223</v>
       </c>
       <c r="J5" s="11" t="n">
-        <v>68.32298136645899</v>
+        <v>24.19842710223837</v>
       </c>
       <c r="K5" s="11" t="n">
-        <v>0.6832298136645899</v>
+        <v>0.2419842710223837</v>
       </c>
       <c r="L5" s="11" t="inlineStr"/>
       <c r="M5" s="11" t="inlineStr"/>
@@ -14663,16 +14663,16 @@
         <v>-0.346220427005194</v>
       </c>
       <c r="AD5" s="12" t="n">
-        <v>-1.014884979702189</v>
+        <v>-2.024974687816629</v>
       </c>
       <c r="AE5" s="12" t="n">
-        <v>-0.03382949932340629</v>
+        <v>-0.0674991562605543</v>
       </c>
       <c r="AF5" s="12" t="n">
-        <v>31</v>
+        <v>-154</v>
       </c>
       <c r="AG5" s="12" t="n">
-        <v>0.31</v>
+        <v>-1.54</v>
       </c>
       <c r="AH5" s="0" t="n">
         <v>197.030035634891</v>
@@ -15455,10 +15455,10 @@
       <c r="AB19" s="11" t="inlineStr"/>
       <c r="AC19" s="11" t="inlineStr"/>
       <c r="AD19" s="12" t="n">
-        <v>396.5517241379313</v>
+        <v>403.448275862069</v>
       </c>
       <c r="AE19" s="12" t="n">
-        <v>13.21839080459771</v>
+        <v>13.44827586206896</v>
       </c>
       <c r="AF19" s="0" t="inlineStr"/>
       <c r="AG19" s="0" t="inlineStr"/>
@@ -16213,22 +16213,22 @@
       <c r="D31" s="0" t="inlineStr"/>
       <c r="E31" s="0" t="inlineStr"/>
       <c r="F31" s="12" t="n">
-        <v>276.7349565590468</v>
+        <v>714.3623297221924</v>
       </c>
       <c r="G31" s="12" t="n">
-        <v>2.767349565590468</v>
+        <v>7.143623297221923</v>
       </c>
       <c r="H31" s="12" t="n">
-        <v>242.3705612368147</v>
+        <v>438.8437072228037</v>
       </c>
       <c r="I31" s="12" t="n">
-        <v>2.423705612368147</v>
+        <v>4.388437072228037</v>
       </c>
       <c r="J31" s="12" t="n">
-        <v>285.5329949238574</v>
+        <v>513.9593908629439</v>
       </c>
       <c r="K31" s="12" t="n">
-        <v>2.855329949238574</v>
+        <v>5.139593908629439</v>
       </c>
       <c r="L31" s="0" t="inlineStr"/>
       <c r="M31" s="0" t="inlineStr"/>
@@ -16251,10 +16251,10 @@
       <c r="AD31" s="12" t="inlineStr"/>
       <c r="AE31" s="12" t="inlineStr"/>
       <c r="AF31" s="12" t="n">
-        <v>384.0930251310898</v>
+        <v>277.5477717706593</v>
       </c>
       <c r="AG31" s="12" t="n">
-        <v>3.840930251310898</v>
+        <v>2.775477717706593</v>
       </c>
       <c r="AH31" s="0" t="inlineStr"/>
       <c r="AI31" s="0" t="inlineStr"/>
@@ -16671,6 +16671,12 @@
     <cfRule type="cellIs" priority="6622" operator="lessThan" dxfId="9" stopIfTrue="1">
       <formula>0</formula>
     </cfRule>
+    <cfRule type="cellIs" priority="6689" operator="greaterThan" dxfId="8" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6690" operator="lessThan" dxfId="9" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
     <cfRule type="cellIs" priority="2045" operator="greaterThan" dxfId="6" stopIfTrue="1">
@@ -16931,6 +16937,12 @@
     <cfRule type="cellIs" priority="6624" operator="lessThan" dxfId="9" stopIfTrue="1">
       <formula>0</formula>
     </cfRule>
+    <cfRule type="cellIs" priority="6691" operator="greaterThan" dxfId="8" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6692" operator="lessThan" dxfId="9" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
     <cfRule type="cellIs" priority="2203" operator="greaterThan" dxfId="6" stopIfTrue="1">
@@ -17411,6 +17423,12 @@
     <cfRule type="cellIs" priority="6566" operator="lessThan" dxfId="9" stopIfTrue="1">
       <formula>0</formula>
     </cfRule>
+    <cfRule type="cellIs" priority="6633" operator="greaterThan" dxfId="8" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6634" operator="lessThan" dxfId="9" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:K4">
     <cfRule type="cellIs" priority="1901" operator="greaterThan" dxfId="6" stopIfTrue="1">
@@ -20667,6 +20685,12 @@
     <cfRule type="cellIs" priority="6602" operator="lessThan" dxfId="9" stopIfTrue="1">
       <formula>0</formula>
     </cfRule>
+    <cfRule type="cellIs" priority="6669" operator="greaterThan" dxfId="8" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6670" operator="lessThan" dxfId="9" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE4">
     <cfRule type="cellIs" priority="2025" operator="greaterThan" dxfId="6" stopIfTrue="1">
@@ -20843,6 +20867,12 @@
     <cfRule type="cellIs" priority="6604" operator="lessThan" dxfId="9" stopIfTrue="1">
       <formula>0</formula>
     </cfRule>
+    <cfRule type="cellIs" priority="6671" operator="greaterThan" dxfId="8" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6672" operator="lessThan" dxfId="9" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF4">
     <cfRule type="cellIs" priority="2035" operator="greaterThan" dxfId="6" stopIfTrue="1">
@@ -21007,6 +21037,12 @@
     <cfRule type="cellIs" priority="6614" operator="lessThan" dxfId="9" stopIfTrue="1">
       <formula>0</formula>
     </cfRule>
+    <cfRule type="cellIs" priority="6681" operator="greaterThan" dxfId="8" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6682" operator="lessThan" dxfId="9" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG4">
     <cfRule type="cellIs" priority="2037" operator="greaterThan" dxfId="6" stopIfTrue="1">
@@ -21171,6 +21207,12 @@
     <cfRule type="cellIs" priority="6616" operator="lessThan" dxfId="9" stopIfTrue="1">
       <formula>0</formula>
     </cfRule>
+    <cfRule type="cellIs" priority="6683" operator="greaterThan" dxfId="8" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6684" operator="lessThan" dxfId="9" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
     <cfRule type="cellIs" priority="2047" operator="greaterThan" dxfId="6" stopIfTrue="1">
@@ -21431,6 +21473,12 @@
     <cfRule type="cellIs" priority="6626" operator="lessThan" dxfId="9" stopIfTrue="1">
       <formula>0</formula>
     </cfRule>
+    <cfRule type="cellIs" priority="6693" operator="greaterThan" dxfId="8" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6694" operator="lessThan" dxfId="9" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
     <cfRule type="cellIs" priority="2049" operator="greaterThan" dxfId="6" stopIfTrue="1">
@@ -21691,6 +21739,12 @@
     <cfRule type="cellIs" priority="6628" operator="lessThan" dxfId="9" stopIfTrue="1">
       <formula>0</formula>
     </cfRule>
+    <cfRule type="cellIs" priority="6695" operator="greaterThan" dxfId="8" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6696" operator="lessThan" dxfId="9" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
     <cfRule type="cellIs" priority="2205" operator="greaterThan" dxfId="6" stopIfTrue="1">
@@ -22171,6 +22225,12 @@
     <cfRule type="cellIs" priority="6570" operator="lessThan" dxfId="9" stopIfTrue="1">
       <formula>0</formula>
     </cfRule>
+    <cfRule type="cellIs" priority="6637" operator="greaterThan" dxfId="8" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6638" operator="lessThan" dxfId="9" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:K5">
     <cfRule type="cellIs" priority="1905" operator="greaterThan" dxfId="6" stopIfTrue="1">
@@ -25427,6 +25487,12 @@
     <cfRule type="cellIs" priority="6606" operator="lessThan" dxfId="9" stopIfTrue="1">
       <formula>0</formula>
     </cfRule>
+    <cfRule type="cellIs" priority="6673" operator="greaterThan" dxfId="8" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6674" operator="lessThan" dxfId="9" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE5">
     <cfRule type="cellIs" priority="2029" operator="greaterThan" dxfId="6" stopIfTrue="1">
@@ -25603,6 +25669,12 @@
     <cfRule type="cellIs" priority="6608" operator="lessThan" dxfId="9" stopIfTrue="1">
       <formula>0</formula>
     </cfRule>
+    <cfRule type="cellIs" priority="6675" operator="greaterThan" dxfId="8" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6676" operator="lessThan" dxfId="9" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF5">
     <cfRule type="cellIs" priority="2039" operator="greaterThan" dxfId="6" stopIfTrue="1">
@@ -25767,6 +25839,12 @@
     <cfRule type="cellIs" priority="6618" operator="lessThan" dxfId="9" stopIfTrue="1">
       <formula>0</formula>
     </cfRule>
+    <cfRule type="cellIs" priority="6685" operator="greaterThan" dxfId="8" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6686" operator="lessThan" dxfId="9" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG5">
     <cfRule type="cellIs" priority="2041" operator="greaterThan" dxfId="6" stopIfTrue="1">
@@ -25931,6 +26009,12 @@
     <cfRule type="cellIs" priority="6620" operator="lessThan" dxfId="9" stopIfTrue="1">
       <formula>0</formula>
     </cfRule>
+    <cfRule type="cellIs" priority="6687" operator="greaterThan" dxfId="8" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6688" operator="lessThan" dxfId="9" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD7:AK7">
     <cfRule type="cellIs" priority="7" operator="lessThan" dxfId="2">
@@ -29461,6 +29545,12 @@
     <cfRule type="cellIs" priority="6598" operator="lessThan" dxfId="9" stopIfTrue="1">
       <formula>0</formula>
     </cfRule>
+    <cfRule type="cellIs" priority="6665" operator="greaterThan" dxfId="8" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6666" operator="lessThan" dxfId="9" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE19">
     <cfRule type="cellIs" priority="522" operator="lessThan" dxfId="7" stopIfTrue="1">
@@ -29703,6 +29793,12 @@
     <cfRule type="cellIs" priority="6600" operator="lessThan" dxfId="9" stopIfTrue="1">
       <formula>0</formula>
     </cfRule>
+    <cfRule type="cellIs" priority="6667" operator="greaterThan" dxfId="8" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6668" operator="lessThan" dxfId="9" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L21">
     <cfRule type="cellIs" priority="491" operator="lessThan" dxfId="7" stopIfTrue="1">
@@ -36129,6 +36225,12 @@
     <cfRule type="cellIs" priority="6562" operator="lessThan" dxfId="9" stopIfTrue="1">
       <formula>0</formula>
     </cfRule>
+    <cfRule type="cellIs" priority="6629" operator="greaterThan" dxfId="8" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6630" operator="lessThan" dxfId="9" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G31">
     <cfRule type="cellIs" priority="6359" operator="greaterThan" dxfId="8" stopIfTrue="1">
@@ -36155,6 +36257,12 @@
     <cfRule type="cellIs" priority="6564" operator="lessThan" dxfId="9" stopIfTrue="1">
       <formula>0</formula>
     </cfRule>
+    <cfRule type="cellIs" priority="6631" operator="greaterThan" dxfId="8" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6632" operator="lessThan" dxfId="9" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4">
     <cfRule type="cellIs" priority="6363" operator="greaterThan" dxfId="8" stopIfTrue="1">
@@ -36181,6 +36289,12 @@
     <cfRule type="cellIs" priority="6568" operator="lessThan" dxfId="9" stopIfTrue="1">
       <formula>0</formula>
     </cfRule>
+    <cfRule type="cellIs" priority="6635" operator="greaterThan" dxfId="8" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6636" operator="lessThan" dxfId="9" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5">
     <cfRule type="cellIs" priority="6367" operator="greaterThan" dxfId="8" stopIfTrue="1">
@@ -36207,6 +36321,12 @@
     <cfRule type="cellIs" priority="6572" operator="lessThan" dxfId="9" stopIfTrue="1">
       <formula>0</formula>
     </cfRule>
+    <cfRule type="cellIs" priority="6639" operator="greaterThan" dxfId="8" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6640" operator="lessThan" dxfId="9" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H31">
     <cfRule type="cellIs" priority="6369" operator="greaterThan" dxfId="8" stopIfTrue="1">
@@ -36233,6 +36353,12 @@
     <cfRule type="cellIs" priority="6574" operator="lessThan" dxfId="9" stopIfTrue="1">
       <formula>0</formula>
     </cfRule>
+    <cfRule type="cellIs" priority="6641" operator="greaterThan" dxfId="8" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6642" operator="lessThan" dxfId="9" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I31">
     <cfRule type="cellIs" priority="6371" operator="greaterThan" dxfId="8" stopIfTrue="1">
@@ -36259,6 +36385,12 @@
     <cfRule type="cellIs" priority="6576" operator="lessThan" dxfId="9" stopIfTrue="1">
       <formula>0</formula>
     </cfRule>
+    <cfRule type="cellIs" priority="6643" operator="greaterThan" dxfId="8" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6644" operator="lessThan" dxfId="9" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
     <cfRule type="cellIs" priority="6373" operator="greaterThan" dxfId="8" stopIfTrue="1">
@@ -36285,6 +36417,12 @@
     <cfRule type="cellIs" priority="6578" operator="lessThan" dxfId="9" stopIfTrue="1">
       <formula>0</formula>
     </cfRule>
+    <cfRule type="cellIs" priority="6645" operator="greaterThan" dxfId="8" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6646" operator="lessThan" dxfId="9" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
     <cfRule type="cellIs" priority="6375" operator="greaterThan" dxfId="8" stopIfTrue="1">
@@ -36311,6 +36449,12 @@
     <cfRule type="cellIs" priority="6580" operator="lessThan" dxfId="9" stopIfTrue="1">
       <formula>0</formula>
     </cfRule>
+    <cfRule type="cellIs" priority="6647" operator="greaterThan" dxfId="8" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6648" operator="lessThan" dxfId="9" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
     <cfRule type="cellIs" priority="6377" operator="greaterThan" dxfId="8" stopIfTrue="1">
@@ -36337,6 +36481,12 @@
     <cfRule type="cellIs" priority="6582" operator="lessThan" dxfId="9" stopIfTrue="1">
       <formula>0</formula>
     </cfRule>
+    <cfRule type="cellIs" priority="6649" operator="greaterThan" dxfId="8" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6650" operator="lessThan" dxfId="9" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
     <cfRule type="cellIs" priority="6379" operator="greaterThan" dxfId="8" stopIfTrue="1">
@@ -36363,6 +36513,12 @@
     <cfRule type="cellIs" priority="6584" operator="lessThan" dxfId="9" stopIfTrue="1">
       <formula>0</formula>
     </cfRule>
+    <cfRule type="cellIs" priority="6651" operator="greaterThan" dxfId="8" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6652" operator="lessThan" dxfId="9" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J31">
     <cfRule type="cellIs" priority="6381" operator="greaterThan" dxfId="8" stopIfTrue="1">
@@ -36389,6 +36545,12 @@
     <cfRule type="cellIs" priority="6586" operator="lessThan" dxfId="9" stopIfTrue="1">
       <formula>0</formula>
     </cfRule>
+    <cfRule type="cellIs" priority="6653" operator="greaterThan" dxfId="8" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6654" operator="lessThan" dxfId="9" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31">
     <cfRule type="cellIs" priority="6383" operator="greaterThan" dxfId="8" stopIfTrue="1">
@@ -36415,6 +36577,12 @@
     <cfRule type="cellIs" priority="6588" operator="lessThan" dxfId="9" stopIfTrue="1">
       <formula>0</formula>
     </cfRule>
+    <cfRule type="cellIs" priority="6655" operator="greaterThan" dxfId="8" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6656" operator="lessThan" dxfId="9" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4">
     <cfRule type="cellIs" priority="6385" operator="greaterThan" dxfId="8" stopIfTrue="1">
@@ -36441,6 +36609,12 @@
     <cfRule type="cellIs" priority="6590" operator="lessThan" dxfId="9" stopIfTrue="1">
       <formula>0</formula>
     </cfRule>
+    <cfRule type="cellIs" priority="6657" operator="greaterThan" dxfId="8" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6658" operator="lessThan" dxfId="9" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4">
     <cfRule type="cellIs" priority="6387" operator="greaterThan" dxfId="8" stopIfTrue="1">
@@ -36467,6 +36641,12 @@
     <cfRule type="cellIs" priority="6592" operator="lessThan" dxfId="9" stopIfTrue="1">
       <formula>0</formula>
     </cfRule>
+    <cfRule type="cellIs" priority="6659" operator="greaterThan" dxfId="8" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6660" operator="lessThan" dxfId="9" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5">
     <cfRule type="cellIs" priority="6389" operator="greaterThan" dxfId="8" stopIfTrue="1">
@@ -36493,6 +36673,12 @@
     <cfRule type="cellIs" priority="6594" operator="lessThan" dxfId="9" stopIfTrue="1">
       <formula>0</formula>
     </cfRule>
+    <cfRule type="cellIs" priority="6661" operator="greaterThan" dxfId="8" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6662" operator="lessThan" dxfId="9" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
     <cfRule type="cellIs" priority="6391" operator="greaterThan" dxfId="8" stopIfTrue="1">
@@ -36519,6 +36705,12 @@
     <cfRule type="cellIs" priority="6596" operator="lessThan" dxfId="9" stopIfTrue="1">
       <formula>0</formula>
     </cfRule>
+    <cfRule type="cellIs" priority="6663" operator="greaterThan" dxfId="8" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6664" operator="lessThan" dxfId="9" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD31">
     <cfRule type="cellIs" priority="6405" operator="greaterThan" dxfId="8" stopIfTrue="1">
@@ -36561,6 +36753,12 @@
     <cfRule type="cellIs" priority="6610" operator="lessThan" dxfId="9" stopIfTrue="1">
       <formula>0</formula>
     </cfRule>
+    <cfRule type="cellIs" priority="6677" operator="greaterThan" dxfId="8" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6678" operator="lessThan" dxfId="9" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG31">
     <cfRule type="cellIs" priority="6543" operator="greaterThan" dxfId="8" stopIfTrue="1">
@@ -36573,6 +36771,12 @@
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" priority="6612" operator="lessThan" dxfId="9" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6679" operator="greaterThan" dxfId="8" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6680" operator="lessThan" dxfId="9" stopIfTrue="1">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>